<commit_message>
First raw calibration for Bhutan
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A506B9C9-AD24-4FCF-81D9-8A36816D59AE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5490" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>parameter</t>
   </si>
@@ -59,12 +65,36 @@
   <si>
     <t>runge_kutta</t>
   </si>
+  <si>
+    <t>tb_n_contact</t>
+  </si>
+  <si>
+    <t>program_prop_death_reporting</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>susceptible_fully</t>
+  </si>
+  <si>
+    <t>target_population</t>
+  </si>
+  <si>
+    <t>age_breakpoints</t>
+  </si>
+  <si>
+    <t>plot_start_time</t>
+  </si>
+  <si>
+    <t>program_perc_detect</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,8 +159,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +204,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,7 +956,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
@@ -919,671 +977,687 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="661" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="661" applyFont="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="662" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="662" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="662" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="662" applyFont="1"/>
   </cellXfs>
   <cellStyles count="663">
-    <cellStyle name="Comma 2" xfId="614"/>
-    <cellStyle name="Comma 2 2" xfId="626"/>
-    <cellStyle name="Input 2" xfId="378"/>
+    <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 2 2" xfId="626" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Input 2" xfId="378" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="545"/>
-    <cellStyle name="Normal 2" xfId="449"/>
-    <cellStyle name="Normal 2 2" xfId="439"/>
-    <cellStyle name="Normal 3" xfId="448"/>
-    <cellStyle name="Normal 3 2" xfId="500"/>
-    <cellStyle name="Normal 4" xfId="451"/>
-    <cellStyle name="Normal 4 2" xfId="81"/>
-    <cellStyle name="Normal 5" xfId="450"/>
-    <cellStyle name="Normal 5 2" xfId="242"/>
-    <cellStyle name="Normal 6" xfId="453"/>
-    <cellStyle name="Normal 6 10" xfId="41"/>
-    <cellStyle name="Normal 6 10 2" xfId="121"/>
-    <cellStyle name="Normal 6 10 2 2" xfId="168"/>
-    <cellStyle name="Normal 6 10 2 3" xfId="167"/>
-    <cellStyle name="Normal 6 10 3" xfId="118"/>
-    <cellStyle name="Normal 6 10 4" xfId="117"/>
-    <cellStyle name="Normal 6 11" xfId="40"/>
-    <cellStyle name="Normal 6 11 2" xfId="251"/>
-    <cellStyle name="Normal 6 11 2 2" xfId="421"/>
-    <cellStyle name="Normal 6 11 2 3" xfId="422"/>
-    <cellStyle name="Normal 6 11 3" xfId="252"/>
-    <cellStyle name="Normal 6 11 4" xfId="250"/>
-    <cellStyle name="Normal 6 12" xfId="43"/>
-    <cellStyle name="Normal 6 12 2" xfId="227"/>
-    <cellStyle name="Normal 6 12 2 2" xfId="181"/>
-    <cellStyle name="Normal 6 12 2 3" xfId="180"/>
-    <cellStyle name="Normal 6 12 3" xfId="226"/>
-    <cellStyle name="Normal 6 12 4" xfId="225"/>
-    <cellStyle name="Normal 6 13" xfId="42"/>
-    <cellStyle name="Normal 6 13 2" xfId="16"/>
-    <cellStyle name="Normal 6 13 2 2" xfId="503"/>
-    <cellStyle name="Normal 6 13 2 3" xfId="504"/>
-    <cellStyle name="Normal 6 13 3" xfId="17"/>
-    <cellStyle name="Normal 6 13 4" xfId="11"/>
-    <cellStyle name="Normal 6 14" xfId="45"/>
-    <cellStyle name="Normal 6 14 2" xfId="337"/>
-    <cellStyle name="Normal 6 14 2 2" xfId="76"/>
-    <cellStyle name="Normal 6 14 2 3" xfId="75"/>
-    <cellStyle name="Normal 6 14 3" xfId="336"/>
-    <cellStyle name="Normal 6 14 4" xfId="338"/>
-    <cellStyle name="Normal 6 15" xfId="44"/>
-    <cellStyle name="Normal 6 15 2" xfId="130"/>
-    <cellStyle name="Normal 6 15 3" xfId="131"/>
-    <cellStyle name="Normal 6 16" xfId="47"/>
-    <cellStyle name="Normal 6 17" xfId="46"/>
-    <cellStyle name="Normal 6 2" xfId="315"/>
-    <cellStyle name="Normal 6 2 10" xfId="233"/>
-    <cellStyle name="Normal 6 2 11" xfId="232"/>
-    <cellStyle name="Normal 6 2 2" xfId="578"/>
-    <cellStyle name="Normal 6 2 2 10" xfId="528"/>
-    <cellStyle name="Normal 6 2 2 2" xfId="465"/>
-    <cellStyle name="Normal 6 2 2 2 2" xfId="485"/>
-    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8"/>
-    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220"/>
-    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436"/>
-    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260"/>
-    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508"/>
-    <cellStyle name="Normal 6 2 2 2 3" xfId="191"/>
-    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497"/>
-    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57"/>
-    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54"/>
-    <cellStyle name="Normal 6 2 2 2 4" xfId="178"/>
-    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71"/>
-    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384"/>
-    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389"/>
-    <cellStyle name="Normal 6 2 2 2 5" xfId="177"/>
-    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592"/>
-    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593"/>
-    <cellStyle name="Normal 6 2 2 2 6" xfId="483"/>
-    <cellStyle name="Normal 6 2 2 2 7" xfId="482"/>
-    <cellStyle name="Normal 6 2 2 3" xfId="464"/>
-    <cellStyle name="Normal 6 2 2 3 2" xfId="24"/>
-    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561"/>
-    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231"/>
-    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228"/>
-    <cellStyle name="Normal 6 2 2 3 3" xfId="25"/>
-    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132"/>
-    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30"/>
-    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27"/>
-    <cellStyle name="Normal 6 2 2 3 4" xfId="20"/>
-    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193"/>
-    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194"/>
-    <cellStyle name="Normal 6 2 2 3 5" xfId="21"/>
-    <cellStyle name="Normal 6 2 2 3 6" xfId="22"/>
-    <cellStyle name="Normal 6 2 2 4" xfId="467"/>
-    <cellStyle name="Normal 6 2 2 4 2" xfId="206"/>
-    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143"/>
-    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544"/>
-    <cellStyle name="Normal 6 2 2 4 3" xfId="205"/>
-    <cellStyle name="Normal 6 2 2 4 4" xfId="533"/>
-    <cellStyle name="Normal 6 2 2 5" xfId="466"/>
-    <cellStyle name="Normal 6 2 2 5 2" xfId="405"/>
-    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248"/>
-    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249"/>
-    <cellStyle name="Normal 6 2 2 5 3" xfId="406"/>
-    <cellStyle name="Normal 6 2 2 5 4" xfId="408"/>
-    <cellStyle name="Normal 6 2 2 6" xfId="469"/>
-    <cellStyle name="Normal 6 2 2 6 2" xfId="602"/>
-    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590"/>
-    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589"/>
-    <cellStyle name="Normal 6 2 2 6 3" xfId="601"/>
-    <cellStyle name="Normal 6 2 2 6 4" xfId="603"/>
-    <cellStyle name="Normal 6 2 2 7" xfId="468"/>
-    <cellStyle name="Normal 6 2 2 7 2" xfId="156"/>
-    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262"/>
-    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263"/>
-    <cellStyle name="Normal 6 2 2 7 3" xfId="157"/>
-    <cellStyle name="Normal 6 2 2 7 4" xfId="158"/>
-    <cellStyle name="Normal 6 2 2 8" xfId="101"/>
-    <cellStyle name="Normal 6 2 2 8 2" xfId="349"/>
-    <cellStyle name="Normal 6 2 2 8 3" xfId="348"/>
-    <cellStyle name="Normal 6 2 2 9" xfId="99"/>
-    <cellStyle name="Normal 6 2 3" xfId="577"/>
-    <cellStyle name="Normal 6 2 3 2" xfId="12"/>
-    <cellStyle name="Normal 6 2 3 2 2" xfId="294"/>
-    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527"/>
-    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361"/>
-    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355"/>
-    <cellStyle name="Normal 6 2 3 2 3" xfId="295"/>
-    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442"/>
-    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172"/>
-    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169"/>
-    <cellStyle name="Normal 6 2 3 2 4" xfId="289"/>
-    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213"/>
-    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214"/>
-    <cellStyle name="Normal 6 2 3 2 5" xfId="290"/>
-    <cellStyle name="Normal 6 2 3 2 6" xfId="291"/>
-    <cellStyle name="Normal 6 2 3 3" xfId="13"/>
-    <cellStyle name="Normal 6 2 3 3 2" xfId="84"/>
-    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543"/>
-    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542"/>
-    <cellStyle name="Normal 6 2 3 3 3" xfId="83"/>
-    <cellStyle name="Normal 6 2 3 3 4" xfId="82"/>
-    <cellStyle name="Normal 6 2 3 4" xfId="14"/>
-    <cellStyle name="Normal 6 2 3 4 2" xfId="216"/>
-    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660"/>
-    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661"/>
-    <cellStyle name="Normal 6 2 3 4 3" xfId="55"/>
-    <cellStyle name="Normal 6 2 3 4 4" xfId="223"/>
-    <cellStyle name="Normal 6 2 3 5" xfId="15"/>
-    <cellStyle name="Normal 6 2 3 5 2" xfId="506"/>
-    <cellStyle name="Normal 6 2 3 5 3" xfId="505"/>
-    <cellStyle name="Normal 6 2 3 6" xfId="69"/>
-    <cellStyle name="Normal 6 2 3 7" xfId="72"/>
-    <cellStyle name="Normal 6 2 4" xfId="331"/>
-    <cellStyle name="Normal 6 2 4 2" xfId="400"/>
-    <cellStyle name="Normal 6 2 4 2 2" xfId="256"/>
-    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274"/>
-    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270"/>
-    <cellStyle name="Normal 6 2 4 2 3" xfId="255"/>
-    <cellStyle name="Normal 6 2 4 2 4" xfId="257"/>
-    <cellStyle name="Normal 6 2 4 3" xfId="399"/>
-    <cellStyle name="Normal 6 2 4 3 2" xfId="458"/>
-    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150"/>
-    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151"/>
-    <cellStyle name="Normal 6 2 4 3 3" xfId="459"/>
-    <cellStyle name="Normal 6 2 4 3 4" xfId="463"/>
-    <cellStyle name="Normal 6 2 4 4" xfId="398"/>
-    <cellStyle name="Normal 6 2 4 4 2" xfId="522"/>
-    <cellStyle name="Normal 6 2 4 4 3" xfId="521"/>
-    <cellStyle name="Normal 6 2 4 5" xfId="397"/>
-    <cellStyle name="Normal 6 2 4 6" xfId="396"/>
-    <cellStyle name="Normal 6 2 5" xfId="330"/>
-    <cellStyle name="Normal 6 2 5 2" xfId="569"/>
-    <cellStyle name="Normal 6 2 5 2 2" xfId="376"/>
-    <cellStyle name="Normal 6 2 5 2 3" xfId="377"/>
-    <cellStyle name="Normal 6 2 5 3" xfId="570"/>
-    <cellStyle name="Normal 6 2 5 4" xfId="568"/>
-    <cellStyle name="Normal 6 2 6" xfId="333"/>
-    <cellStyle name="Normal 6 2 6 2" xfId="632"/>
-    <cellStyle name="Normal 6 2 6 2 2" xfId="175"/>
-    <cellStyle name="Normal 6 2 6 2 3" xfId="174"/>
-    <cellStyle name="Normal 6 2 6 3" xfId="631"/>
-    <cellStyle name="Normal 6 2 6 4" xfId="630"/>
-    <cellStyle name="Normal 6 2 7" xfId="332"/>
-    <cellStyle name="Normal 6 2 7 2" xfId="195"/>
-    <cellStyle name="Normal 6 2 7 2 2" xfId="635"/>
-    <cellStyle name="Normal 6 2 7 2 3" xfId="636"/>
-    <cellStyle name="Normal 6 2 7 3" xfId="196"/>
-    <cellStyle name="Normal 6 2 7 4" xfId="427"/>
-    <cellStyle name="Normal 6 2 8" xfId="335"/>
-    <cellStyle name="Normal 6 2 8 2" xfId="474"/>
-    <cellStyle name="Normal 6 2 8 2 2" xfId="524"/>
-    <cellStyle name="Normal 6 2 8 2 3" xfId="523"/>
-    <cellStyle name="Normal 6 2 8 3" xfId="473"/>
-    <cellStyle name="Normal 6 2 8 4" xfId="479"/>
-    <cellStyle name="Normal 6 2 9" xfId="334"/>
-    <cellStyle name="Normal 6 2 9 2" xfId="26"/>
-    <cellStyle name="Normal 6 2 9 3" xfId="98"/>
-    <cellStyle name="Normal 6 3" xfId="314"/>
-    <cellStyle name="Normal 6 3 10" xfId="183"/>
-    <cellStyle name="Normal 6 3 2" xfId="548"/>
-    <cellStyle name="Normal 6 3 2 2" xfId="207"/>
-    <cellStyle name="Normal 6 3 2 2 2" xfId="237"/>
-    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90"/>
-    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51"/>
-    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48"/>
-    <cellStyle name="Normal 6 3 2 2 3" xfId="238"/>
-    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287"/>
-    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498"/>
-    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495"/>
-    <cellStyle name="Normal 6 3 2 2 4" xfId="234"/>
-    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612"/>
-    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613"/>
-    <cellStyle name="Normal 6 3 2 2 5" xfId="235"/>
-    <cellStyle name="Normal 6 3 2 2 6" xfId="236"/>
-    <cellStyle name="Normal 6 3 2 3" xfId="208"/>
-    <cellStyle name="Normal 6 3 2 3 2" xfId="37"/>
-    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394"/>
-    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393"/>
-    <cellStyle name="Normal 6 3 2 3 3" xfId="36"/>
-    <cellStyle name="Normal 6 3 2 3 4" xfId="35"/>
-    <cellStyle name="Normal 6 3 2 4" xfId="209"/>
-    <cellStyle name="Normal 6 3 2 4 2" xfId="627"/>
-    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486"/>
-    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487"/>
-    <cellStyle name="Normal 6 3 2 4 3" xfId="628"/>
-    <cellStyle name="Normal 6 3 2 4 4" xfId="629"/>
-    <cellStyle name="Normal 6 3 2 5" xfId="210"/>
-    <cellStyle name="Normal 6 3 2 5 2" xfId="431"/>
-    <cellStyle name="Normal 6 3 2 5 3" xfId="430"/>
-    <cellStyle name="Normal 6 3 2 6" xfId="211"/>
-    <cellStyle name="Normal 6 3 2 7" xfId="212"/>
-    <cellStyle name="Normal 6 3 3" xfId="549"/>
-    <cellStyle name="Normal 6 3 3 2" xfId="645"/>
-    <cellStyle name="Normal 6 3 3 2 2" xfId="558"/>
-    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190"/>
-    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189"/>
-    <cellStyle name="Normal 6 3 3 2 3" xfId="557"/>
-    <cellStyle name="Normal 6 3 3 2 4" xfId="556"/>
-    <cellStyle name="Normal 6 3 3 3" xfId="644"/>
-    <cellStyle name="Normal 6 3 3 3 2" xfId="114"/>
-    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653"/>
-    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654"/>
-    <cellStyle name="Normal 6 3 3 3 3" xfId="115"/>
-    <cellStyle name="Normal 6 3 3 3 4" xfId="112"/>
-    <cellStyle name="Normal 6 3 3 4" xfId="647"/>
-    <cellStyle name="Normal 6 3 3 4 2" xfId="317"/>
-    <cellStyle name="Normal 6 3 3 4 3" xfId="316"/>
-    <cellStyle name="Normal 6 3 3 5" xfId="646"/>
-    <cellStyle name="Normal 6 3 3 6" xfId="648"/>
-    <cellStyle name="Normal 6 3 4" xfId="550"/>
-    <cellStyle name="Normal 6 3 4 2" xfId="160"/>
-    <cellStyle name="Normal 6 3 4 2 2" xfId="470"/>
-    <cellStyle name="Normal 6 3 4 2 3" xfId="471"/>
-    <cellStyle name="Normal 6 3 4 3" xfId="164"/>
-    <cellStyle name="Normal 6 3 4 4" xfId="155"/>
-    <cellStyle name="Normal 6 3 5" xfId="551"/>
-    <cellStyle name="Normal 6 3 5 2" xfId="493"/>
-    <cellStyle name="Normal 6 3 5 2 2" xfId="53"/>
-    <cellStyle name="Normal 6 3 5 2 3" xfId="52"/>
-    <cellStyle name="Normal 6 3 5 3" xfId="492"/>
-    <cellStyle name="Normal 6 3 5 4" xfId="491"/>
-    <cellStyle name="Normal 6 3 6" xfId="552"/>
-    <cellStyle name="Normal 6 3 6 2" xfId="323"/>
-    <cellStyle name="Normal 6 3 6 2 2" xfId="153"/>
-    <cellStyle name="Normal 6 3 6 2 3" xfId="154"/>
-    <cellStyle name="Normal 6 3 6 3" xfId="324"/>
-    <cellStyle name="Normal 6 3 6 4" xfId="322"/>
-    <cellStyle name="Normal 6 3 7" xfId="553"/>
-    <cellStyle name="Normal 6 3 7 2" xfId="111"/>
-    <cellStyle name="Normal 6 3 7 2 2" xfId="347"/>
-    <cellStyle name="Normal 6 3 7 2 3" xfId="346"/>
-    <cellStyle name="Normal 6 3 7 3" xfId="110"/>
-    <cellStyle name="Normal 6 3 7 4" xfId="109"/>
-    <cellStyle name="Normal 6 3 8" xfId="501"/>
-    <cellStyle name="Normal 6 3 8 2" xfId="305"/>
-    <cellStyle name="Normal 6 3 8 3" xfId="306"/>
-    <cellStyle name="Normal 6 3 9" xfId="502"/>
-    <cellStyle name="Normal 6 4" xfId="311"/>
-    <cellStyle name="Normal 6 4 10" xfId="100"/>
-    <cellStyle name="Normal 6 4 2" xfId="92"/>
-    <cellStyle name="Normal 6 4 2 2" xfId="140"/>
-    <cellStyle name="Normal 6 4 2 2 2" xfId="375"/>
-    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381"/>
-    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266"/>
-    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268"/>
-    <cellStyle name="Normal 6 4 2 2 3" xfId="395"/>
-    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188"/>
-    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481"/>
-    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484"/>
-    <cellStyle name="Normal 6 4 2 2 4" xfId="402"/>
-    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429"/>
-    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428"/>
-    <cellStyle name="Normal 6 4 2 2 5" xfId="401"/>
-    <cellStyle name="Normal 6 4 2 2 6" xfId="379"/>
-    <cellStyle name="Normal 6 4 2 3" xfId="139"/>
-    <cellStyle name="Normal 6 4 2 3 2" xfId="587"/>
-    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655"/>
-    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656"/>
-    <cellStyle name="Normal 6 4 2 3 3" xfId="588"/>
-    <cellStyle name="Normal 6 4 2 3 4" xfId="591"/>
-    <cellStyle name="Normal 6 4 2 4" xfId="138"/>
-    <cellStyle name="Normal 6 4 2 4 2" xfId="623"/>
-    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605"/>
-    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604"/>
-    <cellStyle name="Normal 6 4 2 4 3" xfId="622"/>
-    <cellStyle name="Normal 6 4 2 4 4" xfId="621"/>
-    <cellStyle name="Normal 6 4 2 5" xfId="137"/>
-    <cellStyle name="Normal 6 4 2 5 2" xfId="184"/>
-    <cellStyle name="Normal 6 4 2 5 3" xfId="185"/>
-    <cellStyle name="Normal 6 4 2 6" xfId="136"/>
-    <cellStyle name="Normal 6 4 2 7" xfId="135"/>
-    <cellStyle name="Normal 6 4 3" xfId="91"/>
-    <cellStyle name="Normal 6 4 3 2" xfId="342"/>
-    <cellStyle name="Normal 6 4 3 2 2" xfId="200"/>
-    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127"/>
-    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128"/>
-    <cellStyle name="Normal 6 4 3 2 3" xfId="201"/>
-    <cellStyle name="Normal 6 4 3 2 4" xfId="204"/>
-    <cellStyle name="Normal 6 4 3 3" xfId="343"/>
-    <cellStyle name="Normal 6 4 3 3 2" xfId="643"/>
-    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298"/>
-    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297"/>
-    <cellStyle name="Normal 6 4 3 3 3" xfId="642"/>
-    <cellStyle name="Normal 6 4 3 3 4" xfId="583"/>
-    <cellStyle name="Normal 6 4 3 4" xfId="340"/>
-    <cellStyle name="Normal 6 4 3 4 2" xfId="444"/>
-    <cellStyle name="Normal 6 4 3 4 3" xfId="445"/>
-    <cellStyle name="Normal 6 4 3 5" xfId="341"/>
-    <cellStyle name="Normal 6 4 3 6" xfId="339"/>
-    <cellStyle name="Normal 6 4 4" xfId="441"/>
-    <cellStyle name="Normal 6 4 4 2" xfId="292"/>
-    <cellStyle name="Normal 6 4 4 2 2" xfId="247"/>
-    <cellStyle name="Normal 6 4 4 2 3" xfId="246"/>
-    <cellStyle name="Normal 6 4 4 3" xfId="412"/>
-    <cellStyle name="Normal 6 4 4 4" xfId="293"/>
-    <cellStyle name="Normal 6 4 5" xfId="440"/>
-    <cellStyle name="Normal 6 4 5 2" xfId="460"/>
-    <cellStyle name="Normal 6 4 5 2 2" xfId="517"/>
-    <cellStyle name="Normal 6 4 5 2 3" xfId="520"/>
-    <cellStyle name="Normal 6 4 5 3" xfId="461"/>
-    <cellStyle name="Normal 6 4 5 4" xfId="462"/>
-    <cellStyle name="Normal 6 4 6" xfId="88"/>
-    <cellStyle name="Normal 6 4 6 2" xfId="5"/>
-    <cellStyle name="Normal 6 4 6 2 2" xfId="595"/>
-    <cellStyle name="Normal 6 4 6 2 3" xfId="594"/>
-    <cellStyle name="Normal 6 4 6 3" xfId="4"/>
-    <cellStyle name="Normal 6 4 6 4" xfId="10"/>
-    <cellStyle name="Normal 6 4 7" xfId="87"/>
-    <cellStyle name="Normal 6 4 7 2" xfId="221"/>
-    <cellStyle name="Normal 6 4 7 2 2" xfId="403"/>
-    <cellStyle name="Normal 6 4 7 2 3" xfId="404"/>
-    <cellStyle name="Normal 6 4 7 3" xfId="222"/>
-    <cellStyle name="Normal 6 4 7 4" xfId="224"/>
-    <cellStyle name="Normal 6 4 8" xfId="97"/>
-    <cellStyle name="Normal 6 4 8 2" xfId="95"/>
-    <cellStyle name="Normal 6 4 8 3" xfId="380"/>
-    <cellStyle name="Normal 6 4 9" xfId="96"/>
-    <cellStyle name="Normal 6 5" xfId="310"/>
-    <cellStyle name="Normal 6 5 2" xfId="285"/>
-    <cellStyle name="Normal 6 5 2 2" xfId="534"/>
-    <cellStyle name="Normal 6 5 2 2 2" xfId="182"/>
-    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547"/>
-    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259"/>
-    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261"/>
-    <cellStyle name="Normal 6 5 2 2 3" xfId="417"/>
-    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106"/>
-    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301"/>
-    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79"/>
-    <cellStyle name="Normal 6 5 2 2 4" xfId="253"/>
-    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419"/>
-    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420"/>
-    <cellStyle name="Normal 6 5 2 2 5" xfId="254"/>
-    <cellStyle name="Normal 6 5 2 2 6" xfId="192"/>
-    <cellStyle name="Normal 6 5 2 3" xfId="535"/>
-    <cellStyle name="Normal 6 5 2 3 2" xfId="649"/>
-    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370"/>
-    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369"/>
-    <cellStyle name="Normal 6 5 2 3 3" xfId="70"/>
-    <cellStyle name="Normal 6 5 2 3 4" xfId="276"/>
-    <cellStyle name="Normal 6 5 2 4" xfId="532"/>
-    <cellStyle name="Normal 6 5 2 4 2" xfId="518"/>
-    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633"/>
-    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634"/>
-    <cellStyle name="Normal 6 5 2 4 3" xfId="519"/>
-    <cellStyle name="Normal 6 5 2 4 4" xfId="514"/>
-    <cellStyle name="Normal 6 5 2 5" xfId="447"/>
-    <cellStyle name="Normal 6 5 2 5 2" xfId="304"/>
-    <cellStyle name="Normal 6 5 2 5 3" xfId="303"/>
-    <cellStyle name="Normal 6 5 2 6" xfId="530"/>
-    <cellStyle name="Normal 6 5 2 7" xfId="531"/>
-    <cellStyle name="Normal 6 5 3" xfId="286"/>
-    <cellStyle name="Normal 6 5 3 2" xfId="321"/>
-    <cellStyle name="Normal 6 5 3 2 2" xfId="134"/>
-    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600"/>
-    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599"/>
-    <cellStyle name="Normal 6 5 3 2 3" xfId="229"/>
-    <cellStyle name="Normal 6 5 3 2 4" xfId="472"/>
-    <cellStyle name="Normal 6 5 3 3" xfId="320"/>
-    <cellStyle name="Normal 6 5 3 3 2" xfId="32"/>
-    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423"/>
-    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424"/>
-    <cellStyle name="Normal 6 5 3 3 3" xfId="34"/>
-    <cellStyle name="Normal 6 5 3 3 4" xfId="9"/>
-    <cellStyle name="Normal 6 5 3 4" xfId="319"/>
-    <cellStyle name="Normal 6 5 3 4 2" xfId="94"/>
-    <cellStyle name="Normal 6 5 3 4 3" xfId="93"/>
-    <cellStyle name="Normal 6 5 3 5" xfId="318"/>
-    <cellStyle name="Normal 6 5 3 6" xfId="525"/>
-    <cellStyle name="Normal 6 5 4" xfId="283"/>
-    <cellStyle name="Normal 6 5 4 2" xfId="582"/>
-    <cellStyle name="Normal 6 5 4 2 2" xfId="478"/>
-    <cellStyle name="Normal 6 5 4 2 3" xfId="639"/>
-    <cellStyle name="Normal 6 5 4 3" xfId="197"/>
-    <cellStyle name="Normal 6 5 4 4" xfId="584"/>
-    <cellStyle name="Normal 6 5 5" xfId="284"/>
-    <cellStyle name="Normal 6 5 5 2" xfId="387"/>
-    <cellStyle name="Normal 6 5 5 2 2" xfId="119"/>
-    <cellStyle name="Normal 6 5 5 2 3" xfId="33"/>
-    <cellStyle name="Normal 6 5 5 3" xfId="386"/>
-    <cellStyle name="Normal 6 5 5 4" xfId="388"/>
-    <cellStyle name="Normal 6 5 6" xfId="281"/>
-    <cellStyle name="Normal 6 5 6 2" xfId="74"/>
-    <cellStyle name="Normal 6 5 6 3" xfId="356"/>
-    <cellStyle name="Normal 6 5 7" xfId="282"/>
-    <cellStyle name="Normal 6 5 8" xfId="280"/>
-    <cellStyle name="Normal 6 6" xfId="313"/>
-    <cellStyle name="Normal 6 6 2" xfId="326"/>
-    <cellStyle name="Normal 6 6 2 2" xfId="245"/>
-    <cellStyle name="Normal 6 6 2 2 2" xfId="64"/>
-    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515"/>
-    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617"/>
-    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619"/>
-    <cellStyle name="Normal 6 6 2 2 3" xfId="113"/>
-    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457"/>
-    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296"/>
-    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176"/>
-    <cellStyle name="Normal 6 6 2 2 4" xfId="80"/>
-    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199"/>
-    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198"/>
-    <cellStyle name="Normal 6 6 2 2 5" xfId="77"/>
-    <cellStyle name="Normal 6 6 2 2 6" xfId="129"/>
-    <cellStyle name="Normal 6 6 2 3" xfId="163"/>
-    <cellStyle name="Normal 6 6 2 3 2" xfId="662"/>
-    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278"/>
-    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279"/>
-    <cellStyle name="Normal 6 6 2 3 3" xfId="1"/>
-    <cellStyle name="Normal 6 6 2 3 4" xfId="2"/>
-    <cellStyle name="Normal 6 6 2 4" xfId="586"/>
-    <cellStyle name="Normal 6 6 2 4 2" xfId="581"/>
-    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383"/>
-    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516"/>
-    <cellStyle name="Normal 6 6 2 4 3" xfId="580"/>
-    <cellStyle name="Normal 6 6 2 4 4" xfId="579"/>
-    <cellStyle name="Normal 6 6 2 5" xfId="159"/>
-    <cellStyle name="Normal 6 6 2 5 2" xfId="141"/>
-    <cellStyle name="Normal 6 6 2 5 3" xfId="142"/>
-    <cellStyle name="Normal 6 6 2 6" xfId="162"/>
-    <cellStyle name="Normal 6 6 2 7" xfId="161"/>
-    <cellStyle name="Normal 6 6 3" xfId="325"/>
-    <cellStyle name="Normal 6 6 3 2" xfId="374"/>
-    <cellStyle name="Normal 6 6 3 2 2" xfId="275"/>
-    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410"/>
-    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411"/>
-    <cellStyle name="Normal 6 6 3 2 3" xfId="362"/>
-    <cellStyle name="Normal 6 6 3 2 4" xfId="277"/>
-    <cellStyle name="Normal 6 6 3 3" xfId="186"/>
-    <cellStyle name="Normal 6 6 3 3 2" xfId="105"/>
-    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300"/>
-    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299"/>
-    <cellStyle name="Normal 6 6 3 3 3" xfId="104"/>
-    <cellStyle name="Normal 6 6 3 3 4" xfId="574"/>
-    <cellStyle name="Normal 6 6 3 4" xfId="371"/>
-    <cellStyle name="Normal 6 6 3 4 2" xfId="391"/>
-    <cellStyle name="Normal 6 6 3 4 3" xfId="392"/>
-    <cellStyle name="Normal 6 6 3 5" xfId="372"/>
-    <cellStyle name="Normal 6 6 3 6" xfId="373"/>
-    <cellStyle name="Normal 6 6 4" xfId="108"/>
-    <cellStyle name="Normal 6 6 4 2" xfId="435"/>
-    <cellStyle name="Normal 6 6 4 2 2" xfId="433"/>
-    <cellStyle name="Normal 6 6 4 2 3" xfId="432"/>
-    <cellStyle name="Normal 6 6 4 3" xfId="434"/>
-    <cellStyle name="Normal 6 6 4 4" xfId="438"/>
-    <cellStyle name="Normal 6 6 5" xfId="585"/>
-    <cellStyle name="Normal 6 6 5 2" xfId="596"/>
-    <cellStyle name="Normal 6 6 5 2 2" xfId="554"/>
-    <cellStyle name="Normal 6 6 5 2 3" xfId="555"/>
-    <cellStyle name="Normal 6 6 5 3" xfId="597"/>
-    <cellStyle name="Normal 6 6 5 4" xfId="598"/>
-    <cellStyle name="Normal 6 6 6" xfId="616"/>
-    <cellStyle name="Normal 6 6 6 2" xfId="29"/>
-    <cellStyle name="Normal 6 6 6 3" xfId="28"/>
-    <cellStyle name="Normal 6 6 7" xfId="507"/>
-    <cellStyle name="Normal 6 6 8" xfId="513"/>
-    <cellStyle name="Normal 6 7" xfId="312"/>
-    <cellStyle name="Normal 6 7 2" xfId="65"/>
-    <cellStyle name="Normal 6 7 2 2" xfId="610"/>
-    <cellStyle name="Normal 6 7 2 2 2" xfId="122"/>
-    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244"/>
-    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120"/>
-    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562"/>
-    <cellStyle name="Normal 6 7 2 2 3" xfId="123"/>
-    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144"/>
-    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357"/>
-    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359"/>
-    <cellStyle name="Normal 6 7 2 2 4" xfId="124"/>
-    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170"/>
-    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171"/>
-    <cellStyle name="Normal 6 7 2 2 5" xfId="125"/>
-    <cellStyle name="Normal 6 7 2 2 6" xfId="126"/>
-    <cellStyle name="Normal 6 7 2 3" xfId="611"/>
-    <cellStyle name="Normal 6 7 2 3 2" xfId="572"/>
-    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49"/>
-    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327"/>
-    <cellStyle name="Normal 6 7 2 3 3" xfId="571"/>
-    <cellStyle name="Normal 6 7 2 3 4" xfId="573"/>
-    <cellStyle name="Normal 6 7 2 4" xfId="606"/>
-    <cellStyle name="Normal 6 7 2 4 2" xfId="272"/>
-    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179"/>
-    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536"/>
-    <cellStyle name="Normal 6 7 2 4 3" xfId="273"/>
-    <cellStyle name="Normal 6 7 2 4 4" xfId="271"/>
-    <cellStyle name="Normal 6 7 2 5" xfId="607"/>
-    <cellStyle name="Normal 6 7 2 5 2" xfId="86"/>
-    <cellStyle name="Normal 6 7 2 5 3" xfId="85"/>
-    <cellStyle name="Normal 6 7 2 6" xfId="608"/>
-    <cellStyle name="Normal 6 7 2 7" xfId="609"/>
-    <cellStyle name="Normal 6 7 3" xfId="66"/>
-    <cellStyle name="Normal 6 7 3 2" xfId="409"/>
-    <cellStyle name="Normal 6 7 3 2 2" xfId="476"/>
-    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353"/>
-    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352"/>
-    <cellStyle name="Normal 6 7 3 2 3" xfId="475"/>
-    <cellStyle name="Normal 6 7 3 2 4" xfId="477"/>
-    <cellStyle name="Normal 6 7 3 3" xfId="418"/>
-    <cellStyle name="Normal 6 7 3 3 2" xfId="650"/>
-    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19"/>
-    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23"/>
-    <cellStyle name="Normal 6 7 3 3 3" xfId="651"/>
-    <cellStyle name="Normal 6 7 3 3 4" xfId="652"/>
-    <cellStyle name="Normal 6 7 3 4" xfId="414"/>
-    <cellStyle name="Normal 6 7 3 4 2" xfId="563"/>
-    <cellStyle name="Normal 6 7 3 4 3" xfId="620"/>
-    <cellStyle name="Normal 6 7 3 5" xfId="413"/>
-    <cellStyle name="Normal 6 7 3 6" xfId="407"/>
-    <cellStyle name="Normal 6 7 4" xfId="60"/>
-    <cellStyle name="Normal 6 7 4 2" xfId="166"/>
-    <cellStyle name="Normal 6 7 4 2 2" xfId="509"/>
-    <cellStyle name="Normal 6 7 4 2 3" xfId="510"/>
-    <cellStyle name="Normal 6 7 4 3" xfId="490"/>
-    <cellStyle name="Normal 6 7 4 4" xfId="494"/>
-    <cellStyle name="Normal 6 7 5" xfId="61"/>
-    <cellStyle name="Normal 6 7 5 2" xfId="638"/>
-    <cellStyle name="Normal 6 7 5 2 2" xfId="152"/>
-    <cellStyle name="Normal 6 7 5 2 3" xfId="38"/>
-    <cellStyle name="Normal 6 7 5 3" xfId="637"/>
-    <cellStyle name="Normal 6 7 5 4" xfId="641"/>
-    <cellStyle name="Normal 6 7 6" xfId="62"/>
-    <cellStyle name="Normal 6 7 6 2" xfId="415"/>
-    <cellStyle name="Normal 6 7 6 3" xfId="416"/>
-    <cellStyle name="Normal 6 7 7" xfId="63"/>
-    <cellStyle name="Normal 6 7 8" xfId="59"/>
-    <cellStyle name="Normal 6 8" xfId="308"/>
-    <cellStyle name="Normal 6 8 2" xfId="364"/>
-    <cellStyle name="Normal 6 8 2 2" xfId="146"/>
-    <cellStyle name="Normal 6 8 2 2 2" xfId="3"/>
-    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345"/>
-    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344"/>
-    <cellStyle name="Normal 6 8 2 2 3" xfId="18"/>
-    <cellStyle name="Normal 6 8 2 2 4" xfId="575"/>
-    <cellStyle name="Normal 6 8 2 3" xfId="145"/>
-    <cellStyle name="Normal 6 8 2 3 2" xfId="240"/>
-    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202"/>
-    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203"/>
-    <cellStyle name="Normal 6 8 2 3 3" xfId="241"/>
-    <cellStyle name="Normal 6 8 2 3 4" xfId="239"/>
-    <cellStyle name="Normal 6 8 2 4" xfId="149"/>
-    <cellStyle name="Normal 6 8 2 4 2" xfId="625"/>
-    <cellStyle name="Normal 6 8 2 4 3" xfId="624"/>
-    <cellStyle name="Normal 6 8 2 5" xfId="148"/>
-    <cellStyle name="Normal 6 8 2 6" xfId="147"/>
-    <cellStyle name="Normal 6 8 3" xfId="363"/>
-    <cellStyle name="Normal 6 8 3 2" xfId="350"/>
-    <cellStyle name="Normal 6 8 3 2 2" xfId="488"/>
-    <cellStyle name="Normal 6 8 3 2 3" xfId="489"/>
-    <cellStyle name="Normal 6 8 3 3" xfId="351"/>
-    <cellStyle name="Normal 6 8 3 4" xfId="354"/>
-    <cellStyle name="Normal 6 8 4" xfId="368"/>
-    <cellStyle name="Normal 6 8 4 2" xfId="565"/>
-    <cellStyle name="Normal 6 8 4 2 2" xfId="165"/>
-    <cellStyle name="Normal 6 8 4 2 3" xfId="446"/>
-    <cellStyle name="Normal 6 8 4 3" xfId="564"/>
-    <cellStyle name="Normal 6 8 4 4" xfId="559"/>
-    <cellStyle name="Normal 6 8 5" xfId="367"/>
-    <cellStyle name="Normal 6 8 5 2" xfId="102"/>
-    <cellStyle name="Normal 6 8 5 3" xfId="103"/>
-    <cellStyle name="Normal 6 8 6" xfId="366"/>
-    <cellStyle name="Normal 6 8 7" xfId="365"/>
-    <cellStyle name="Normal 6 9" xfId="307"/>
-    <cellStyle name="Normal 6 9 2" xfId="537"/>
-    <cellStyle name="Normal 6 9 2 2" xfId="215"/>
-    <cellStyle name="Normal 6 9 2 2 2" xfId="264"/>
-    <cellStyle name="Normal 6 9 2 2 3" xfId="265"/>
-    <cellStyle name="Normal 6 9 2 3" xfId="566"/>
-    <cellStyle name="Normal 6 9 2 4" xfId="217"/>
-    <cellStyle name="Normal 6 9 3" xfId="538"/>
-    <cellStyle name="Normal 6 9 3 2" xfId="658"/>
-    <cellStyle name="Normal 6 9 3 2 2" xfId="426"/>
-    <cellStyle name="Normal 6 9 3 2 3" xfId="425"/>
-    <cellStyle name="Normal 6 9 3 3" xfId="657"/>
-    <cellStyle name="Normal 6 9 3 4" xfId="659"/>
-    <cellStyle name="Normal 6 9 4" xfId="540"/>
-    <cellStyle name="Normal 6 9 4 2" xfId="640"/>
-    <cellStyle name="Normal 6 9 4 3" xfId="567"/>
-    <cellStyle name="Normal 6 9 5" xfId="541"/>
-    <cellStyle name="Normal 6 9 6" xfId="539"/>
-    <cellStyle name="Normal 7" xfId="452"/>
-    <cellStyle name="Normal 7 2" xfId="529"/>
-    <cellStyle name="Normal 8" xfId="455"/>
-    <cellStyle name="Normal 8 2" xfId="576"/>
-    <cellStyle name="Normal 9" xfId="454"/>
-    <cellStyle name="Normal 9 2" xfId="58"/>
-    <cellStyle name="Percent 2" xfId="269"/>
-    <cellStyle name="Percent 2 2" xfId="78"/>
+    <cellStyle name="Normal 10" xfId="545" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="449" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2" xfId="439" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 3" xfId="448" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3 2" xfId="500" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 4" xfId="451" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 4 2" xfId="81" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 5" xfId="450" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 5 2" xfId="242" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 6" xfId="453" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 6 10" xfId="41" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 6 10 2" xfId="121" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 6 10 2 2" xfId="168" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 6 10 2 3" xfId="167" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 6 10 3" xfId="118" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 6 10 4" xfId="117" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 6 11" xfId="40" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 6 11 2" xfId="251" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 6 11 2 2" xfId="421" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 6 11 2 3" xfId="422" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 6 11 3" xfId="252" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 6 11 4" xfId="250" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 6 12" xfId="43" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 6 12 2" xfId="227" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 6 12 2 2" xfId="181" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 6 12 2 3" xfId="180" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Normal 6 12 3" xfId="226" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 6 12 4" xfId="225" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Normal 6 13" xfId="42" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 6 13 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normal 6 13 2 2" xfId="503" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normal 6 13 2 3" xfId="504" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normal 6 13 3" xfId="17" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normal 6 13 4" xfId="11" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 6 14" xfId="45" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 6 14 2" xfId="337" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 6 14 2 2" xfId="76" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 6 14 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 6 14 3" xfId="336" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 6 14 4" xfId="338" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 6 15" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Normal 6 15 2" xfId="130" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Normal 6 15 3" xfId="131" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Normal 6 16" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 6 17" xfId="46" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Normal 6 2" xfId="315" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 6 2 10" xfId="233" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 6 2 11" xfId="232" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Normal 6 2 2" xfId="578" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Normal 6 2 2 10" xfId="528" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 6 2 2 2" xfId="465" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2" xfId="485" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3" xfId="191" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4" xfId="178" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5" xfId="177" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 6 2 2 2 6" xfId="483" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 6 2 2 2 7" xfId="482" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 6 2 2 3" xfId="464" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3" xfId="25" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4" xfId="20" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 6 2 2 3 5" xfId="21" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal 6 2 2 3 6" xfId="22" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Normal 6 2 2 4" xfId="467" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2" xfId="206" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Normal 6 2 2 4 3" xfId="205" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Normal 6 2 2 4 4" xfId="533" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Normal 6 2 2 5" xfId="466" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2" xfId="405" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Normal 6 2 2 5 3" xfId="406" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Normal 6 2 2 5 4" xfId="408" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Normal 6 2 2 6" xfId="469" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2" xfId="602" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Normal 6 2 2 6 3" xfId="601" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Normal 6 2 2 6 4" xfId="603" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Normal 6 2 2 7" xfId="468" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2" xfId="156" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Normal 6 2 2 7 3" xfId="157" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Normal 6 2 2 7 4" xfId="158" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Normal 6 2 2 8" xfId="101" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Normal 6 2 2 8 2" xfId="349" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Normal 6 2 2 8 3" xfId="348" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Normal 6 2 2 9" xfId="99" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Normal 6 2 3" xfId="577" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Normal 6 2 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2" xfId="294" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3" xfId="295" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4" xfId="289" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Normal 6 2 3 2 5" xfId="290" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Normal 6 2 3 2 6" xfId="291" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Normal 6 2 3 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2" xfId="84" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Normal 6 2 3 3 3" xfId="83" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Normal 6 2 3 3 4" xfId="82" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Normal 6 2 3 4" xfId="14" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2" xfId="216" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="Normal 6 2 3 4 3" xfId="55" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Normal 6 2 3 4 4" xfId="223" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Normal 6 2 3 5" xfId="15" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="Normal 6 2 3 5 2" xfId="506" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="Normal 6 2 3 5 3" xfId="505" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Normal 6 2 3 6" xfId="69" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Normal 6 2 3 7" xfId="72" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="Normal 6 2 4" xfId="331" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="Normal 6 2 4 2" xfId="400" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2" xfId="256" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="Normal 6 2 4 2 3" xfId="255" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="Normal 6 2 4 2 4" xfId="257" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="Normal 6 2 4 3" xfId="399" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2" xfId="458" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="Normal 6 2 4 3 3" xfId="459" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="Normal 6 2 4 3 4" xfId="463" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
+    <cellStyle name="Normal 6 2 4 4" xfId="398" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
+    <cellStyle name="Normal 6 2 4 4 2" xfId="522" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
+    <cellStyle name="Normal 6 2 4 4 3" xfId="521" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
+    <cellStyle name="Normal 6 2 4 5" xfId="397" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
+    <cellStyle name="Normal 6 2 4 6" xfId="396" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
+    <cellStyle name="Normal 6 2 5" xfId="330" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
+    <cellStyle name="Normal 6 2 5 2" xfId="569" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
+    <cellStyle name="Normal 6 2 5 2 2" xfId="376" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="Normal 6 2 5 2 3" xfId="377" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="Normal 6 2 5 3" xfId="570" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="Normal 6 2 5 4" xfId="568" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="Normal 6 2 6" xfId="333" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="Normal 6 2 6 2" xfId="632" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="Normal 6 2 6 2 2" xfId="175" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="Normal 6 2 6 2 3" xfId="174" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="Normal 6 2 6 3" xfId="631" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="Normal 6 2 6 4" xfId="630" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="Normal 6 2 7" xfId="332" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="Normal 6 2 7 2" xfId="195" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="Normal 6 2 7 2 2" xfId="635" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="Normal 6 2 7 2 3" xfId="636" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="Normal 6 2 7 3" xfId="196" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="Normal 6 2 7 4" xfId="427" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="Normal 6 2 8" xfId="335" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="Normal 6 2 8 2" xfId="474" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="Normal 6 2 8 2 2" xfId="524" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="Normal 6 2 8 2 3" xfId="523" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="Normal 6 2 8 3" xfId="473" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="Normal 6 2 8 4" xfId="479" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="Normal 6 2 9" xfId="334" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="Normal 6 2 9 2" xfId="26" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="Normal 6 2 9 3" xfId="98" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="Normal 6 3" xfId="314" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="Normal 6 3 10" xfId="183" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="Normal 6 3 2" xfId="548" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="Normal 6 3 2 2" xfId="207" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2" xfId="237" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3" xfId="238" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4" xfId="234" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
+    <cellStyle name="Normal 6 3 2 2 5" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="Normal 6 3 2 2 6" xfId="236" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
+    <cellStyle name="Normal 6 3 2 3" xfId="208" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2" xfId="37" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
+    <cellStyle name="Normal 6 3 2 3 3" xfId="36" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
+    <cellStyle name="Normal 6 3 2 3 4" xfId="35" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
+    <cellStyle name="Normal 6 3 2 4" xfId="209" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2" xfId="627" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
+    <cellStyle name="Normal 6 3 2 4 3" xfId="628" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="Normal 6 3 2 4 4" xfId="629" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
+    <cellStyle name="Normal 6 3 2 5" xfId="210" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="Normal 6 3 2 5 2" xfId="431" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
+    <cellStyle name="Normal 6 3 2 5 3" xfId="430" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
+    <cellStyle name="Normal 6 3 2 6" xfId="211" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
+    <cellStyle name="Normal 6 3 2 7" xfId="212" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
+    <cellStyle name="Normal 6 3 3" xfId="549" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
+    <cellStyle name="Normal 6 3 3 2" xfId="645" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2" xfId="558" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
+    <cellStyle name="Normal 6 3 3 2 3" xfId="557" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
+    <cellStyle name="Normal 6 3 3 2 4" xfId="556" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
+    <cellStyle name="Normal 6 3 3 3" xfId="644" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
+    <cellStyle name="Normal 6 3 3 3 3" xfId="115" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="Normal 6 3 3 3 4" xfId="112" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
+    <cellStyle name="Normal 6 3 3 4" xfId="647" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
+    <cellStyle name="Normal 6 3 3 4 2" xfId="317" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
+    <cellStyle name="Normal 6 3 3 4 3" xfId="316" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
+    <cellStyle name="Normal 6 3 3 5" xfId="646" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
+    <cellStyle name="Normal 6 3 3 6" xfId="648" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
+    <cellStyle name="Normal 6 3 4" xfId="550" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
+    <cellStyle name="Normal 6 3 4 2" xfId="160" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
+    <cellStyle name="Normal 6 3 4 2 2" xfId="470" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
+    <cellStyle name="Normal 6 3 4 2 3" xfId="471" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
+    <cellStyle name="Normal 6 3 4 3" xfId="164" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
+    <cellStyle name="Normal 6 3 4 4" xfId="155" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
+    <cellStyle name="Normal 6 3 5" xfId="551" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
+    <cellStyle name="Normal 6 3 5 2" xfId="493" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
+    <cellStyle name="Normal 6 3 5 2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
+    <cellStyle name="Normal 6 3 5 2 3" xfId="52" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
+    <cellStyle name="Normal 6 3 5 3" xfId="492" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
+    <cellStyle name="Normal 6 3 5 4" xfId="491" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
+    <cellStyle name="Normal 6 3 6" xfId="552" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
+    <cellStyle name="Normal 6 3 6 2" xfId="323" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
+    <cellStyle name="Normal 6 3 6 2 2" xfId="153" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
+    <cellStyle name="Normal 6 3 6 2 3" xfId="154" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
+    <cellStyle name="Normal 6 3 6 3" xfId="324" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
+    <cellStyle name="Normal 6 3 6 4" xfId="322" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
+    <cellStyle name="Normal 6 3 7" xfId="553" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
+    <cellStyle name="Normal 6 3 7 2" xfId="111" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
+    <cellStyle name="Normal 6 3 7 2 2" xfId="347" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
+    <cellStyle name="Normal 6 3 7 2 3" xfId="346" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
+    <cellStyle name="Normal 6 3 7 3" xfId="110" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
+    <cellStyle name="Normal 6 3 7 4" xfId="109" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
+    <cellStyle name="Normal 6 3 8" xfId="501" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
+    <cellStyle name="Normal 6 3 8 2" xfId="305" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
+    <cellStyle name="Normal 6 3 8 3" xfId="306" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
+    <cellStyle name="Normal 6 3 9" xfId="502" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
+    <cellStyle name="Normal 6 4" xfId="311" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
+    <cellStyle name="Normal 6 4 10" xfId="100" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
+    <cellStyle name="Normal 6 4 2" xfId="92" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
+    <cellStyle name="Normal 6 4 2 2" xfId="140" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2" xfId="375" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3" xfId="395" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4" xfId="402" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
+    <cellStyle name="Normal 6 4 2 2 5" xfId="401" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
+    <cellStyle name="Normal 6 4 2 2 6" xfId="379" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="Normal 6 4 2 3" xfId="139" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2" xfId="587" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
+    <cellStyle name="Normal 6 4 2 3 3" xfId="588" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
+    <cellStyle name="Normal 6 4 2 3 4" xfId="591" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="Normal 6 4 2 4" xfId="138" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2" xfId="623" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
+    <cellStyle name="Normal 6 4 2 4 3" xfId="622" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
+    <cellStyle name="Normal 6 4 2 4 4" xfId="621" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
+    <cellStyle name="Normal 6 4 2 5" xfId="137" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
+    <cellStyle name="Normal 6 4 2 5 2" xfId="184" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
+    <cellStyle name="Normal 6 4 2 5 3" xfId="185" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
+    <cellStyle name="Normal 6 4 2 6" xfId="136" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
+    <cellStyle name="Normal 6 4 2 7" xfId="135" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="Normal 6 4 3" xfId="91" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
+    <cellStyle name="Normal 6 4 3 2" xfId="342" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2" xfId="200" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
+    <cellStyle name="Normal 6 4 3 2 3" xfId="201" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
+    <cellStyle name="Normal 6 4 3 2 4" xfId="204" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
+    <cellStyle name="Normal 6 4 3 3" xfId="343" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2" xfId="643" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="Normal 6 4 3 3 3" xfId="642" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
+    <cellStyle name="Normal 6 4 3 3 4" xfId="583" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
+    <cellStyle name="Normal 6 4 3 4" xfId="340" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="Normal 6 4 3 4 2" xfId="444" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
+    <cellStyle name="Normal 6 4 3 4 3" xfId="445" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
+    <cellStyle name="Normal 6 4 3 5" xfId="341" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
+    <cellStyle name="Normal 6 4 3 6" xfId="339" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
+    <cellStyle name="Normal 6 4 4" xfId="441" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
+    <cellStyle name="Normal 6 4 4 2" xfId="292" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
+    <cellStyle name="Normal 6 4 4 2 2" xfId="247" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
+    <cellStyle name="Normal 6 4 4 2 3" xfId="246" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
+    <cellStyle name="Normal 6 4 4 3" xfId="412" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
+    <cellStyle name="Normal 6 4 4 4" xfId="293" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
+    <cellStyle name="Normal 6 4 5" xfId="440" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
+    <cellStyle name="Normal 6 4 5 2" xfId="460" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
+    <cellStyle name="Normal 6 4 5 2 2" xfId="517" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
+    <cellStyle name="Normal 6 4 5 2 3" xfId="520" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
+    <cellStyle name="Normal 6 4 5 3" xfId="461" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
+    <cellStyle name="Normal 6 4 5 4" xfId="462" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
+    <cellStyle name="Normal 6 4 6" xfId="88" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
+    <cellStyle name="Normal 6 4 6 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
+    <cellStyle name="Normal 6 4 6 2 2" xfId="595" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
+    <cellStyle name="Normal 6 4 6 2 3" xfId="594" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
+    <cellStyle name="Normal 6 4 6 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
+    <cellStyle name="Normal 6 4 6 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
+    <cellStyle name="Normal 6 4 7" xfId="87" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
+    <cellStyle name="Normal 6 4 7 2" xfId="221" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
+    <cellStyle name="Normal 6 4 7 2 2" xfId="403" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
+    <cellStyle name="Normal 6 4 7 2 3" xfId="404" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
+    <cellStyle name="Normal 6 4 7 3" xfId="222" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
+    <cellStyle name="Normal 6 4 7 4" xfId="224" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
+    <cellStyle name="Normal 6 4 8" xfId="97" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
+    <cellStyle name="Normal 6 4 8 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
+    <cellStyle name="Normal 6 4 8 3" xfId="380" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
+    <cellStyle name="Normal 6 4 9" xfId="96" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
+    <cellStyle name="Normal 6 5" xfId="310" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
+    <cellStyle name="Normal 6 5 2" xfId="285" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
+    <cellStyle name="Normal 6 5 2 2" xfId="534" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2" xfId="182" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3" xfId="417" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4" xfId="253" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
+    <cellStyle name="Normal 6 5 2 2 5" xfId="254" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
+    <cellStyle name="Normal 6 5 2 2 6" xfId="192" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
+    <cellStyle name="Normal 6 5 2 3" xfId="535" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2" xfId="649" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
+    <cellStyle name="Normal 6 5 2 3 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
+    <cellStyle name="Normal 6 5 2 3 4" xfId="276" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
+    <cellStyle name="Normal 6 5 2 4" xfId="532" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2" xfId="518" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
+    <cellStyle name="Normal 6 5 2 4 3" xfId="519" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
+    <cellStyle name="Normal 6 5 2 4 4" xfId="514" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
+    <cellStyle name="Normal 6 5 2 5" xfId="447" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
+    <cellStyle name="Normal 6 5 2 5 2" xfId="304" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
+    <cellStyle name="Normal 6 5 2 5 3" xfId="303" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
+    <cellStyle name="Normal 6 5 2 6" xfId="530" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
+    <cellStyle name="Normal 6 5 2 7" xfId="531" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
+    <cellStyle name="Normal 6 5 3" xfId="286" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
+    <cellStyle name="Normal 6 5 3 2" xfId="321" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2" xfId="134" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
+    <cellStyle name="Normal 6 5 3 2 3" xfId="229" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
+    <cellStyle name="Normal 6 5 3 2 4" xfId="472" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
+    <cellStyle name="Normal 6 5 3 3" xfId="320" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
+    <cellStyle name="Normal 6 5 3 3 3" xfId="34" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
+    <cellStyle name="Normal 6 5 3 3 4" xfId="9" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
+    <cellStyle name="Normal 6 5 3 4" xfId="319" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
+    <cellStyle name="Normal 6 5 3 4 2" xfId="94" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
+    <cellStyle name="Normal 6 5 3 4 3" xfId="93" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
+    <cellStyle name="Normal 6 5 3 5" xfId="318" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
+    <cellStyle name="Normal 6 5 3 6" xfId="525" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
+    <cellStyle name="Normal 6 5 4" xfId="283" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
+    <cellStyle name="Normal 6 5 4 2" xfId="582" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
+    <cellStyle name="Normal 6 5 4 2 2" xfId="478" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
+    <cellStyle name="Normal 6 5 4 2 3" xfId="639" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
+    <cellStyle name="Normal 6 5 4 3" xfId="197" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
+    <cellStyle name="Normal 6 5 4 4" xfId="584" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
+    <cellStyle name="Normal 6 5 5" xfId="284" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
+    <cellStyle name="Normal 6 5 5 2" xfId="387" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
+    <cellStyle name="Normal 6 5 5 2 2" xfId="119" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
+    <cellStyle name="Normal 6 5 5 2 3" xfId="33" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
+    <cellStyle name="Normal 6 5 5 3" xfId="386" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
+    <cellStyle name="Normal 6 5 5 4" xfId="388" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
+    <cellStyle name="Normal 6 5 6" xfId="281" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
+    <cellStyle name="Normal 6 5 6 2" xfId="74" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
+    <cellStyle name="Normal 6 5 6 3" xfId="356" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
+    <cellStyle name="Normal 6 5 7" xfId="282" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
+    <cellStyle name="Normal 6 5 8" xfId="280" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
+    <cellStyle name="Normal 6 6" xfId="313" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
+    <cellStyle name="Normal 6 6 2" xfId="326" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
+    <cellStyle name="Normal 6 6 2 2" xfId="245" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2" xfId="64" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3" xfId="113" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4" xfId="80" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
+    <cellStyle name="Normal 6 6 2 2 5" xfId="77" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
+    <cellStyle name="Normal 6 6 2 2 6" xfId="129" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
+    <cellStyle name="Normal 6 6 2 3" xfId="163" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2" xfId="662" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
+    <cellStyle name="Normal 6 6 2 3 3" xfId="1" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
+    <cellStyle name="Normal 6 6 2 3 4" xfId="2" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
+    <cellStyle name="Normal 6 6 2 4" xfId="586" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2" xfId="581" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
+    <cellStyle name="Normal 6 6 2 4 3" xfId="580" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
+    <cellStyle name="Normal 6 6 2 4 4" xfId="579" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
+    <cellStyle name="Normal 6 6 2 5" xfId="159" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
+    <cellStyle name="Normal 6 6 2 5 2" xfId="141" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
+    <cellStyle name="Normal 6 6 2 5 3" xfId="142" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
+    <cellStyle name="Normal 6 6 2 6" xfId="162" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
+    <cellStyle name="Normal 6 6 2 7" xfId="161" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
+    <cellStyle name="Normal 6 6 3" xfId="325" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
+    <cellStyle name="Normal 6 6 3 2" xfId="374" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2" xfId="275" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
+    <cellStyle name="Normal 6 6 3 2 3" xfId="362" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
+    <cellStyle name="Normal 6 6 3 2 4" xfId="277" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
+    <cellStyle name="Normal 6 6 3 3" xfId="186" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2" xfId="105" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
+    <cellStyle name="Normal 6 6 3 3 3" xfId="104" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
+    <cellStyle name="Normal 6 6 3 3 4" xfId="574" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
+    <cellStyle name="Normal 6 6 3 4" xfId="371" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
+    <cellStyle name="Normal 6 6 3 4 2" xfId="391" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
+    <cellStyle name="Normal 6 6 3 4 3" xfId="392" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
+    <cellStyle name="Normal 6 6 3 5" xfId="372" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
+    <cellStyle name="Normal 6 6 3 6" xfId="373" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
+    <cellStyle name="Normal 6 6 4" xfId="108" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
+    <cellStyle name="Normal 6 6 4 2" xfId="435" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
+    <cellStyle name="Normal 6 6 4 2 2" xfId="433" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
+    <cellStyle name="Normal 6 6 4 2 3" xfId="432" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
+    <cellStyle name="Normal 6 6 4 3" xfId="434" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
+    <cellStyle name="Normal 6 6 4 4" xfId="438" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
+    <cellStyle name="Normal 6 6 5" xfId="585" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
+    <cellStyle name="Normal 6 6 5 2" xfId="596" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
+    <cellStyle name="Normal 6 6 5 2 2" xfId="554" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
+    <cellStyle name="Normal 6 6 5 2 3" xfId="555" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
+    <cellStyle name="Normal 6 6 5 3" xfId="597" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
+    <cellStyle name="Normal 6 6 5 4" xfId="598" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
+    <cellStyle name="Normal 6 6 6" xfId="616" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
+    <cellStyle name="Normal 6 6 6 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
+    <cellStyle name="Normal 6 6 6 3" xfId="28" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
+    <cellStyle name="Normal 6 6 7" xfId="507" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
+    <cellStyle name="Normal 6 6 8" xfId="513" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
+    <cellStyle name="Normal 6 7" xfId="312" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
+    <cellStyle name="Normal 6 7 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
+    <cellStyle name="Normal 6 7 2 2" xfId="610" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4" xfId="124" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
+    <cellStyle name="Normal 6 7 2 2 5" xfId="125" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
+    <cellStyle name="Normal 6 7 2 2 6" xfId="126" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
+    <cellStyle name="Normal 6 7 2 3" xfId="611" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2" xfId="572" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
+    <cellStyle name="Normal 6 7 2 3 3" xfId="571" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
+    <cellStyle name="Normal 6 7 2 3 4" xfId="573" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
+    <cellStyle name="Normal 6 7 2 4" xfId="606" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2" xfId="272" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
+    <cellStyle name="Normal 6 7 2 4 3" xfId="273" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
+    <cellStyle name="Normal 6 7 2 4 4" xfId="271" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
+    <cellStyle name="Normal 6 7 2 5" xfId="607" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
+    <cellStyle name="Normal 6 7 2 5 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
+    <cellStyle name="Normal 6 7 2 5 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
+    <cellStyle name="Normal 6 7 2 6" xfId="608" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
+    <cellStyle name="Normal 6 7 2 7" xfId="609" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
+    <cellStyle name="Normal 6 7 3" xfId="66" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
+    <cellStyle name="Normal 6 7 3 2" xfId="409" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2" xfId="476" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
+    <cellStyle name="Normal 6 7 3 2 3" xfId="475" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
+    <cellStyle name="Normal 6 7 3 2 4" xfId="477" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
+    <cellStyle name="Normal 6 7 3 3" xfId="418" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2" xfId="650" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
+    <cellStyle name="Normal 6 7 3 3 3" xfId="651" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
+    <cellStyle name="Normal 6 7 3 3 4" xfId="652" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
+    <cellStyle name="Normal 6 7 3 4" xfId="414" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
+    <cellStyle name="Normal 6 7 3 4 2" xfId="563" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
+    <cellStyle name="Normal 6 7 3 4 3" xfId="620" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
+    <cellStyle name="Normal 6 7 3 5" xfId="413" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
+    <cellStyle name="Normal 6 7 3 6" xfId="407" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
+    <cellStyle name="Normal 6 7 4" xfId="60" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
+    <cellStyle name="Normal 6 7 4 2" xfId="166" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
+    <cellStyle name="Normal 6 7 4 2 2" xfId="509" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
+    <cellStyle name="Normal 6 7 4 2 3" xfId="510" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
+    <cellStyle name="Normal 6 7 4 3" xfId="490" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
+    <cellStyle name="Normal 6 7 4 4" xfId="494" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
+    <cellStyle name="Normal 6 7 5" xfId="61" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
+    <cellStyle name="Normal 6 7 5 2" xfId="638" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
+    <cellStyle name="Normal 6 7 5 2 2" xfId="152" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
+    <cellStyle name="Normal 6 7 5 2 3" xfId="38" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
+    <cellStyle name="Normal 6 7 5 3" xfId="637" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
+    <cellStyle name="Normal 6 7 5 4" xfId="641" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
+    <cellStyle name="Normal 6 7 6" xfId="62" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
+    <cellStyle name="Normal 6 7 6 2" xfId="415" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
+    <cellStyle name="Normal 6 7 6 3" xfId="416" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
+    <cellStyle name="Normal 6 7 7" xfId="63" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
+    <cellStyle name="Normal 6 7 8" xfId="59" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
+    <cellStyle name="Normal 6 8" xfId="308" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
+    <cellStyle name="Normal 6 8 2" xfId="364" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
+    <cellStyle name="Normal 6 8 2 2" xfId="146" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
+    <cellStyle name="Normal 6 8 2 2 3" xfId="18" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
+    <cellStyle name="Normal 6 8 2 2 4" xfId="575" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
+    <cellStyle name="Normal 6 8 2 3" xfId="145" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2" xfId="240" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
+    <cellStyle name="Normal 6 8 2 3 3" xfId="241" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
+    <cellStyle name="Normal 6 8 2 3 4" xfId="239" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
+    <cellStyle name="Normal 6 8 2 4" xfId="149" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
+    <cellStyle name="Normal 6 8 2 4 2" xfId="625" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
+    <cellStyle name="Normal 6 8 2 4 3" xfId="624" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
+    <cellStyle name="Normal 6 8 2 5" xfId="148" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
+    <cellStyle name="Normal 6 8 2 6" xfId="147" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
+    <cellStyle name="Normal 6 8 3" xfId="363" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
+    <cellStyle name="Normal 6 8 3 2" xfId="350" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
+    <cellStyle name="Normal 6 8 3 2 2" xfId="488" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
+    <cellStyle name="Normal 6 8 3 2 3" xfId="489" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
+    <cellStyle name="Normal 6 8 3 3" xfId="351" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
+    <cellStyle name="Normal 6 8 3 4" xfId="354" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
+    <cellStyle name="Normal 6 8 4" xfId="368" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
+    <cellStyle name="Normal 6 8 4 2" xfId="565" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
+    <cellStyle name="Normal 6 8 4 2 2" xfId="165" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
+    <cellStyle name="Normal 6 8 4 2 3" xfId="446" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
+    <cellStyle name="Normal 6 8 4 3" xfId="564" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
+    <cellStyle name="Normal 6 8 4 4" xfId="559" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
+    <cellStyle name="Normal 6 8 5" xfId="367" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
+    <cellStyle name="Normal 6 8 5 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
+    <cellStyle name="Normal 6 8 5 3" xfId="103" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
+    <cellStyle name="Normal 6 8 6" xfId="366" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
+    <cellStyle name="Normal 6 8 7" xfId="365" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
+    <cellStyle name="Normal 6 9" xfId="307" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
+    <cellStyle name="Normal 6 9 2" xfId="537" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
+    <cellStyle name="Normal 6 9 2 2" xfId="215" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
+    <cellStyle name="Normal 6 9 2 2 2" xfId="264" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
+    <cellStyle name="Normal 6 9 2 2 3" xfId="265" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
+    <cellStyle name="Normal 6 9 2 3" xfId="566" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
+    <cellStyle name="Normal 6 9 2 4" xfId="217" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
+    <cellStyle name="Normal 6 9 3" xfId="538" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
+    <cellStyle name="Normal 6 9 3 2" xfId="658" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
+    <cellStyle name="Normal 6 9 3 2 2" xfId="426" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
+    <cellStyle name="Normal 6 9 3 2 3" xfId="425" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
+    <cellStyle name="Normal 6 9 3 3" xfId="657" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
+    <cellStyle name="Normal 6 9 3 4" xfId="659" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
+    <cellStyle name="Normal 6 9 4" xfId="540" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
+    <cellStyle name="Normal 6 9 4 2" xfId="640" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
+    <cellStyle name="Normal 6 9 4 3" xfId="567" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
+    <cellStyle name="Normal 6 9 5" xfId="541" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
+    <cellStyle name="Normal 6 9 6" xfId="539" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
+    <cellStyle name="Normal 7" xfId="452" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
+    <cellStyle name="Normal 7 2" xfId="529" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
+    <cellStyle name="Normal 8" xfId="455" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
+    <cellStyle name="Normal 8 2" xfId="576" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
+    <cellStyle name="Normal 9" xfId="454" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
+    <cellStyle name="Normal 9 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
+    <cellStyle name="Percent 2" xfId="269" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
+    <cellStyle name="Percent 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1641,7 +1715,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1674,9 +1748,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1709,6 +1800,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1884,25 +1992,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="19" customWidth="1"/>
-    <col min="3" max="8" width="9.140625" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="51.5546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="19" customWidth="1"/>
+    <col min="3" max="8" width="9.109375" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1910,42 +2018,122 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="23">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="25">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="26">
+        <v>220000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="26">
+        <v>807610</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="19">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="19">
+        <v>2000</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{FAA95EF1-203A-4444-9E84-DB4F2FBB8CD8}">
+      <formula1>-10000</formula1>
+      <formula2>10000</formula2>
+    </dataValidation>
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B5:B6" xr:uid="{0FC7A138-FA33-4811-8FA6-C94730F85756}">
+      <formula1>0</formula1>
+      <formula2>10000000000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{3E598E5F-6CB6-4BE4-88E7-3E3DC2A25D2F}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{1E31B6DE-8F0F-4067-A47F-00EDE838D564}">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="56" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" customWidth="1"/>
     <col min="4" max="4" width="11" style="17" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="7.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="7.44140625" style="1" customWidth="1"/>
     <col min="8" max="11" width="7" style="1" customWidth="1"/>
-    <col min="12" max="13" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7.85546875" style="1" customWidth="1"/>
-    <col min="16" max="20" width="9.140625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="13" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="7.88671875" style="1" customWidth="1"/>
+    <col min="16" max="20" width="9.109375" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1992,7 +2180,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
@@ -2008,7 +2196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -2024,14 +2212,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E2:O2">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E2:O2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2042,7 +2254,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
@@ -2052,7 +2264,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Prepare spreadsheet to run a scenario for Bhutan
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A506B9C9-AD24-4FCF-81D9-8A36816D59AE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EA281E0-7D00-47A6-81BE-24C109BBF993}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>parameter</t>
   </si>
@@ -48,9 +48,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>riskgroup_perc_diabetes</t>
-  </si>
-  <si>
     <t>scipy</t>
   </si>
   <si>
@@ -87,7 +84,19 @@
     <t>plot_start_time</t>
   </si>
   <si>
-    <t>program_perc_detect</t>
+    <t>program_perc_treatment_new_success</t>
+  </si>
+  <si>
+    <t>scenario_1</t>
+  </si>
+  <si>
+    <t>scenario_2</t>
+  </si>
+  <si>
+    <t>scenario_3</t>
+  </si>
+  <si>
+    <t>scenario_4</t>
   </si>
 </sst>
 </file>
@@ -145,14 +154,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="5" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="5" tint="-0.499984740745262"/>
       <name val="Calibri"/>
@@ -176,13 +177,18 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,19 +203,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -956,43 +956,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="661" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="661" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="661" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="661" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="661" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="661" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="661" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="661" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="661" applyFont="1"/>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="661" applyFont="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="662" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="662" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="662" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="662" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="661" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="661" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="661" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="661" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="661" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="661" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1999,84 +2000,82 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="19" customWidth="1"/>
-    <col min="3" max="8" width="9.109375" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="16"/>
+    <col min="1" max="1" width="51.5546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="6" customWidth="1"/>
+    <col min="3" max="8" width="9.109375" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="21">
-        <v>40</v>
+      <c r="A2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="8">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="23">
+      <c r="A3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="10">
         <v>0.99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="25">
+      <c r="A4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="12">
         <v>1900</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="26">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="13">
         <v>220000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="26">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="13">
         <v>807610</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="19">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6">
         <v>5</v>
       </c>
       <c r="C7">
         <v>15</v>
       </c>
-      <c r="D7">
-        <v>25</v>
-      </c>
+      <c r="D7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="19">
+      <c r="A8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6">
         <v>2000</v>
       </c>
     </row>
@@ -2109,147 +2108,167 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11" style="17" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="7.44140625" style="1" customWidth="1"/>
-    <col min="8" max="11" width="7" style="1" customWidth="1"/>
-    <col min="12" max="13" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7.88671875" style="1" customWidth="1"/>
-    <col min="16" max="20" width="9.109375" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="56" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="23" customWidth="1"/>
+    <col min="4" max="4" width="11" style="24" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" style="24" customWidth="1"/>
+    <col min="6" max="7" width="7.44140625" style="24" customWidth="1"/>
+    <col min="8" max="11" width="7" style="24" customWidth="1"/>
+    <col min="12" max="13" width="7.44140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="7.88671875" style="24" customWidth="1"/>
+    <col min="16" max="16" width="10.77734375" style="24" customWidth="1"/>
+    <col min="17" max="18" width="10" style="24" customWidth="1"/>
+    <col min="19" max="19" width="10.21875" style="24" customWidth="1"/>
+    <col min="20" max="20" width="9.109375" style="24" customWidth="1"/>
+    <col min="21" max="16384" width="9.109375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="17">
         <v>1920</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="17">
         <v>1980</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="17">
         <v>1993</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="17">
         <v>2000</v>
       </c>
-      <c r="H1" s="14">
+      <c r="H1" s="17">
         <v>2002</v>
       </c>
-      <c r="I1" s="14">
+      <c r="I1" s="17">
         <v>2004</v>
       </c>
-      <c r="J1" s="14">
+      <c r="J1" s="17">
         <v>2009</v>
       </c>
-      <c r="K1" s="14">
+      <c r="K1" s="17">
         <v>2011</v>
       </c>
-      <c r="L1" s="14">
+      <c r="L1" s="17">
         <v>2012</v>
       </c>
-      <c r="M1" s="14">
+      <c r="M1" s="17">
         <v>2013</v>
       </c>
-      <c r="N1" s="14">
+      <c r="N1" s="17">
         <v>2014</v>
       </c>
-      <c r="O1" s="14">
+      <c r="O1" s="17">
         <v>2015</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="12"/>
-      <c r="K2" s="6">
+      <c r="C2" s="19"/>
+      <c r="J2" s="20">
         <v>0</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="20">
         <v>1</v>
       </c>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
     </row>
-    <row r="3" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="13"/>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="O3" s="8">
-        <v>1</v>
-      </c>
+      <c r="C3" s="19"/>
+      <c r="P3" s="20">
+        <v>75</v>
+      </c>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
     </row>
-    <row r="4" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
+    <row r="4" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+    </row>
+    <row r="6" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E2:O2" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations count="4">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E2:O2 Q2:Q3" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E3:Q3" xr:uid="{402091F8-A3FA-4E40-8099-07B402378B02}">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C6:C1048576 C2:C4" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2274,10 +2293,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2288,15 +2307,15 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bhutan calibration after adjusting CDR curve
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EA281E0-7D00-47A6-81BE-24C109BBF993}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0498D65B-1BE2-4E99-BB7F-6CAEF1FFAB3E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,12 @@
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>parameter</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>scenario_4</t>
+  </si>
+  <si>
+    <t>program_perc_detect</t>
+  </si>
+  <si>
+    <t>program_perc_nonsuccess_new_death</t>
   </si>
 </sst>
 </file>
@@ -188,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,12 +210,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -956,7 +956,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="661" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -988,12 +988,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="661" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="661" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="661" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="662" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="662" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="662" applyFont="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2000,7 +1997,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2024,7 +2021,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="8">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2108,13 +2105,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2152,7 +2149,7 @@
         <v>1980</v>
       </c>
       <c r="F1" s="17">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="G1" s="17">
         <v>2000</v>
@@ -2235,34 +2232,66 @@
       <c r="V3" s="21"/>
     </row>
     <row r="4" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
+      <c r="A4" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
     </row>
     <row r="6" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>5</v>
+      </c>
       <c r="C6" s="19"/>
+      <c r="F6" s="20">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="21"/>
+    </row>
+    <row r="7" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E2:O2 Q2:Q3" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E2:O2 Q2:Q3 Q5:Q6" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E3:Q3" xr:uid="{402091F8-A3FA-4E40-8099-07B402378B02}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E3:Q3 E5:Q6" xr:uid="{402091F8-A3FA-4E40-8099-07B402378B02}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C6:C1048576 C2:C4" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
remove compartments and flow for dorm age0to5
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swas0001\swas_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0498D65B-1BE2-4E99-BB7F-6CAEF1FFAB3E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15340" windowHeight="5500"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -108,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -993,669 +992,669 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="662" applyFont="1"/>
   </cellXfs>
   <cellStyles count="663">
-    <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Comma 2 2" xfId="626" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Input 2" xfId="378" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Comma 2" xfId="614"/>
+    <cellStyle name="Comma 2 2" xfId="626"/>
+    <cellStyle name="Input 2" xfId="378"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="545" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 2" xfId="449" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 2 2" xfId="439" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 3" xfId="448" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 3 2" xfId="500" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 4" xfId="451" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 4 2" xfId="81" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 5" xfId="450" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 5 2" xfId="242" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 6" xfId="453" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Normal 6 10" xfId="41" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Normal 6 10 2" xfId="121" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Normal 6 10 2 2" xfId="168" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Normal 6 10 2 3" xfId="167" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Normal 6 10 3" xfId="118" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Normal 6 10 4" xfId="117" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Normal 6 11" xfId="40" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Normal 6 11 2" xfId="251" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Normal 6 11 2 2" xfId="421" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Normal 6 11 2 3" xfId="422" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Normal 6 11 3" xfId="252" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Normal 6 11 4" xfId="250" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Normal 6 12" xfId="43" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Normal 6 12 2" xfId="227" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Normal 6 12 2 2" xfId="181" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Normal 6 12 2 3" xfId="180" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Normal 6 12 3" xfId="226" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Normal 6 12 4" xfId="225" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Normal 6 13" xfId="42" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Normal 6 13 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Normal 6 13 2 2" xfId="503" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Normal 6 13 2 3" xfId="504" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Normal 6 13 3" xfId="17" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Normal 6 13 4" xfId="11" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Normal 6 14" xfId="45" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Normal 6 14 2" xfId="337" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Normal 6 14 2 2" xfId="76" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Normal 6 14 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Normal 6 14 3" xfId="336" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Normal 6 14 4" xfId="338" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Normal 6 15" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Normal 6 15 2" xfId="130" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Normal 6 15 3" xfId="131" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Normal 6 16" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Normal 6 17" xfId="46" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Normal 6 2" xfId="315" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Normal 6 2 10" xfId="233" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Normal 6 2 11" xfId="232" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Normal 6 2 2" xfId="578" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Normal 6 2 2 10" xfId="528" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Normal 6 2 2 2" xfId="465" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2" xfId="485" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Normal 6 2 2 2 3" xfId="191" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 6 2 2 2 4" xfId="178" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Normal 6 2 2 2 5" xfId="177" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 6 2 2 2 6" xfId="483" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 6 2 2 2 7" xfId="482" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 6 2 2 3" xfId="464" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 6 2 2 3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3" xfId="25" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 6 2 2 3 4" xfId="20" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 6 2 2 3 5" xfId="21" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 6 2 2 3 6" xfId="22" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 6 2 2 4" xfId="467" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 6 2 2 4 2" xfId="206" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 6 2 2 4 3" xfId="205" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 6 2 2 4 4" xfId="533" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Normal 6 2 2 5" xfId="466" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Normal 6 2 2 5 2" xfId="405" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Normal 6 2 2 5 3" xfId="406" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Normal 6 2 2 5 4" xfId="408" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Normal 6 2 2 6" xfId="469" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Normal 6 2 2 6 2" xfId="602" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Normal 6 2 2 6 3" xfId="601" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Normal 6 2 2 6 4" xfId="603" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Normal 6 2 2 7" xfId="468" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Normal 6 2 2 7 2" xfId="156" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Normal 6 2 2 7 3" xfId="157" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Normal 6 2 2 7 4" xfId="158" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Normal 6 2 2 8" xfId="101" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Normal 6 2 2 8 2" xfId="349" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Normal 6 2 2 8 3" xfId="348" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Normal 6 2 2 9" xfId="99" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Normal 6 2 3" xfId="577" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Normal 6 2 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Normal 6 2 3 2 2" xfId="294" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Normal 6 2 3 2 3" xfId="295" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Normal 6 2 3 2 4" xfId="289" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Normal 6 2 3 2 5" xfId="290" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="Normal 6 2 3 2 6" xfId="291" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="Normal 6 2 3 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="Normal 6 2 3 3 2" xfId="84" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="Normal 6 2 3 3 3" xfId="83" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="Normal 6 2 3 3 4" xfId="82" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
-    <cellStyle name="Normal 6 2 3 4" xfId="14" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="Normal 6 2 3 4 2" xfId="216" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
-    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
-    <cellStyle name="Normal 6 2 3 4 3" xfId="55" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
-    <cellStyle name="Normal 6 2 3 4 4" xfId="223" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
-    <cellStyle name="Normal 6 2 3 5" xfId="15" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
-    <cellStyle name="Normal 6 2 3 5 2" xfId="506" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
-    <cellStyle name="Normal 6 2 3 5 3" xfId="505" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
-    <cellStyle name="Normal 6 2 3 6" xfId="69" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
-    <cellStyle name="Normal 6 2 3 7" xfId="72" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
-    <cellStyle name="Normal 6 2 4" xfId="331" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
-    <cellStyle name="Normal 6 2 4 2" xfId="400" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
-    <cellStyle name="Normal 6 2 4 2 2" xfId="256" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
-    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
-    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
-    <cellStyle name="Normal 6 2 4 2 3" xfId="255" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
-    <cellStyle name="Normal 6 2 4 2 4" xfId="257" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
-    <cellStyle name="Normal 6 2 4 3" xfId="399" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
-    <cellStyle name="Normal 6 2 4 3 2" xfId="458" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
-    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
-    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
-    <cellStyle name="Normal 6 2 4 3 3" xfId="459" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
-    <cellStyle name="Normal 6 2 4 3 4" xfId="463" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
-    <cellStyle name="Normal 6 2 4 4" xfId="398" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
-    <cellStyle name="Normal 6 2 4 4 2" xfId="522" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
-    <cellStyle name="Normal 6 2 4 4 3" xfId="521" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
-    <cellStyle name="Normal 6 2 4 5" xfId="397" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
-    <cellStyle name="Normal 6 2 4 6" xfId="396" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
-    <cellStyle name="Normal 6 2 5" xfId="330" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
-    <cellStyle name="Normal 6 2 5 2" xfId="569" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
-    <cellStyle name="Normal 6 2 5 2 2" xfId="376" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
-    <cellStyle name="Normal 6 2 5 2 3" xfId="377" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
-    <cellStyle name="Normal 6 2 5 3" xfId="570" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
-    <cellStyle name="Normal 6 2 5 4" xfId="568" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
-    <cellStyle name="Normal 6 2 6" xfId="333" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
-    <cellStyle name="Normal 6 2 6 2" xfId="632" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
-    <cellStyle name="Normal 6 2 6 2 2" xfId="175" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
-    <cellStyle name="Normal 6 2 6 2 3" xfId="174" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
-    <cellStyle name="Normal 6 2 6 3" xfId="631" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
-    <cellStyle name="Normal 6 2 6 4" xfId="630" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
-    <cellStyle name="Normal 6 2 7" xfId="332" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
-    <cellStyle name="Normal 6 2 7 2" xfId="195" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
-    <cellStyle name="Normal 6 2 7 2 2" xfId="635" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
-    <cellStyle name="Normal 6 2 7 2 3" xfId="636" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
-    <cellStyle name="Normal 6 2 7 3" xfId="196" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
-    <cellStyle name="Normal 6 2 7 4" xfId="427" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
-    <cellStyle name="Normal 6 2 8" xfId="335" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
-    <cellStyle name="Normal 6 2 8 2" xfId="474" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
-    <cellStyle name="Normal 6 2 8 2 2" xfId="524" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
-    <cellStyle name="Normal 6 2 8 2 3" xfId="523" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
-    <cellStyle name="Normal 6 2 8 3" xfId="473" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
-    <cellStyle name="Normal 6 2 8 4" xfId="479" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
-    <cellStyle name="Normal 6 2 9" xfId="334" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
-    <cellStyle name="Normal 6 2 9 2" xfId="26" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
-    <cellStyle name="Normal 6 2 9 3" xfId="98" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
-    <cellStyle name="Normal 6 3" xfId="314" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
-    <cellStyle name="Normal 6 3 10" xfId="183" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
-    <cellStyle name="Normal 6 3 2" xfId="548" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
-    <cellStyle name="Normal 6 3 2 2" xfId="207" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2" xfId="237" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
-    <cellStyle name="Normal 6 3 2 2 3" xfId="238" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
-    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
-    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
-    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
-    <cellStyle name="Normal 6 3 2 2 4" xfId="234" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
-    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
-    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
-    <cellStyle name="Normal 6 3 2 2 5" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
-    <cellStyle name="Normal 6 3 2 2 6" xfId="236" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
-    <cellStyle name="Normal 6 3 2 3" xfId="208" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
-    <cellStyle name="Normal 6 3 2 3 2" xfId="37" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
-    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
-    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
-    <cellStyle name="Normal 6 3 2 3 3" xfId="36" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
-    <cellStyle name="Normal 6 3 2 3 4" xfId="35" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
-    <cellStyle name="Normal 6 3 2 4" xfId="209" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
-    <cellStyle name="Normal 6 3 2 4 2" xfId="627" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
-    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
-    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
-    <cellStyle name="Normal 6 3 2 4 3" xfId="628" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
-    <cellStyle name="Normal 6 3 2 4 4" xfId="629" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
-    <cellStyle name="Normal 6 3 2 5" xfId="210" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
-    <cellStyle name="Normal 6 3 2 5 2" xfId="431" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
-    <cellStyle name="Normal 6 3 2 5 3" xfId="430" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
-    <cellStyle name="Normal 6 3 2 6" xfId="211" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
-    <cellStyle name="Normal 6 3 2 7" xfId="212" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
-    <cellStyle name="Normal 6 3 3" xfId="549" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
-    <cellStyle name="Normal 6 3 3 2" xfId="645" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
-    <cellStyle name="Normal 6 3 3 2 2" xfId="558" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
-    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
-    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
-    <cellStyle name="Normal 6 3 3 2 3" xfId="557" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
-    <cellStyle name="Normal 6 3 3 2 4" xfId="556" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
-    <cellStyle name="Normal 6 3 3 3" xfId="644" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
-    <cellStyle name="Normal 6 3 3 3 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
-    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
-    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
-    <cellStyle name="Normal 6 3 3 3 3" xfId="115" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
-    <cellStyle name="Normal 6 3 3 3 4" xfId="112" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
-    <cellStyle name="Normal 6 3 3 4" xfId="647" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
-    <cellStyle name="Normal 6 3 3 4 2" xfId="317" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
-    <cellStyle name="Normal 6 3 3 4 3" xfId="316" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
-    <cellStyle name="Normal 6 3 3 5" xfId="646" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
-    <cellStyle name="Normal 6 3 3 6" xfId="648" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
-    <cellStyle name="Normal 6 3 4" xfId="550" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
-    <cellStyle name="Normal 6 3 4 2" xfId="160" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
-    <cellStyle name="Normal 6 3 4 2 2" xfId="470" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
-    <cellStyle name="Normal 6 3 4 2 3" xfId="471" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
-    <cellStyle name="Normal 6 3 4 3" xfId="164" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
-    <cellStyle name="Normal 6 3 4 4" xfId="155" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
-    <cellStyle name="Normal 6 3 5" xfId="551" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
-    <cellStyle name="Normal 6 3 5 2" xfId="493" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
-    <cellStyle name="Normal 6 3 5 2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
-    <cellStyle name="Normal 6 3 5 2 3" xfId="52" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
-    <cellStyle name="Normal 6 3 5 3" xfId="492" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
-    <cellStyle name="Normal 6 3 5 4" xfId="491" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
-    <cellStyle name="Normal 6 3 6" xfId="552" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
-    <cellStyle name="Normal 6 3 6 2" xfId="323" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
-    <cellStyle name="Normal 6 3 6 2 2" xfId="153" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
-    <cellStyle name="Normal 6 3 6 2 3" xfId="154" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
-    <cellStyle name="Normal 6 3 6 3" xfId="324" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
-    <cellStyle name="Normal 6 3 6 4" xfId="322" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
-    <cellStyle name="Normal 6 3 7" xfId="553" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
-    <cellStyle name="Normal 6 3 7 2" xfId="111" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
-    <cellStyle name="Normal 6 3 7 2 2" xfId="347" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
-    <cellStyle name="Normal 6 3 7 2 3" xfId="346" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
-    <cellStyle name="Normal 6 3 7 3" xfId="110" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
-    <cellStyle name="Normal 6 3 7 4" xfId="109" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
-    <cellStyle name="Normal 6 3 8" xfId="501" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
-    <cellStyle name="Normal 6 3 8 2" xfId="305" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
-    <cellStyle name="Normal 6 3 8 3" xfId="306" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
-    <cellStyle name="Normal 6 3 9" xfId="502" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
-    <cellStyle name="Normal 6 4" xfId="311" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
-    <cellStyle name="Normal 6 4 10" xfId="100" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
-    <cellStyle name="Normal 6 4 2" xfId="92" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
-    <cellStyle name="Normal 6 4 2 2" xfId="140" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
-    <cellStyle name="Normal 6 4 2 2 2" xfId="375" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
-    <cellStyle name="Normal 6 4 2 2 3" xfId="395" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
-    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
-    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
-    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
-    <cellStyle name="Normal 6 4 2 2 4" xfId="402" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
-    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
-    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
-    <cellStyle name="Normal 6 4 2 2 5" xfId="401" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
-    <cellStyle name="Normal 6 4 2 2 6" xfId="379" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
-    <cellStyle name="Normal 6 4 2 3" xfId="139" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
-    <cellStyle name="Normal 6 4 2 3 2" xfId="587" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
-    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
-    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
-    <cellStyle name="Normal 6 4 2 3 3" xfId="588" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
-    <cellStyle name="Normal 6 4 2 3 4" xfId="591" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
-    <cellStyle name="Normal 6 4 2 4" xfId="138" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
-    <cellStyle name="Normal 6 4 2 4 2" xfId="623" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
-    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
-    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
-    <cellStyle name="Normal 6 4 2 4 3" xfId="622" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
-    <cellStyle name="Normal 6 4 2 4 4" xfId="621" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
-    <cellStyle name="Normal 6 4 2 5" xfId="137" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
-    <cellStyle name="Normal 6 4 2 5 2" xfId="184" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
-    <cellStyle name="Normal 6 4 2 5 3" xfId="185" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
-    <cellStyle name="Normal 6 4 2 6" xfId="136" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
-    <cellStyle name="Normal 6 4 2 7" xfId="135" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
-    <cellStyle name="Normal 6 4 3" xfId="91" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
-    <cellStyle name="Normal 6 4 3 2" xfId="342" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
-    <cellStyle name="Normal 6 4 3 2 2" xfId="200" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
-    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
-    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
-    <cellStyle name="Normal 6 4 3 2 3" xfId="201" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
-    <cellStyle name="Normal 6 4 3 2 4" xfId="204" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
-    <cellStyle name="Normal 6 4 3 3" xfId="343" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
-    <cellStyle name="Normal 6 4 3 3 2" xfId="643" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
-    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
-    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
-    <cellStyle name="Normal 6 4 3 3 3" xfId="642" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
-    <cellStyle name="Normal 6 4 3 3 4" xfId="583" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
-    <cellStyle name="Normal 6 4 3 4" xfId="340" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
-    <cellStyle name="Normal 6 4 3 4 2" xfId="444" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
-    <cellStyle name="Normal 6 4 3 4 3" xfId="445" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
-    <cellStyle name="Normal 6 4 3 5" xfId="341" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
-    <cellStyle name="Normal 6 4 3 6" xfId="339" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
-    <cellStyle name="Normal 6 4 4" xfId="441" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
-    <cellStyle name="Normal 6 4 4 2" xfId="292" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
-    <cellStyle name="Normal 6 4 4 2 2" xfId="247" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
-    <cellStyle name="Normal 6 4 4 2 3" xfId="246" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
-    <cellStyle name="Normal 6 4 4 3" xfId="412" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
-    <cellStyle name="Normal 6 4 4 4" xfId="293" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
-    <cellStyle name="Normal 6 4 5" xfId="440" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
-    <cellStyle name="Normal 6 4 5 2" xfId="460" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
-    <cellStyle name="Normal 6 4 5 2 2" xfId="517" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
-    <cellStyle name="Normal 6 4 5 2 3" xfId="520" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
-    <cellStyle name="Normal 6 4 5 3" xfId="461" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
-    <cellStyle name="Normal 6 4 5 4" xfId="462" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
-    <cellStyle name="Normal 6 4 6" xfId="88" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
-    <cellStyle name="Normal 6 4 6 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
-    <cellStyle name="Normal 6 4 6 2 2" xfId="595" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
-    <cellStyle name="Normal 6 4 6 2 3" xfId="594" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
-    <cellStyle name="Normal 6 4 6 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
-    <cellStyle name="Normal 6 4 6 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
-    <cellStyle name="Normal 6 4 7" xfId="87" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
-    <cellStyle name="Normal 6 4 7 2" xfId="221" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
-    <cellStyle name="Normal 6 4 7 2 2" xfId="403" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
-    <cellStyle name="Normal 6 4 7 2 3" xfId="404" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
-    <cellStyle name="Normal 6 4 7 3" xfId="222" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
-    <cellStyle name="Normal 6 4 7 4" xfId="224" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
-    <cellStyle name="Normal 6 4 8" xfId="97" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
-    <cellStyle name="Normal 6 4 8 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
-    <cellStyle name="Normal 6 4 8 3" xfId="380" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
-    <cellStyle name="Normal 6 4 9" xfId="96" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
-    <cellStyle name="Normal 6 5" xfId="310" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
-    <cellStyle name="Normal 6 5 2" xfId="285" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
-    <cellStyle name="Normal 6 5 2 2" xfId="534" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
-    <cellStyle name="Normal 6 5 2 2 2" xfId="182" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
-    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
-    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
-    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
-    <cellStyle name="Normal 6 5 2 2 3" xfId="417" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
-    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
-    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
-    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
-    <cellStyle name="Normal 6 5 2 2 4" xfId="253" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
-    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
-    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
-    <cellStyle name="Normal 6 5 2 2 5" xfId="254" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
-    <cellStyle name="Normal 6 5 2 2 6" xfId="192" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
-    <cellStyle name="Normal 6 5 2 3" xfId="535" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
-    <cellStyle name="Normal 6 5 2 3 2" xfId="649" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
-    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
-    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
-    <cellStyle name="Normal 6 5 2 3 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
-    <cellStyle name="Normal 6 5 2 3 4" xfId="276" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
-    <cellStyle name="Normal 6 5 2 4" xfId="532" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
-    <cellStyle name="Normal 6 5 2 4 2" xfId="518" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
-    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
-    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
-    <cellStyle name="Normal 6 5 2 4 3" xfId="519" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
-    <cellStyle name="Normal 6 5 2 4 4" xfId="514" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
-    <cellStyle name="Normal 6 5 2 5" xfId="447" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
-    <cellStyle name="Normal 6 5 2 5 2" xfId="304" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
-    <cellStyle name="Normal 6 5 2 5 3" xfId="303" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
-    <cellStyle name="Normal 6 5 2 6" xfId="530" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
-    <cellStyle name="Normal 6 5 2 7" xfId="531" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
-    <cellStyle name="Normal 6 5 3" xfId="286" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
-    <cellStyle name="Normal 6 5 3 2" xfId="321" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
-    <cellStyle name="Normal 6 5 3 2 2" xfId="134" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
-    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
-    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
-    <cellStyle name="Normal 6 5 3 2 3" xfId="229" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
-    <cellStyle name="Normal 6 5 3 2 4" xfId="472" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
-    <cellStyle name="Normal 6 5 3 3" xfId="320" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
-    <cellStyle name="Normal 6 5 3 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
-    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
-    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
-    <cellStyle name="Normal 6 5 3 3 3" xfId="34" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
-    <cellStyle name="Normal 6 5 3 3 4" xfId="9" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
-    <cellStyle name="Normal 6 5 3 4" xfId="319" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
-    <cellStyle name="Normal 6 5 3 4 2" xfId="94" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
-    <cellStyle name="Normal 6 5 3 4 3" xfId="93" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
-    <cellStyle name="Normal 6 5 3 5" xfId="318" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
-    <cellStyle name="Normal 6 5 3 6" xfId="525" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
-    <cellStyle name="Normal 6 5 4" xfId="283" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
-    <cellStyle name="Normal 6 5 4 2" xfId="582" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
-    <cellStyle name="Normal 6 5 4 2 2" xfId="478" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
-    <cellStyle name="Normal 6 5 4 2 3" xfId="639" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
-    <cellStyle name="Normal 6 5 4 3" xfId="197" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
-    <cellStyle name="Normal 6 5 4 4" xfId="584" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
-    <cellStyle name="Normal 6 5 5" xfId="284" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
-    <cellStyle name="Normal 6 5 5 2" xfId="387" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
-    <cellStyle name="Normal 6 5 5 2 2" xfId="119" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
-    <cellStyle name="Normal 6 5 5 2 3" xfId="33" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
-    <cellStyle name="Normal 6 5 5 3" xfId="386" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
-    <cellStyle name="Normal 6 5 5 4" xfId="388" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
-    <cellStyle name="Normal 6 5 6" xfId="281" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
-    <cellStyle name="Normal 6 5 6 2" xfId="74" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
-    <cellStyle name="Normal 6 5 6 3" xfId="356" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
-    <cellStyle name="Normal 6 5 7" xfId="282" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
-    <cellStyle name="Normal 6 5 8" xfId="280" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
-    <cellStyle name="Normal 6 6" xfId="313" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
-    <cellStyle name="Normal 6 6 2" xfId="326" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
-    <cellStyle name="Normal 6 6 2 2" xfId="245" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
-    <cellStyle name="Normal 6 6 2 2 2" xfId="64" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
-    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
-    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
-    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
-    <cellStyle name="Normal 6 6 2 2 3" xfId="113" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
-    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
-    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
-    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
-    <cellStyle name="Normal 6 6 2 2 4" xfId="80" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
-    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
-    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
-    <cellStyle name="Normal 6 6 2 2 5" xfId="77" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
-    <cellStyle name="Normal 6 6 2 2 6" xfId="129" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
-    <cellStyle name="Normal 6 6 2 3" xfId="163" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
-    <cellStyle name="Normal 6 6 2 3 2" xfId="662" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
-    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
-    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
-    <cellStyle name="Normal 6 6 2 3 3" xfId="1" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
-    <cellStyle name="Normal 6 6 2 3 4" xfId="2" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
-    <cellStyle name="Normal 6 6 2 4" xfId="586" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
-    <cellStyle name="Normal 6 6 2 4 2" xfId="581" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
-    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
-    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
-    <cellStyle name="Normal 6 6 2 4 3" xfId="580" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
-    <cellStyle name="Normal 6 6 2 4 4" xfId="579" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
-    <cellStyle name="Normal 6 6 2 5" xfId="159" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
-    <cellStyle name="Normal 6 6 2 5 2" xfId="141" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
-    <cellStyle name="Normal 6 6 2 5 3" xfId="142" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
-    <cellStyle name="Normal 6 6 2 6" xfId="162" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
-    <cellStyle name="Normal 6 6 2 7" xfId="161" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
-    <cellStyle name="Normal 6 6 3" xfId="325" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
-    <cellStyle name="Normal 6 6 3 2" xfId="374" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
-    <cellStyle name="Normal 6 6 3 2 2" xfId="275" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
-    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
-    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
-    <cellStyle name="Normal 6 6 3 2 3" xfId="362" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
-    <cellStyle name="Normal 6 6 3 2 4" xfId="277" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
-    <cellStyle name="Normal 6 6 3 3" xfId="186" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
-    <cellStyle name="Normal 6 6 3 3 2" xfId="105" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
-    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
-    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
-    <cellStyle name="Normal 6 6 3 3 3" xfId="104" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
-    <cellStyle name="Normal 6 6 3 3 4" xfId="574" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
-    <cellStyle name="Normal 6 6 3 4" xfId="371" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
-    <cellStyle name="Normal 6 6 3 4 2" xfId="391" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
-    <cellStyle name="Normal 6 6 3 4 3" xfId="392" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
-    <cellStyle name="Normal 6 6 3 5" xfId="372" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
-    <cellStyle name="Normal 6 6 3 6" xfId="373" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
-    <cellStyle name="Normal 6 6 4" xfId="108" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
-    <cellStyle name="Normal 6 6 4 2" xfId="435" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
-    <cellStyle name="Normal 6 6 4 2 2" xfId="433" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
-    <cellStyle name="Normal 6 6 4 2 3" xfId="432" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
-    <cellStyle name="Normal 6 6 4 3" xfId="434" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
-    <cellStyle name="Normal 6 6 4 4" xfId="438" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
-    <cellStyle name="Normal 6 6 5" xfId="585" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
-    <cellStyle name="Normal 6 6 5 2" xfId="596" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
-    <cellStyle name="Normal 6 6 5 2 2" xfId="554" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
-    <cellStyle name="Normal 6 6 5 2 3" xfId="555" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
-    <cellStyle name="Normal 6 6 5 3" xfId="597" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
-    <cellStyle name="Normal 6 6 5 4" xfId="598" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
-    <cellStyle name="Normal 6 6 6" xfId="616" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
-    <cellStyle name="Normal 6 6 6 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
-    <cellStyle name="Normal 6 6 6 3" xfId="28" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
-    <cellStyle name="Normal 6 6 7" xfId="507" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
-    <cellStyle name="Normal 6 6 8" xfId="513" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
-    <cellStyle name="Normal 6 7" xfId="312" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
-    <cellStyle name="Normal 6 7 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
-    <cellStyle name="Normal 6 7 2 2" xfId="610" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
-    <cellStyle name="Normal 6 7 2 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
-    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
-    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
-    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
-    <cellStyle name="Normal 6 7 2 2 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
-    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
-    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
-    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
-    <cellStyle name="Normal 6 7 2 2 4" xfId="124" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
-    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
-    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
-    <cellStyle name="Normal 6 7 2 2 5" xfId="125" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
-    <cellStyle name="Normal 6 7 2 2 6" xfId="126" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
-    <cellStyle name="Normal 6 7 2 3" xfId="611" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
-    <cellStyle name="Normal 6 7 2 3 2" xfId="572" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
-    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
-    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
-    <cellStyle name="Normal 6 7 2 3 3" xfId="571" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
-    <cellStyle name="Normal 6 7 2 3 4" xfId="573" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
-    <cellStyle name="Normal 6 7 2 4" xfId="606" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
-    <cellStyle name="Normal 6 7 2 4 2" xfId="272" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
-    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
-    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
-    <cellStyle name="Normal 6 7 2 4 3" xfId="273" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
-    <cellStyle name="Normal 6 7 2 4 4" xfId="271" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
-    <cellStyle name="Normal 6 7 2 5" xfId="607" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
-    <cellStyle name="Normal 6 7 2 5 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
-    <cellStyle name="Normal 6 7 2 5 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
-    <cellStyle name="Normal 6 7 2 6" xfId="608" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
-    <cellStyle name="Normal 6 7 2 7" xfId="609" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
-    <cellStyle name="Normal 6 7 3" xfId="66" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
-    <cellStyle name="Normal 6 7 3 2" xfId="409" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
-    <cellStyle name="Normal 6 7 3 2 2" xfId="476" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
-    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
-    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
-    <cellStyle name="Normal 6 7 3 2 3" xfId="475" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
-    <cellStyle name="Normal 6 7 3 2 4" xfId="477" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
-    <cellStyle name="Normal 6 7 3 3" xfId="418" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
-    <cellStyle name="Normal 6 7 3 3 2" xfId="650" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
-    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
-    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
-    <cellStyle name="Normal 6 7 3 3 3" xfId="651" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
-    <cellStyle name="Normal 6 7 3 3 4" xfId="652" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
-    <cellStyle name="Normal 6 7 3 4" xfId="414" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
-    <cellStyle name="Normal 6 7 3 4 2" xfId="563" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
-    <cellStyle name="Normal 6 7 3 4 3" xfId="620" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
-    <cellStyle name="Normal 6 7 3 5" xfId="413" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
-    <cellStyle name="Normal 6 7 3 6" xfId="407" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
-    <cellStyle name="Normal 6 7 4" xfId="60" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
-    <cellStyle name="Normal 6 7 4 2" xfId="166" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
-    <cellStyle name="Normal 6 7 4 2 2" xfId="509" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
-    <cellStyle name="Normal 6 7 4 2 3" xfId="510" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
-    <cellStyle name="Normal 6 7 4 3" xfId="490" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
-    <cellStyle name="Normal 6 7 4 4" xfId="494" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
-    <cellStyle name="Normal 6 7 5" xfId="61" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
-    <cellStyle name="Normal 6 7 5 2" xfId="638" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
-    <cellStyle name="Normal 6 7 5 2 2" xfId="152" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
-    <cellStyle name="Normal 6 7 5 2 3" xfId="38" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
-    <cellStyle name="Normal 6 7 5 3" xfId="637" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
-    <cellStyle name="Normal 6 7 5 4" xfId="641" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
-    <cellStyle name="Normal 6 7 6" xfId="62" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
-    <cellStyle name="Normal 6 7 6 2" xfId="415" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
-    <cellStyle name="Normal 6 7 6 3" xfId="416" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
-    <cellStyle name="Normal 6 7 7" xfId="63" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
-    <cellStyle name="Normal 6 7 8" xfId="59" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
-    <cellStyle name="Normal 6 8" xfId="308" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
-    <cellStyle name="Normal 6 8 2" xfId="364" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
-    <cellStyle name="Normal 6 8 2 2" xfId="146" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
-    <cellStyle name="Normal 6 8 2 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
-    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
-    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
-    <cellStyle name="Normal 6 8 2 2 3" xfId="18" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
-    <cellStyle name="Normal 6 8 2 2 4" xfId="575" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
-    <cellStyle name="Normal 6 8 2 3" xfId="145" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
-    <cellStyle name="Normal 6 8 2 3 2" xfId="240" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
-    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
-    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
-    <cellStyle name="Normal 6 8 2 3 3" xfId="241" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
-    <cellStyle name="Normal 6 8 2 3 4" xfId="239" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
-    <cellStyle name="Normal 6 8 2 4" xfId="149" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
-    <cellStyle name="Normal 6 8 2 4 2" xfId="625" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
-    <cellStyle name="Normal 6 8 2 4 3" xfId="624" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
-    <cellStyle name="Normal 6 8 2 5" xfId="148" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
-    <cellStyle name="Normal 6 8 2 6" xfId="147" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
-    <cellStyle name="Normal 6 8 3" xfId="363" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
-    <cellStyle name="Normal 6 8 3 2" xfId="350" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
-    <cellStyle name="Normal 6 8 3 2 2" xfId="488" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
-    <cellStyle name="Normal 6 8 3 2 3" xfId="489" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
-    <cellStyle name="Normal 6 8 3 3" xfId="351" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
-    <cellStyle name="Normal 6 8 3 4" xfId="354" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
-    <cellStyle name="Normal 6 8 4" xfId="368" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
-    <cellStyle name="Normal 6 8 4 2" xfId="565" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
-    <cellStyle name="Normal 6 8 4 2 2" xfId="165" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
-    <cellStyle name="Normal 6 8 4 2 3" xfId="446" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
-    <cellStyle name="Normal 6 8 4 3" xfId="564" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
-    <cellStyle name="Normal 6 8 4 4" xfId="559" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
-    <cellStyle name="Normal 6 8 5" xfId="367" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
-    <cellStyle name="Normal 6 8 5 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
-    <cellStyle name="Normal 6 8 5 3" xfId="103" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
-    <cellStyle name="Normal 6 8 6" xfId="366" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
-    <cellStyle name="Normal 6 8 7" xfId="365" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
-    <cellStyle name="Normal 6 9" xfId="307" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
-    <cellStyle name="Normal 6 9 2" xfId="537" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
-    <cellStyle name="Normal 6 9 2 2" xfId="215" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
-    <cellStyle name="Normal 6 9 2 2 2" xfId="264" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
-    <cellStyle name="Normal 6 9 2 2 3" xfId="265" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
-    <cellStyle name="Normal 6 9 2 3" xfId="566" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
-    <cellStyle name="Normal 6 9 2 4" xfId="217" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
-    <cellStyle name="Normal 6 9 3" xfId="538" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
-    <cellStyle name="Normal 6 9 3 2" xfId="658" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
-    <cellStyle name="Normal 6 9 3 2 2" xfId="426" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
-    <cellStyle name="Normal 6 9 3 2 3" xfId="425" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
-    <cellStyle name="Normal 6 9 3 3" xfId="657" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
-    <cellStyle name="Normal 6 9 3 4" xfId="659" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
-    <cellStyle name="Normal 6 9 4" xfId="540" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
-    <cellStyle name="Normal 6 9 4 2" xfId="640" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
-    <cellStyle name="Normal 6 9 4 3" xfId="567" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
-    <cellStyle name="Normal 6 9 5" xfId="541" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
-    <cellStyle name="Normal 6 9 6" xfId="539" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
-    <cellStyle name="Normal 7" xfId="452" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
-    <cellStyle name="Normal 7 2" xfId="529" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
-    <cellStyle name="Normal 8" xfId="455" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
-    <cellStyle name="Normal 8 2" xfId="576" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
-    <cellStyle name="Normal 9" xfId="454" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
-    <cellStyle name="Normal 9 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
-    <cellStyle name="Percent 2" xfId="269" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
-    <cellStyle name="Percent 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
+    <cellStyle name="Normal 10" xfId="545"/>
+    <cellStyle name="Normal 2" xfId="449"/>
+    <cellStyle name="Normal 2 2" xfId="439"/>
+    <cellStyle name="Normal 3" xfId="448"/>
+    <cellStyle name="Normal 3 2" xfId="500"/>
+    <cellStyle name="Normal 4" xfId="451"/>
+    <cellStyle name="Normal 4 2" xfId="81"/>
+    <cellStyle name="Normal 5" xfId="450"/>
+    <cellStyle name="Normal 5 2" xfId="242"/>
+    <cellStyle name="Normal 6" xfId="453"/>
+    <cellStyle name="Normal 6 10" xfId="41"/>
+    <cellStyle name="Normal 6 10 2" xfId="121"/>
+    <cellStyle name="Normal 6 10 2 2" xfId="168"/>
+    <cellStyle name="Normal 6 10 2 3" xfId="167"/>
+    <cellStyle name="Normal 6 10 3" xfId="118"/>
+    <cellStyle name="Normal 6 10 4" xfId="117"/>
+    <cellStyle name="Normal 6 11" xfId="40"/>
+    <cellStyle name="Normal 6 11 2" xfId="251"/>
+    <cellStyle name="Normal 6 11 2 2" xfId="421"/>
+    <cellStyle name="Normal 6 11 2 3" xfId="422"/>
+    <cellStyle name="Normal 6 11 3" xfId="252"/>
+    <cellStyle name="Normal 6 11 4" xfId="250"/>
+    <cellStyle name="Normal 6 12" xfId="43"/>
+    <cellStyle name="Normal 6 12 2" xfId="227"/>
+    <cellStyle name="Normal 6 12 2 2" xfId="181"/>
+    <cellStyle name="Normal 6 12 2 3" xfId="180"/>
+    <cellStyle name="Normal 6 12 3" xfId="226"/>
+    <cellStyle name="Normal 6 12 4" xfId="225"/>
+    <cellStyle name="Normal 6 13" xfId="42"/>
+    <cellStyle name="Normal 6 13 2" xfId="16"/>
+    <cellStyle name="Normal 6 13 2 2" xfId="503"/>
+    <cellStyle name="Normal 6 13 2 3" xfId="504"/>
+    <cellStyle name="Normal 6 13 3" xfId="17"/>
+    <cellStyle name="Normal 6 13 4" xfId="11"/>
+    <cellStyle name="Normal 6 14" xfId="45"/>
+    <cellStyle name="Normal 6 14 2" xfId="337"/>
+    <cellStyle name="Normal 6 14 2 2" xfId="76"/>
+    <cellStyle name="Normal 6 14 2 3" xfId="75"/>
+    <cellStyle name="Normal 6 14 3" xfId="336"/>
+    <cellStyle name="Normal 6 14 4" xfId="338"/>
+    <cellStyle name="Normal 6 15" xfId="44"/>
+    <cellStyle name="Normal 6 15 2" xfId="130"/>
+    <cellStyle name="Normal 6 15 3" xfId="131"/>
+    <cellStyle name="Normal 6 16" xfId="47"/>
+    <cellStyle name="Normal 6 17" xfId="46"/>
+    <cellStyle name="Normal 6 2" xfId="315"/>
+    <cellStyle name="Normal 6 2 10" xfId="233"/>
+    <cellStyle name="Normal 6 2 11" xfId="232"/>
+    <cellStyle name="Normal 6 2 2" xfId="578"/>
+    <cellStyle name="Normal 6 2 2 10" xfId="528"/>
+    <cellStyle name="Normal 6 2 2 2" xfId="465"/>
+    <cellStyle name="Normal 6 2 2 2 2" xfId="485"/>
+    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8"/>
+    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220"/>
+    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436"/>
+    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260"/>
+    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508"/>
+    <cellStyle name="Normal 6 2 2 2 3" xfId="191"/>
+    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497"/>
+    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57"/>
+    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54"/>
+    <cellStyle name="Normal 6 2 2 2 4" xfId="178"/>
+    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71"/>
+    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384"/>
+    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389"/>
+    <cellStyle name="Normal 6 2 2 2 5" xfId="177"/>
+    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592"/>
+    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593"/>
+    <cellStyle name="Normal 6 2 2 2 6" xfId="483"/>
+    <cellStyle name="Normal 6 2 2 2 7" xfId="482"/>
+    <cellStyle name="Normal 6 2 2 3" xfId="464"/>
+    <cellStyle name="Normal 6 2 2 3 2" xfId="24"/>
+    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561"/>
+    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231"/>
+    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228"/>
+    <cellStyle name="Normal 6 2 2 3 3" xfId="25"/>
+    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132"/>
+    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30"/>
+    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27"/>
+    <cellStyle name="Normal 6 2 2 3 4" xfId="20"/>
+    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193"/>
+    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194"/>
+    <cellStyle name="Normal 6 2 2 3 5" xfId="21"/>
+    <cellStyle name="Normal 6 2 2 3 6" xfId="22"/>
+    <cellStyle name="Normal 6 2 2 4" xfId="467"/>
+    <cellStyle name="Normal 6 2 2 4 2" xfId="206"/>
+    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143"/>
+    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544"/>
+    <cellStyle name="Normal 6 2 2 4 3" xfId="205"/>
+    <cellStyle name="Normal 6 2 2 4 4" xfId="533"/>
+    <cellStyle name="Normal 6 2 2 5" xfId="466"/>
+    <cellStyle name="Normal 6 2 2 5 2" xfId="405"/>
+    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248"/>
+    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249"/>
+    <cellStyle name="Normal 6 2 2 5 3" xfId="406"/>
+    <cellStyle name="Normal 6 2 2 5 4" xfId="408"/>
+    <cellStyle name="Normal 6 2 2 6" xfId="469"/>
+    <cellStyle name="Normal 6 2 2 6 2" xfId="602"/>
+    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590"/>
+    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589"/>
+    <cellStyle name="Normal 6 2 2 6 3" xfId="601"/>
+    <cellStyle name="Normal 6 2 2 6 4" xfId="603"/>
+    <cellStyle name="Normal 6 2 2 7" xfId="468"/>
+    <cellStyle name="Normal 6 2 2 7 2" xfId="156"/>
+    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262"/>
+    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263"/>
+    <cellStyle name="Normal 6 2 2 7 3" xfId="157"/>
+    <cellStyle name="Normal 6 2 2 7 4" xfId="158"/>
+    <cellStyle name="Normal 6 2 2 8" xfId="101"/>
+    <cellStyle name="Normal 6 2 2 8 2" xfId="349"/>
+    <cellStyle name="Normal 6 2 2 8 3" xfId="348"/>
+    <cellStyle name="Normal 6 2 2 9" xfId="99"/>
+    <cellStyle name="Normal 6 2 3" xfId="577"/>
+    <cellStyle name="Normal 6 2 3 2" xfId="12"/>
+    <cellStyle name="Normal 6 2 3 2 2" xfId="294"/>
+    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527"/>
+    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361"/>
+    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355"/>
+    <cellStyle name="Normal 6 2 3 2 3" xfId="295"/>
+    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442"/>
+    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172"/>
+    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169"/>
+    <cellStyle name="Normal 6 2 3 2 4" xfId="289"/>
+    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213"/>
+    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214"/>
+    <cellStyle name="Normal 6 2 3 2 5" xfId="290"/>
+    <cellStyle name="Normal 6 2 3 2 6" xfId="291"/>
+    <cellStyle name="Normal 6 2 3 3" xfId="13"/>
+    <cellStyle name="Normal 6 2 3 3 2" xfId="84"/>
+    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543"/>
+    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542"/>
+    <cellStyle name="Normal 6 2 3 3 3" xfId="83"/>
+    <cellStyle name="Normal 6 2 3 3 4" xfId="82"/>
+    <cellStyle name="Normal 6 2 3 4" xfId="14"/>
+    <cellStyle name="Normal 6 2 3 4 2" xfId="216"/>
+    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660"/>
+    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661"/>
+    <cellStyle name="Normal 6 2 3 4 3" xfId="55"/>
+    <cellStyle name="Normal 6 2 3 4 4" xfId="223"/>
+    <cellStyle name="Normal 6 2 3 5" xfId="15"/>
+    <cellStyle name="Normal 6 2 3 5 2" xfId="506"/>
+    <cellStyle name="Normal 6 2 3 5 3" xfId="505"/>
+    <cellStyle name="Normal 6 2 3 6" xfId="69"/>
+    <cellStyle name="Normal 6 2 3 7" xfId="72"/>
+    <cellStyle name="Normal 6 2 4" xfId="331"/>
+    <cellStyle name="Normal 6 2 4 2" xfId="400"/>
+    <cellStyle name="Normal 6 2 4 2 2" xfId="256"/>
+    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274"/>
+    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270"/>
+    <cellStyle name="Normal 6 2 4 2 3" xfId="255"/>
+    <cellStyle name="Normal 6 2 4 2 4" xfId="257"/>
+    <cellStyle name="Normal 6 2 4 3" xfId="399"/>
+    <cellStyle name="Normal 6 2 4 3 2" xfId="458"/>
+    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150"/>
+    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151"/>
+    <cellStyle name="Normal 6 2 4 3 3" xfId="459"/>
+    <cellStyle name="Normal 6 2 4 3 4" xfId="463"/>
+    <cellStyle name="Normal 6 2 4 4" xfId="398"/>
+    <cellStyle name="Normal 6 2 4 4 2" xfId="522"/>
+    <cellStyle name="Normal 6 2 4 4 3" xfId="521"/>
+    <cellStyle name="Normal 6 2 4 5" xfId="397"/>
+    <cellStyle name="Normal 6 2 4 6" xfId="396"/>
+    <cellStyle name="Normal 6 2 5" xfId="330"/>
+    <cellStyle name="Normal 6 2 5 2" xfId="569"/>
+    <cellStyle name="Normal 6 2 5 2 2" xfId="376"/>
+    <cellStyle name="Normal 6 2 5 2 3" xfId="377"/>
+    <cellStyle name="Normal 6 2 5 3" xfId="570"/>
+    <cellStyle name="Normal 6 2 5 4" xfId="568"/>
+    <cellStyle name="Normal 6 2 6" xfId="333"/>
+    <cellStyle name="Normal 6 2 6 2" xfId="632"/>
+    <cellStyle name="Normal 6 2 6 2 2" xfId="175"/>
+    <cellStyle name="Normal 6 2 6 2 3" xfId="174"/>
+    <cellStyle name="Normal 6 2 6 3" xfId="631"/>
+    <cellStyle name="Normal 6 2 6 4" xfId="630"/>
+    <cellStyle name="Normal 6 2 7" xfId="332"/>
+    <cellStyle name="Normal 6 2 7 2" xfId="195"/>
+    <cellStyle name="Normal 6 2 7 2 2" xfId="635"/>
+    <cellStyle name="Normal 6 2 7 2 3" xfId="636"/>
+    <cellStyle name="Normal 6 2 7 3" xfId="196"/>
+    <cellStyle name="Normal 6 2 7 4" xfId="427"/>
+    <cellStyle name="Normal 6 2 8" xfId="335"/>
+    <cellStyle name="Normal 6 2 8 2" xfId="474"/>
+    <cellStyle name="Normal 6 2 8 2 2" xfId="524"/>
+    <cellStyle name="Normal 6 2 8 2 3" xfId="523"/>
+    <cellStyle name="Normal 6 2 8 3" xfId="473"/>
+    <cellStyle name="Normal 6 2 8 4" xfId="479"/>
+    <cellStyle name="Normal 6 2 9" xfId="334"/>
+    <cellStyle name="Normal 6 2 9 2" xfId="26"/>
+    <cellStyle name="Normal 6 2 9 3" xfId="98"/>
+    <cellStyle name="Normal 6 3" xfId="314"/>
+    <cellStyle name="Normal 6 3 10" xfId="183"/>
+    <cellStyle name="Normal 6 3 2" xfId="548"/>
+    <cellStyle name="Normal 6 3 2 2" xfId="207"/>
+    <cellStyle name="Normal 6 3 2 2 2" xfId="237"/>
+    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90"/>
+    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51"/>
+    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48"/>
+    <cellStyle name="Normal 6 3 2 2 3" xfId="238"/>
+    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287"/>
+    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498"/>
+    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495"/>
+    <cellStyle name="Normal 6 3 2 2 4" xfId="234"/>
+    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612"/>
+    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613"/>
+    <cellStyle name="Normal 6 3 2 2 5" xfId="235"/>
+    <cellStyle name="Normal 6 3 2 2 6" xfId="236"/>
+    <cellStyle name="Normal 6 3 2 3" xfId="208"/>
+    <cellStyle name="Normal 6 3 2 3 2" xfId="37"/>
+    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394"/>
+    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393"/>
+    <cellStyle name="Normal 6 3 2 3 3" xfId="36"/>
+    <cellStyle name="Normal 6 3 2 3 4" xfId="35"/>
+    <cellStyle name="Normal 6 3 2 4" xfId="209"/>
+    <cellStyle name="Normal 6 3 2 4 2" xfId="627"/>
+    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486"/>
+    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487"/>
+    <cellStyle name="Normal 6 3 2 4 3" xfId="628"/>
+    <cellStyle name="Normal 6 3 2 4 4" xfId="629"/>
+    <cellStyle name="Normal 6 3 2 5" xfId="210"/>
+    <cellStyle name="Normal 6 3 2 5 2" xfId="431"/>
+    <cellStyle name="Normal 6 3 2 5 3" xfId="430"/>
+    <cellStyle name="Normal 6 3 2 6" xfId="211"/>
+    <cellStyle name="Normal 6 3 2 7" xfId="212"/>
+    <cellStyle name="Normal 6 3 3" xfId="549"/>
+    <cellStyle name="Normal 6 3 3 2" xfId="645"/>
+    <cellStyle name="Normal 6 3 3 2 2" xfId="558"/>
+    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190"/>
+    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189"/>
+    <cellStyle name="Normal 6 3 3 2 3" xfId="557"/>
+    <cellStyle name="Normal 6 3 3 2 4" xfId="556"/>
+    <cellStyle name="Normal 6 3 3 3" xfId="644"/>
+    <cellStyle name="Normal 6 3 3 3 2" xfId="114"/>
+    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653"/>
+    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654"/>
+    <cellStyle name="Normal 6 3 3 3 3" xfId="115"/>
+    <cellStyle name="Normal 6 3 3 3 4" xfId="112"/>
+    <cellStyle name="Normal 6 3 3 4" xfId="647"/>
+    <cellStyle name="Normal 6 3 3 4 2" xfId="317"/>
+    <cellStyle name="Normal 6 3 3 4 3" xfId="316"/>
+    <cellStyle name="Normal 6 3 3 5" xfId="646"/>
+    <cellStyle name="Normal 6 3 3 6" xfId="648"/>
+    <cellStyle name="Normal 6 3 4" xfId="550"/>
+    <cellStyle name="Normal 6 3 4 2" xfId="160"/>
+    <cellStyle name="Normal 6 3 4 2 2" xfId="470"/>
+    <cellStyle name="Normal 6 3 4 2 3" xfId="471"/>
+    <cellStyle name="Normal 6 3 4 3" xfId="164"/>
+    <cellStyle name="Normal 6 3 4 4" xfId="155"/>
+    <cellStyle name="Normal 6 3 5" xfId="551"/>
+    <cellStyle name="Normal 6 3 5 2" xfId="493"/>
+    <cellStyle name="Normal 6 3 5 2 2" xfId="53"/>
+    <cellStyle name="Normal 6 3 5 2 3" xfId="52"/>
+    <cellStyle name="Normal 6 3 5 3" xfId="492"/>
+    <cellStyle name="Normal 6 3 5 4" xfId="491"/>
+    <cellStyle name="Normal 6 3 6" xfId="552"/>
+    <cellStyle name="Normal 6 3 6 2" xfId="323"/>
+    <cellStyle name="Normal 6 3 6 2 2" xfId="153"/>
+    <cellStyle name="Normal 6 3 6 2 3" xfId="154"/>
+    <cellStyle name="Normal 6 3 6 3" xfId="324"/>
+    <cellStyle name="Normal 6 3 6 4" xfId="322"/>
+    <cellStyle name="Normal 6 3 7" xfId="553"/>
+    <cellStyle name="Normal 6 3 7 2" xfId="111"/>
+    <cellStyle name="Normal 6 3 7 2 2" xfId="347"/>
+    <cellStyle name="Normal 6 3 7 2 3" xfId="346"/>
+    <cellStyle name="Normal 6 3 7 3" xfId="110"/>
+    <cellStyle name="Normal 6 3 7 4" xfId="109"/>
+    <cellStyle name="Normal 6 3 8" xfId="501"/>
+    <cellStyle name="Normal 6 3 8 2" xfId="305"/>
+    <cellStyle name="Normal 6 3 8 3" xfId="306"/>
+    <cellStyle name="Normal 6 3 9" xfId="502"/>
+    <cellStyle name="Normal 6 4" xfId="311"/>
+    <cellStyle name="Normal 6 4 10" xfId="100"/>
+    <cellStyle name="Normal 6 4 2" xfId="92"/>
+    <cellStyle name="Normal 6 4 2 2" xfId="140"/>
+    <cellStyle name="Normal 6 4 2 2 2" xfId="375"/>
+    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381"/>
+    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266"/>
+    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268"/>
+    <cellStyle name="Normal 6 4 2 2 3" xfId="395"/>
+    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188"/>
+    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481"/>
+    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484"/>
+    <cellStyle name="Normal 6 4 2 2 4" xfId="402"/>
+    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429"/>
+    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428"/>
+    <cellStyle name="Normal 6 4 2 2 5" xfId="401"/>
+    <cellStyle name="Normal 6 4 2 2 6" xfId="379"/>
+    <cellStyle name="Normal 6 4 2 3" xfId="139"/>
+    <cellStyle name="Normal 6 4 2 3 2" xfId="587"/>
+    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655"/>
+    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656"/>
+    <cellStyle name="Normal 6 4 2 3 3" xfId="588"/>
+    <cellStyle name="Normal 6 4 2 3 4" xfId="591"/>
+    <cellStyle name="Normal 6 4 2 4" xfId="138"/>
+    <cellStyle name="Normal 6 4 2 4 2" xfId="623"/>
+    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605"/>
+    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604"/>
+    <cellStyle name="Normal 6 4 2 4 3" xfId="622"/>
+    <cellStyle name="Normal 6 4 2 4 4" xfId="621"/>
+    <cellStyle name="Normal 6 4 2 5" xfId="137"/>
+    <cellStyle name="Normal 6 4 2 5 2" xfId="184"/>
+    <cellStyle name="Normal 6 4 2 5 3" xfId="185"/>
+    <cellStyle name="Normal 6 4 2 6" xfId="136"/>
+    <cellStyle name="Normal 6 4 2 7" xfId="135"/>
+    <cellStyle name="Normal 6 4 3" xfId="91"/>
+    <cellStyle name="Normal 6 4 3 2" xfId="342"/>
+    <cellStyle name="Normal 6 4 3 2 2" xfId="200"/>
+    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127"/>
+    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128"/>
+    <cellStyle name="Normal 6 4 3 2 3" xfId="201"/>
+    <cellStyle name="Normal 6 4 3 2 4" xfId="204"/>
+    <cellStyle name="Normal 6 4 3 3" xfId="343"/>
+    <cellStyle name="Normal 6 4 3 3 2" xfId="643"/>
+    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298"/>
+    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297"/>
+    <cellStyle name="Normal 6 4 3 3 3" xfId="642"/>
+    <cellStyle name="Normal 6 4 3 3 4" xfId="583"/>
+    <cellStyle name="Normal 6 4 3 4" xfId="340"/>
+    <cellStyle name="Normal 6 4 3 4 2" xfId="444"/>
+    <cellStyle name="Normal 6 4 3 4 3" xfId="445"/>
+    <cellStyle name="Normal 6 4 3 5" xfId="341"/>
+    <cellStyle name="Normal 6 4 3 6" xfId="339"/>
+    <cellStyle name="Normal 6 4 4" xfId="441"/>
+    <cellStyle name="Normal 6 4 4 2" xfId="292"/>
+    <cellStyle name="Normal 6 4 4 2 2" xfId="247"/>
+    <cellStyle name="Normal 6 4 4 2 3" xfId="246"/>
+    <cellStyle name="Normal 6 4 4 3" xfId="412"/>
+    <cellStyle name="Normal 6 4 4 4" xfId="293"/>
+    <cellStyle name="Normal 6 4 5" xfId="440"/>
+    <cellStyle name="Normal 6 4 5 2" xfId="460"/>
+    <cellStyle name="Normal 6 4 5 2 2" xfId="517"/>
+    <cellStyle name="Normal 6 4 5 2 3" xfId="520"/>
+    <cellStyle name="Normal 6 4 5 3" xfId="461"/>
+    <cellStyle name="Normal 6 4 5 4" xfId="462"/>
+    <cellStyle name="Normal 6 4 6" xfId="88"/>
+    <cellStyle name="Normal 6 4 6 2" xfId="5"/>
+    <cellStyle name="Normal 6 4 6 2 2" xfId="595"/>
+    <cellStyle name="Normal 6 4 6 2 3" xfId="594"/>
+    <cellStyle name="Normal 6 4 6 3" xfId="4"/>
+    <cellStyle name="Normal 6 4 6 4" xfId="10"/>
+    <cellStyle name="Normal 6 4 7" xfId="87"/>
+    <cellStyle name="Normal 6 4 7 2" xfId="221"/>
+    <cellStyle name="Normal 6 4 7 2 2" xfId="403"/>
+    <cellStyle name="Normal 6 4 7 2 3" xfId="404"/>
+    <cellStyle name="Normal 6 4 7 3" xfId="222"/>
+    <cellStyle name="Normal 6 4 7 4" xfId="224"/>
+    <cellStyle name="Normal 6 4 8" xfId="97"/>
+    <cellStyle name="Normal 6 4 8 2" xfId="95"/>
+    <cellStyle name="Normal 6 4 8 3" xfId="380"/>
+    <cellStyle name="Normal 6 4 9" xfId="96"/>
+    <cellStyle name="Normal 6 5" xfId="310"/>
+    <cellStyle name="Normal 6 5 2" xfId="285"/>
+    <cellStyle name="Normal 6 5 2 2" xfId="534"/>
+    <cellStyle name="Normal 6 5 2 2 2" xfId="182"/>
+    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547"/>
+    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259"/>
+    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261"/>
+    <cellStyle name="Normal 6 5 2 2 3" xfId="417"/>
+    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106"/>
+    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301"/>
+    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79"/>
+    <cellStyle name="Normal 6 5 2 2 4" xfId="253"/>
+    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419"/>
+    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420"/>
+    <cellStyle name="Normal 6 5 2 2 5" xfId="254"/>
+    <cellStyle name="Normal 6 5 2 2 6" xfId="192"/>
+    <cellStyle name="Normal 6 5 2 3" xfId="535"/>
+    <cellStyle name="Normal 6 5 2 3 2" xfId="649"/>
+    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370"/>
+    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369"/>
+    <cellStyle name="Normal 6 5 2 3 3" xfId="70"/>
+    <cellStyle name="Normal 6 5 2 3 4" xfId="276"/>
+    <cellStyle name="Normal 6 5 2 4" xfId="532"/>
+    <cellStyle name="Normal 6 5 2 4 2" xfId="518"/>
+    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633"/>
+    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634"/>
+    <cellStyle name="Normal 6 5 2 4 3" xfId="519"/>
+    <cellStyle name="Normal 6 5 2 4 4" xfId="514"/>
+    <cellStyle name="Normal 6 5 2 5" xfId="447"/>
+    <cellStyle name="Normal 6 5 2 5 2" xfId="304"/>
+    <cellStyle name="Normal 6 5 2 5 3" xfId="303"/>
+    <cellStyle name="Normal 6 5 2 6" xfId="530"/>
+    <cellStyle name="Normal 6 5 2 7" xfId="531"/>
+    <cellStyle name="Normal 6 5 3" xfId="286"/>
+    <cellStyle name="Normal 6 5 3 2" xfId="321"/>
+    <cellStyle name="Normal 6 5 3 2 2" xfId="134"/>
+    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600"/>
+    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599"/>
+    <cellStyle name="Normal 6 5 3 2 3" xfId="229"/>
+    <cellStyle name="Normal 6 5 3 2 4" xfId="472"/>
+    <cellStyle name="Normal 6 5 3 3" xfId="320"/>
+    <cellStyle name="Normal 6 5 3 3 2" xfId="32"/>
+    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423"/>
+    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424"/>
+    <cellStyle name="Normal 6 5 3 3 3" xfId="34"/>
+    <cellStyle name="Normal 6 5 3 3 4" xfId="9"/>
+    <cellStyle name="Normal 6 5 3 4" xfId="319"/>
+    <cellStyle name="Normal 6 5 3 4 2" xfId="94"/>
+    <cellStyle name="Normal 6 5 3 4 3" xfId="93"/>
+    <cellStyle name="Normal 6 5 3 5" xfId="318"/>
+    <cellStyle name="Normal 6 5 3 6" xfId="525"/>
+    <cellStyle name="Normal 6 5 4" xfId="283"/>
+    <cellStyle name="Normal 6 5 4 2" xfId="582"/>
+    <cellStyle name="Normal 6 5 4 2 2" xfId="478"/>
+    <cellStyle name="Normal 6 5 4 2 3" xfId="639"/>
+    <cellStyle name="Normal 6 5 4 3" xfId="197"/>
+    <cellStyle name="Normal 6 5 4 4" xfId="584"/>
+    <cellStyle name="Normal 6 5 5" xfId="284"/>
+    <cellStyle name="Normal 6 5 5 2" xfId="387"/>
+    <cellStyle name="Normal 6 5 5 2 2" xfId="119"/>
+    <cellStyle name="Normal 6 5 5 2 3" xfId="33"/>
+    <cellStyle name="Normal 6 5 5 3" xfId="386"/>
+    <cellStyle name="Normal 6 5 5 4" xfId="388"/>
+    <cellStyle name="Normal 6 5 6" xfId="281"/>
+    <cellStyle name="Normal 6 5 6 2" xfId="74"/>
+    <cellStyle name="Normal 6 5 6 3" xfId="356"/>
+    <cellStyle name="Normal 6 5 7" xfId="282"/>
+    <cellStyle name="Normal 6 5 8" xfId="280"/>
+    <cellStyle name="Normal 6 6" xfId="313"/>
+    <cellStyle name="Normal 6 6 2" xfId="326"/>
+    <cellStyle name="Normal 6 6 2 2" xfId="245"/>
+    <cellStyle name="Normal 6 6 2 2 2" xfId="64"/>
+    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515"/>
+    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617"/>
+    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619"/>
+    <cellStyle name="Normal 6 6 2 2 3" xfId="113"/>
+    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457"/>
+    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296"/>
+    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176"/>
+    <cellStyle name="Normal 6 6 2 2 4" xfId="80"/>
+    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199"/>
+    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198"/>
+    <cellStyle name="Normal 6 6 2 2 5" xfId="77"/>
+    <cellStyle name="Normal 6 6 2 2 6" xfId="129"/>
+    <cellStyle name="Normal 6 6 2 3" xfId="163"/>
+    <cellStyle name="Normal 6 6 2 3 2" xfId="662"/>
+    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278"/>
+    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279"/>
+    <cellStyle name="Normal 6 6 2 3 3" xfId="1"/>
+    <cellStyle name="Normal 6 6 2 3 4" xfId="2"/>
+    <cellStyle name="Normal 6 6 2 4" xfId="586"/>
+    <cellStyle name="Normal 6 6 2 4 2" xfId="581"/>
+    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383"/>
+    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516"/>
+    <cellStyle name="Normal 6 6 2 4 3" xfId="580"/>
+    <cellStyle name="Normal 6 6 2 4 4" xfId="579"/>
+    <cellStyle name="Normal 6 6 2 5" xfId="159"/>
+    <cellStyle name="Normal 6 6 2 5 2" xfId="141"/>
+    <cellStyle name="Normal 6 6 2 5 3" xfId="142"/>
+    <cellStyle name="Normal 6 6 2 6" xfId="162"/>
+    <cellStyle name="Normal 6 6 2 7" xfId="161"/>
+    <cellStyle name="Normal 6 6 3" xfId="325"/>
+    <cellStyle name="Normal 6 6 3 2" xfId="374"/>
+    <cellStyle name="Normal 6 6 3 2 2" xfId="275"/>
+    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410"/>
+    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411"/>
+    <cellStyle name="Normal 6 6 3 2 3" xfId="362"/>
+    <cellStyle name="Normal 6 6 3 2 4" xfId="277"/>
+    <cellStyle name="Normal 6 6 3 3" xfId="186"/>
+    <cellStyle name="Normal 6 6 3 3 2" xfId="105"/>
+    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300"/>
+    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299"/>
+    <cellStyle name="Normal 6 6 3 3 3" xfId="104"/>
+    <cellStyle name="Normal 6 6 3 3 4" xfId="574"/>
+    <cellStyle name="Normal 6 6 3 4" xfId="371"/>
+    <cellStyle name="Normal 6 6 3 4 2" xfId="391"/>
+    <cellStyle name="Normal 6 6 3 4 3" xfId="392"/>
+    <cellStyle name="Normal 6 6 3 5" xfId="372"/>
+    <cellStyle name="Normal 6 6 3 6" xfId="373"/>
+    <cellStyle name="Normal 6 6 4" xfId="108"/>
+    <cellStyle name="Normal 6 6 4 2" xfId="435"/>
+    <cellStyle name="Normal 6 6 4 2 2" xfId="433"/>
+    <cellStyle name="Normal 6 6 4 2 3" xfId="432"/>
+    <cellStyle name="Normal 6 6 4 3" xfId="434"/>
+    <cellStyle name="Normal 6 6 4 4" xfId="438"/>
+    <cellStyle name="Normal 6 6 5" xfId="585"/>
+    <cellStyle name="Normal 6 6 5 2" xfId="596"/>
+    <cellStyle name="Normal 6 6 5 2 2" xfId="554"/>
+    <cellStyle name="Normal 6 6 5 2 3" xfId="555"/>
+    <cellStyle name="Normal 6 6 5 3" xfId="597"/>
+    <cellStyle name="Normal 6 6 5 4" xfId="598"/>
+    <cellStyle name="Normal 6 6 6" xfId="616"/>
+    <cellStyle name="Normal 6 6 6 2" xfId="29"/>
+    <cellStyle name="Normal 6 6 6 3" xfId="28"/>
+    <cellStyle name="Normal 6 6 7" xfId="507"/>
+    <cellStyle name="Normal 6 6 8" xfId="513"/>
+    <cellStyle name="Normal 6 7" xfId="312"/>
+    <cellStyle name="Normal 6 7 2" xfId="65"/>
+    <cellStyle name="Normal 6 7 2 2" xfId="610"/>
+    <cellStyle name="Normal 6 7 2 2 2" xfId="122"/>
+    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244"/>
+    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120"/>
+    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562"/>
+    <cellStyle name="Normal 6 7 2 2 3" xfId="123"/>
+    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144"/>
+    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357"/>
+    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359"/>
+    <cellStyle name="Normal 6 7 2 2 4" xfId="124"/>
+    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170"/>
+    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171"/>
+    <cellStyle name="Normal 6 7 2 2 5" xfId="125"/>
+    <cellStyle name="Normal 6 7 2 2 6" xfId="126"/>
+    <cellStyle name="Normal 6 7 2 3" xfId="611"/>
+    <cellStyle name="Normal 6 7 2 3 2" xfId="572"/>
+    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49"/>
+    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327"/>
+    <cellStyle name="Normal 6 7 2 3 3" xfId="571"/>
+    <cellStyle name="Normal 6 7 2 3 4" xfId="573"/>
+    <cellStyle name="Normal 6 7 2 4" xfId="606"/>
+    <cellStyle name="Normal 6 7 2 4 2" xfId="272"/>
+    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179"/>
+    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536"/>
+    <cellStyle name="Normal 6 7 2 4 3" xfId="273"/>
+    <cellStyle name="Normal 6 7 2 4 4" xfId="271"/>
+    <cellStyle name="Normal 6 7 2 5" xfId="607"/>
+    <cellStyle name="Normal 6 7 2 5 2" xfId="86"/>
+    <cellStyle name="Normal 6 7 2 5 3" xfId="85"/>
+    <cellStyle name="Normal 6 7 2 6" xfId="608"/>
+    <cellStyle name="Normal 6 7 2 7" xfId="609"/>
+    <cellStyle name="Normal 6 7 3" xfId="66"/>
+    <cellStyle name="Normal 6 7 3 2" xfId="409"/>
+    <cellStyle name="Normal 6 7 3 2 2" xfId="476"/>
+    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353"/>
+    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352"/>
+    <cellStyle name="Normal 6 7 3 2 3" xfId="475"/>
+    <cellStyle name="Normal 6 7 3 2 4" xfId="477"/>
+    <cellStyle name="Normal 6 7 3 3" xfId="418"/>
+    <cellStyle name="Normal 6 7 3 3 2" xfId="650"/>
+    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19"/>
+    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23"/>
+    <cellStyle name="Normal 6 7 3 3 3" xfId="651"/>
+    <cellStyle name="Normal 6 7 3 3 4" xfId="652"/>
+    <cellStyle name="Normal 6 7 3 4" xfId="414"/>
+    <cellStyle name="Normal 6 7 3 4 2" xfId="563"/>
+    <cellStyle name="Normal 6 7 3 4 3" xfId="620"/>
+    <cellStyle name="Normal 6 7 3 5" xfId="413"/>
+    <cellStyle name="Normal 6 7 3 6" xfId="407"/>
+    <cellStyle name="Normal 6 7 4" xfId="60"/>
+    <cellStyle name="Normal 6 7 4 2" xfId="166"/>
+    <cellStyle name="Normal 6 7 4 2 2" xfId="509"/>
+    <cellStyle name="Normal 6 7 4 2 3" xfId="510"/>
+    <cellStyle name="Normal 6 7 4 3" xfId="490"/>
+    <cellStyle name="Normal 6 7 4 4" xfId="494"/>
+    <cellStyle name="Normal 6 7 5" xfId="61"/>
+    <cellStyle name="Normal 6 7 5 2" xfId="638"/>
+    <cellStyle name="Normal 6 7 5 2 2" xfId="152"/>
+    <cellStyle name="Normal 6 7 5 2 3" xfId="38"/>
+    <cellStyle name="Normal 6 7 5 3" xfId="637"/>
+    <cellStyle name="Normal 6 7 5 4" xfId="641"/>
+    <cellStyle name="Normal 6 7 6" xfId="62"/>
+    <cellStyle name="Normal 6 7 6 2" xfId="415"/>
+    <cellStyle name="Normal 6 7 6 3" xfId="416"/>
+    <cellStyle name="Normal 6 7 7" xfId="63"/>
+    <cellStyle name="Normal 6 7 8" xfId="59"/>
+    <cellStyle name="Normal 6 8" xfId="308"/>
+    <cellStyle name="Normal 6 8 2" xfId="364"/>
+    <cellStyle name="Normal 6 8 2 2" xfId="146"/>
+    <cellStyle name="Normal 6 8 2 2 2" xfId="3"/>
+    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345"/>
+    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344"/>
+    <cellStyle name="Normal 6 8 2 2 3" xfId="18"/>
+    <cellStyle name="Normal 6 8 2 2 4" xfId="575"/>
+    <cellStyle name="Normal 6 8 2 3" xfId="145"/>
+    <cellStyle name="Normal 6 8 2 3 2" xfId="240"/>
+    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202"/>
+    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203"/>
+    <cellStyle name="Normal 6 8 2 3 3" xfId="241"/>
+    <cellStyle name="Normal 6 8 2 3 4" xfId="239"/>
+    <cellStyle name="Normal 6 8 2 4" xfId="149"/>
+    <cellStyle name="Normal 6 8 2 4 2" xfId="625"/>
+    <cellStyle name="Normal 6 8 2 4 3" xfId="624"/>
+    <cellStyle name="Normal 6 8 2 5" xfId="148"/>
+    <cellStyle name="Normal 6 8 2 6" xfId="147"/>
+    <cellStyle name="Normal 6 8 3" xfId="363"/>
+    <cellStyle name="Normal 6 8 3 2" xfId="350"/>
+    <cellStyle name="Normal 6 8 3 2 2" xfId="488"/>
+    <cellStyle name="Normal 6 8 3 2 3" xfId="489"/>
+    <cellStyle name="Normal 6 8 3 3" xfId="351"/>
+    <cellStyle name="Normal 6 8 3 4" xfId="354"/>
+    <cellStyle name="Normal 6 8 4" xfId="368"/>
+    <cellStyle name="Normal 6 8 4 2" xfId="565"/>
+    <cellStyle name="Normal 6 8 4 2 2" xfId="165"/>
+    <cellStyle name="Normal 6 8 4 2 3" xfId="446"/>
+    <cellStyle name="Normal 6 8 4 3" xfId="564"/>
+    <cellStyle name="Normal 6 8 4 4" xfId="559"/>
+    <cellStyle name="Normal 6 8 5" xfId="367"/>
+    <cellStyle name="Normal 6 8 5 2" xfId="102"/>
+    <cellStyle name="Normal 6 8 5 3" xfId="103"/>
+    <cellStyle name="Normal 6 8 6" xfId="366"/>
+    <cellStyle name="Normal 6 8 7" xfId="365"/>
+    <cellStyle name="Normal 6 9" xfId="307"/>
+    <cellStyle name="Normal 6 9 2" xfId="537"/>
+    <cellStyle name="Normal 6 9 2 2" xfId="215"/>
+    <cellStyle name="Normal 6 9 2 2 2" xfId="264"/>
+    <cellStyle name="Normal 6 9 2 2 3" xfId="265"/>
+    <cellStyle name="Normal 6 9 2 3" xfId="566"/>
+    <cellStyle name="Normal 6 9 2 4" xfId="217"/>
+    <cellStyle name="Normal 6 9 3" xfId="538"/>
+    <cellStyle name="Normal 6 9 3 2" xfId="658"/>
+    <cellStyle name="Normal 6 9 3 2 2" xfId="426"/>
+    <cellStyle name="Normal 6 9 3 2 3" xfId="425"/>
+    <cellStyle name="Normal 6 9 3 3" xfId="657"/>
+    <cellStyle name="Normal 6 9 3 4" xfId="659"/>
+    <cellStyle name="Normal 6 9 4" xfId="540"/>
+    <cellStyle name="Normal 6 9 4 2" xfId="640"/>
+    <cellStyle name="Normal 6 9 4 3" xfId="567"/>
+    <cellStyle name="Normal 6 9 5" xfId="541"/>
+    <cellStyle name="Normal 6 9 6" xfId="539"/>
+    <cellStyle name="Normal 7" xfId="452"/>
+    <cellStyle name="Normal 7 2" xfId="529"/>
+    <cellStyle name="Normal 8" xfId="455"/>
+    <cellStyle name="Normal 8 2" xfId="576"/>
+    <cellStyle name="Normal 9" xfId="454"/>
+    <cellStyle name="Normal 9 2" xfId="58"/>
+    <cellStyle name="Percent 2" xfId="269"/>
+    <cellStyle name="Percent 2 2" xfId="78"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1746,23 +1745,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1798,23 +1780,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1990,25 +1955,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="6" customWidth="1"/>
-    <col min="3" max="8" width="9.109375" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="51.54296875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="6" customWidth="1"/>
+    <col min="3" max="8" width="9.08984375" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.08984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2016,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
@@ -2024,7 +1989,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
@@ -2032,7 +1997,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
@@ -2040,7 +2005,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -2048,7 +2013,7 @@
         <v>220000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -2056,7 +2021,7 @@
         <v>807610</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -2066,9 +2031,11 @@
       <c r="C7">
         <v>15</v>
       </c>
-      <c r="D7"/>
+      <c r="D7">
+        <v>25</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
@@ -2078,19 +2045,19 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{FAA95EF1-203A-4444-9E84-DB4F2FBB8CD8}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B4">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B5:B6" xr:uid="{0FC7A138-FA33-4811-8FA6-C94730F85756}">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B5:B6">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{3E598E5F-6CB6-4BE4-88E7-3E3DC2A25D2F}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B3">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{1E31B6DE-8F0F-4067-A47F-00EDE838D564}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
@@ -2101,7 +2068,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -2114,25 +2081,25 @@
       <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="56" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="23" customWidth="1"/>
     <col min="4" max="4" width="11" style="24" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="24" customWidth="1"/>
-    <col min="6" max="7" width="7.44140625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="7.36328125" style="24" customWidth="1"/>
+    <col min="6" max="7" width="7.453125" style="24" customWidth="1"/>
     <col min="8" max="11" width="7" style="24" customWidth="1"/>
-    <col min="12" max="13" width="7.44140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7.88671875" style="24" customWidth="1"/>
-    <col min="16" max="16" width="10.77734375" style="24" customWidth="1"/>
+    <col min="12" max="13" width="7.453125" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="7.90625" style="24" customWidth="1"/>
+    <col min="16" max="16" width="10.81640625" style="24" customWidth="1"/>
     <col min="17" max="18" width="10" style="24" customWidth="1"/>
-    <col min="19" max="19" width="10.21875" style="24" customWidth="1"/>
-    <col min="20" max="20" width="9.109375" style="24" customWidth="1"/>
-    <col min="21" max="16384" width="9.109375" style="24"/>
+    <col min="19" max="19" width="10.1796875" style="24" customWidth="1"/>
+    <col min="20" max="20" width="9.08984375" style="24" customWidth="1"/>
+    <col min="21" max="16384" width="9.08984375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
@@ -2191,7 +2158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
@@ -2213,7 +2180,7 @@
       <c r="U2" s="21"/>
       <c r="V2" s="21"/>
     </row>
-    <row r="3" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2231,7 +2198,7 @@
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
     </row>
-    <row r="4" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>25</v>
       </c>
@@ -2242,7 +2209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>20</v>
       </c>
@@ -2257,7 +2224,7 @@
       <c r="U5" s="21"/>
       <c r="V5" s="21"/>
     </row>
-    <row r="6" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>26</v>
       </c>
@@ -2275,23 +2242,23 @@
       <c r="U6" s="21"/>
       <c r="V6" s="21"/>
     </row>
-    <row r="7" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E2:O2 Q2:Q3 Q5:Q6" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E2:O2 Q2:Q3 Q5:Q6">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E3:Q3 E5:Q6" xr:uid="{402091F8-A3FA-4E40-8099-07B402378B02}">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1"/>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E3:Q3 E5:Q6">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2302,7 +2269,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
@@ -2312,9 +2279,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2328,7 +2295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2339,7 +2306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Ageing flows for diabetes, prison and non risk groups, not generalised for all risk group
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15340" windowHeight="5500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -1962,18 +1962,18 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.54296875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" style="6" customWidth="1"/>
-    <col min="3" max="8" width="9.08984375" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.08984375" style="3"/>
+    <col min="1" max="1" width="51.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="6" customWidth="1"/>
+    <col min="3" max="8" width="9.140625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1981,15 +1981,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="8">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>220000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>807610</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
@@ -2078,28 +2078,27 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="23" customWidth="1"/>
     <col min="4" max="4" width="11" style="24" customWidth="1"/>
-    <col min="5" max="5" width="7.36328125" style="24" customWidth="1"/>
-    <col min="6" max="7" width="7.453125" style="24" customWidth="1"/>
+    <col min="5" max="7" width="7.42578125" style="24" customWidth="1"/>
     <col min="8" max="11" width="7" style="24" customWidth="1"/>
-    <col min="12" max="13" width="7.453125" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7.90625" style="24" customWidth="1"/>
-    <col min="16" max="16" width="10.81640625" style="24" customWidth="1"/>
+    <col min="12" max="13" width="7.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="7.85546875" style="24" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="24" customWidth="1"/>
     <col min="17" max="18" width="10" style="24" customWidth="1"/>
-    <col min="19" max="19" width="10.1796875" style="24" customWidth="1"/>
-    <col min="20" max="20" width="9.08984375" style="24" customWidth="1"/>
-    <col min="21" max="16384" width="9.08984375" style="24"/>
+    <col min="19" max="19" width="10.140625" style="24" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="24" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
@@ -2158,7 +2157,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
@@ -2180,7 +2179,7 @@
       <c r="U2" s="21"/>
       <c r="V2" s="21"/>
     </row>
-    <row r="3" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2198,7 +2197,7 @@
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
     </row>
-    <row r="4" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>25</v>
       </c>
@@ -2209,7 +2208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>20</v>
       </c>
@@ -2224,7 +2223,7 @@
       <c r="U5" s="21"/>
       <c r="V5" s="21"/>
     </row>
-    <row r="6" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>26</v>
       </c>
@@ -2242,7 +2241,7 @@
       <c r="U6" s="21"/>
       <c r="V6" s="21"/>
     </row>
-    <row r="7" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -2279,9 +2278,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2295,7 +2294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Implement dorms for Bhutan application and prepare first model calibration
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -1,27 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20339"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swas0001\swas_AuTuMN\autumn\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\swasnik_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AF9288-F1B4-49A3-9DE4-C511DEDF0EB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Romain Ragonnet</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{49EF9DA3-CAA8-4233-BE26-54D012EF67E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Romain Ragonnet:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Riskgroup prevalence is hard-coded at the moment. Line 309 of base.py (prop_ageing_dorm = 0.105 )</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>parameter</t>
   </si>
@@ -83,9 +118,6 @@
     <t>plot_start_time</t>
   </si>
   <si>
-    <t>program_perc_treatment_new_success</t>
-  </si>
-  <si>
     <t>scenario_1</t>
   </si>
   <si>
@@ -98,17 +130,32 @@
     <t>scenario_4</t>
   </si>
   <si>
+    <t>current_time</t>
+  </si>
+  <si>
+    <t>scenario_start_time</t>
+  </si>
+  <si>
+    <t>scenario_full_time</t>
+  </si>
+  <si>
+    <t>riskgroup_perc_dorm</t>
+  </si>
+  <si>
     <t>program_perc_detect</t>
   </si>
   <si>
     <t>program_perc_nonsuccess_new_death</t>
+  </si>
+  <si>
+    <t>int_perc_ipt_age5to15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +235,27 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -955,7 +1023,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="661" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -987,674 +1055,675 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="661" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="662" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="662" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="662" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="662" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="663">
-    <cellStyle name="Comma 2" xfId="614"/>
-    <cellStyle name="Comma 2 2" xfId="626"/>
-    <cellStyle name="Input 2" xfId="378"/>
+    <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 2 2" xfId="626" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Input 2" xfId="378" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="545"/>
-    <cellStyle name="Normal 2" xfId="449"/>
-    <cellStyle name="Normal 2 2" xfId="439"/>
-    <cellStyle name="Normal 3" xfId="448"/>
-    <cellStyle name="Normal 3 2" xfId="500"/>
-    <cellStyle name="Normal 4" xfId="451"/>
-    <cellStyle name="Normal 4 2" xfId="81"/>
-    <cellStyle name="Normal 5" xfId="450"/>
-    <cellStyle name="Normal 5 2" xfId="242"/>
-    <cellStyle name="Normal 6" xfId="453"/>
-    <cellStyle name="Normal 6 10" xfId="41"/>
-    <cellStyle name="Normal 6 10 2" xfId="121"/>
-    <cellStyle name="Normal 6 10 2 2" xfId="168"/>
-    <cellStyle name="Normal 6 10 2 3" xfId="167"/>
-    <cellStyle name="Normal 6 10 3" xfId="118"/>
-    <cellStyle name="Normal 6 10 4" xfId="117"/>
-    <cellStyle name="Normal 6 11" xfId="40"/>
-    <cellStyle name="Normal 6 11 2" xfId="251"/>
-    <cellStyle name="Normal 6 11 2 2" xfId="421"/>
-    <cellStyle name="Normal 6 11 2 3" xfId="422"/>
-    <cellStyle name="Normal 6 11 3" xfId="252"/>
-    <cellStyle name="Normal 6 11 4" xfId="250"/>
-    <cellStyle name="Normal 6 12" xfId="43"/>
-    <cellStyle name="Normal 6 12 2" xfId="227"/>
-    <cellStyle name="Normal 6 12 2 2" xfId="181"/>
-    <cellStyle name="Normal 6 12 2 3" xfId="180"/>
-    <cellStyle name="Normal 6 12 3" xfId="226"/>
-    <cellStyle name="Normal 6 12 4" xfId="225"/>
-    <cellStyle name="Normal 6 13" xfId="42"/>
-    <cellStyle name="Normal 6 13 2" xfId="16"/>
-    <cellStyle name="Normal 6 13 2 2" xfId="503"/>
-    <cellStyle name="Normal 6 13 2 3" xfId="504"/>
-    <cellStyle name="Normal 6 13 3" xfId="17"/>
-    <cellStyle name="Normal 6 13 4" xfId="11"/>
-    <cellStyle name="Normal 6 14" xfId="45"/>
-    <cellStyle name="Normal 6 14 2" xfId="337"/>
-    <cellStyle name="Normal 6 14 2 2" xfId="76"/>
-    <cellStyle name="Normal 6 14 2 3" xfId="75"/>
-    <cellStyle name="Normal 6 14 3" xfId="336"/>
-    <cellStyle name="Normal 6 14 4" xfId="338"/>
-    <cellStyle name="Normal 6 15" xfId="44"/>
-    <cellStyle name="Normal 6 15 2" xfId="130"/>
-    <cellStyle name="Normal 6 15 3" xfId="131"/>
-    <cellStyle name="Normal 6 16" xfId="47"/>
-    <cellStyle name="Normal 6 17" xfId="46"/>
-    <cellStyle name="Normal 6 2" xfId="315"/>
-    <cellStyle name="Normal 6 2 10" xfId="233"/>
-    <cellStyle name="Normal 6 2 11" xfId="232"/>
-    <cellStyle name="Normal 6 2 2" xfId="578"/>
-    <cellStyle name="Normal 6 2 2 10" xfId="528"/>
-    <cellStyle name="Normal 6 2 2 2" xfId="465"/>
-    <cellStyle name="Normal 6 2 2 2 2" xfId="485"/>
-    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8"/>
-    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220"/>
-    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436"/>
-    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260"/>
-    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508"/>
-    <cellStyle name="Normal 6 2 2 2 3" xfId="191"/>
-    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497"/>
-    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57"/>
-    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54"/>
-    <cellStyle name="Normal 6 2 2 2 4" xfId="178"/>
-    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71"/>
-    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384"/>
-    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389"/>
-    <cellStyle name="Normal 6 2 2 2 5" xfId="177"/>
-    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592"/>
-    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593"/>
-    <cellStyle name="Normal 6 2 2 2 6" xfId="483"/>
-    <cellStyle name="Normal 6 2 2 2 7" xfId="482"/>
-    <cellStyle name="Normal 6 2 2 3" xfId="464"/>
-    <cellStyle name="Normal 6 2 2 3 2" xfId="24"/>
-    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561"/>
-    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231"/>
-    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228"/>
-    <cellStyle name="Normal 6 2 2 3 3" xfId="25"/>
-    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132"/>
-    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30"/>
-    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27"/>
-    <cellStyle name="Normal 6 2 2 3 4" xfId="20"/>
-    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193"/>
-    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194"/>
-    <cellStyle name="Normal 6 2 2 3 5" xfId="21"/>
-    <cellStyle name="Normal 6 2 2 3 6" xfId="22"/>
-    <cellStyle name="Normal 6 2 2 4" xfId="467"/>
-    <cellStyle name="Normal 6 2 2 4 2" xfId="206"/>
-    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143"/>
-    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544"/>
-    <cellStyle name="Normal 6 2 2 4 3" xfId="205"/>
-    <cellStyle name="Normal 6 2 2 4 4" xfId="533"/>
-    <cellStyle name="Normal 6 2 2 5" xfId="466"/>
-    <cellStyle name="Normal 6 2 2 5 2" xfId="405"/>
-    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248"/>
-    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249"/>
-    <cellStyle name="Normal 6 2 2 5 3" xfId="406"/>
-    <cellStyle name="Normal 6 2 2 5 4" xfId="408"/>
-    <cellStyle name="Normal 6 2 2 6" xfId="469"/>
-    <cellStyle name="Normal 6 2 2 6 2" xfId="602"/>
-    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590"/>
-    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589"/>
-    <cellStyle name="Normal 6 2 2 6 3" xfId="601"/>
-    <cellStyle name="Normal 6 2 2 6 4" xfId="603"/>
-    <cellStyle name="Normal 6 2 2 7" xfId="468"/>
-    <cellStyle name="Normal 6 2 2 7 2" xfId="156"/>
-    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262"/>
-    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263"/>
-    <cellStyle name="Normal 6 2 2 7 3" xfId="157"/>
-    <cellStyle name="Normal 6 2 2 7 4" xfId="158"/>
-    <cellStyle name="Normal 6 2 2 8" xfId="101"/>
-    <cellStyle name="Normal 6 2 2 8 2" xfId="349"/>
-    <cellStyle name="Normal 6 2 2 8 3" xfId="348"/>
-    <cellStyle name="Normal 6 2 2 9" xfId="99"/>
-    <cellStyle name="Normal 6 2 3" xfId="577"/>
-    <cellStyle name="Normal 6 2 3 2" xfId="12"/>
-    <cellStyle name="Normal 6 2 3 2 2" xfId="294"/>
-    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527"/>
-    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361"/>
-    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355"/>
-    <cellStyle name="Normal 6 2 3 2 3" xfId="295"/>
-    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442"/>
-    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172"/>
-    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169"/>
-    <cellStyle name="Normal 6 2 3 2 4" xfId="289"/>
-    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213"/>
-    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214"/>
-    <cellStyle name="Normal 6 2 3 2 5" xfId="290"/>
-    <cellStyle name="Normal 6 2 3 2 6" xfId="291"/>
-    <cellStyle name="Normal 6 2 3 3" xfId="13"/>
-    <cellStyle name="Normal 6 2 3 3 2" xfId="84"/>
-    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543"/>
-    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542"/>
-    <cellStyle name="Normal 6 2 3 3 3" xfId="83"/>
-    <cellStyle name="Normal 6 2 3 3 4" xfId="82"/>
-    <cellStyle name="Normal 6 2 3 4" xfId="14"/>
-    <cellStyle name="Normal 6 2 3 4 2" xfId="216"/>
-    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660"/>
-    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661"/>
-    <cellStyle name="Normal 6 2 3 4 3" xfId="55"/>
-    <cellStyle name="Normal 6 2 3 4 4" xfId="223"/>
-    <cellStyle name="Normal 6 2 3 5" xfId="15"/>
-    <cellStyle name="Normal 6 2 3 5 2" xfId="506"/>
-    <cellStyle name="Normal 6 2 3 5 3" xfId="505"/>
-    <cellStyle name="Normal 6 2 3 6" xfId="69"/>
-    <cellStyle name="Normal 6 2 3 7" xfId="72"/>
-    <cellStyle name="Normal 6 2 4" xfId="331"/>
-    <cellStyle name="Normal 6 2 4 2" xfId="400"/>
-    <cellStyle name="Normal 6 2 4 2 2" xfId="256"/>
-    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274"/>
-    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270"/>
-    <cellStyle name="Normal 6 2 4 2 3" xfId="255"/>
-    <cellStyle name="Normal 6 2 4 2 4" xfId="257"/>
-    <cellStyle name="Normal 6 2 4 3" xfId="399"/>
-    <cellStyle name="Normal 6 2 4 3 2" xfId="458"/>
-    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150"/>
-    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151"/>
-    <cellStyle name="Normal 6 2 4 3 3" xfId="459"/>
-    <cellStyle name="Normal 6 2 4 3 4" xfId="463"/>
-    <cellStyle name="Normal 6 2 4 4" xfId="398"/>
-    <cellStyle name="Normal 6 2 4 4 2" xfId="522"/>
-    <cellStyle name="Normal 6 2 4 4 3" xfId="521"/>
-    <cellStyle name="Normal 6 2 4 5" xfId="397"/>
-    <cellStyle name="Normal 6 2 4 6" xfId="396"/>
-    <cellStyle name="Normal 6 2 5" xfId="330"/>
-    <cellStyle name="Normal 6 2 5 2" xfId="569"/>
-    <cellStyle name="Normal 6 2 5 2 2" xfId="376"/>
-    <cellStyle name="Normal 6 2 5 2 3" xfId="377"/>
-    <cellStyle name="Normal 6 2 5 3" xfId="570"/>
-    <cellStyle name="Normal 6 2 5 4" xfId="568"/>
-    <cellStyle name="Normal 6 2 6" xfId="333"/>
-    <cellStyle name="Normal 6 2 6 2" xfId="632"/>
-    <cellStyle name="Normal 6 2 6 2 2" xfId="175"/>
-    <cellStyle name="Normal 6 2 6 2 3" xfId="174"/>
-    <cellStyle name="Normal 6 2 6 3" xfId="631"/>
-    <cellStyle name="Normal 6 2 6 4" xfId="630"/>
-    <cellStyle name="Normal 6 2 7" xfId="332"/>
-    <cellStyle name="Normal 6 2 7 2" xfId="195"/>
-    <cellStyle name="Normal 6 2 7 2 2" xfId="635"/>
-    <cellStyle name="Normal 6 2 7 2 3" xfId="636"/>
-    <cellStyle name="Normal 6 2 7 3" xfId="196"/>
-    <cellStyle name="Normal 6 2 7 4" xfId="427"/>
-    <cellStyle name="Normal 6 2 8" xfId="335"/>
-    <cellStyle name="Normal 6 2 8 2" xfId="474"/>
-    <cellStyle name="Normal 6 2 8 2 2" xfId="524"/>
-    <cellStyle name="Normal 6 2 8 2 3" xfId="523"/>
-    <cellStyle name="Normal 6 2 8 3" xfId="473"/>
-    <cellStyle name="Normal 6 2 8 4" xfId="479"/>
-    <cellStyle name="Normal 6 2 9" xfId="334"/>
-    <cellStyle name="Normal 6 2 9 2" xfId="26"/>
-    <cellStyle name="Normal 6 2 9 3" xfId="98"/>
-    <cellStyle name="Normal 6 3" xfId="314"/>
-    <cellStyle name="Normal 6 3 10" xfId="183"/>
-    <cellStyle name="Normal 6 3 2" xfId="548"/>
-    <cellStyle name="Normal 6 3 2 2" xfId="207"/>
-    <cellStyle name="Normal 6 3 2 2 2" xfId="237"/>
-    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90"/>
-    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51"/>
-    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48"/>
-    <cellStyle name="Normal 6 3 2 2 3" xfId="238"/>
-    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287"/>
-    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498"/>
-    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495"/>
-    <cellStyle name="Normal 6 3 2 2 4" xfId="234"/>
-    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612"/>
-    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613"/>
-    <cellStyle name="Normal 6 3 2 2 5" xfId="235"/>
-    <cellStyle name="Normal 6 3 2 2 6" xfId="236"/>
-    <cellStyle name="Normal 6 3 2 3" xfId="208"/>
-    <cellStyle name="Normal 6 3 2 3 2" xfId="37"/>
-    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394"/>
-    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393"/>
-    <cellStyle name="Normal 6 3 2 3 3" xfId="36"/>
-    <cellStyle name="Normal 6 3 2 3 4" xfId="35"/>
-    <cellStyle name="Normal 6 3 2 4" xfId="209"/>
-    <cellStyle name="Normal 6 3 2 4 2" xfId="627"/>
-    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486"/>
-    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487"/>
-    <cellStyle name="Normal 6 3 2 4 3" xfId="628"/>
-    <cellStyle name="Normal 6 3 2 4 4" xfId="629"/>
-    <cellStyle name="Normal 6 3 2 5" xfId="210"/>
-    <cellStyle name="Normal 6 3 2 5 2" xfId="431"/>
-    <cellStyle name="Normal 6 3 2 5 3" xfId="430"/>
-    <cellStyle name="Normal 6 3 2 6" xfId="211"/>
-    <cellStyle name="Normal 6 3 2 7" xfId="212"/>
-    <cellStyle name="Normal 6 3 3" xfId="549"/>
-    <cellStyle name="Normal 6 3 3 2" xfId="645"/>
-    <cellStyle name="Normal 6 3 3 2 2" xfId="558"/>
-    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190"/>
-    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189"/>
-    <cellStyle name="Normal 6 3 3 2 3" xfId="557"/>
-    <cellStyle name="Normal 6 3 3 2 4" xfId="556"/>
-    <cellStyle name="Normal 6 3 3 3" xfId="644"/>
-    <cellStyle name="Normal 6 3 3 3 2" xfId="114"/>
-    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653"/>
-    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654"/>
-    <cellStyle name="Normal 6 3 3 3 3" xfId="115"/>
-    <cellStyle name="Normal 6 3 3 3 4" xfId="112"/>
-    <cellStyle name="Normal 6 3 3 4" xfId="647"/>
-    <cellStyle name="Normal 6 3 3 4 2" xfId="317"/>
-    <cellStyle name="Normal 6 3 3 4 3" xfId="316"/>
-    <cellStyle name="Normal 6 3 3 5" xfId="646"/>
-    <cellStyle name="Normal 6 3 3 6" xfId="648"/>
-    <cellStyle name="Normal 6 3 4" xfId="550"/>
-    <cellStyle name="Normal 6 3 4 2" xfId="160"/>
-    <cellStyle name="Normal 6 3 4 2 2" xfId="470"/>
-    <cellStyle name="Normal 6 3 4 2 3" xfId="471"/>
-    <cellStyle name="Normal 6 3 4 3" xfId="164"/>
-    <cellStyle name="Normal 6 3 4 4" xfId="155"/>
-    <cellStyle name="Normal 6 3 5" xfId="551"/>
-    <cellStyle name="Normal 6 3 5 2" xfId="493"/>
-    <cellStyle name="Normal 6 3 5 2 2" xfId="53"/>
-    <cellStyle name="Normal 6 3 5 2 3" xfId="52"/>
-    <cellStyle name="Normal 6 3 5 3" xfId="492"/>
-    <cellStyle name="Normal 6 3 5 4" xfId="491"/>
-    <cellStyle name="Normal 6 3 6" xfId="552"/>
-    <cellStyle name="Normal 6 3 6 2" xfId="323"/>
-    <cellStyle name="Normal 6 3 6 2 2" xfId="153"/>
-    <cellStyle name="Normal 6 3 6 2 3" xfId="154"/>
-    <cellStyle name="Normal 6 3 6 3" xfId="324"/>
-    <cellStyle name="Normal 6 3 6 4" xfId="322"/>
-    <cellStyle name="Normal 6 3 7" xfId="553"/>
-    <cellStyle name="Normal 6 3 7 2" xfId="111"/>
-    <cellStyle name="Normal 6 3 7 2 2" xfId="347"/>
-    <cellStyle name="Normal 6 3 7 2 3" xfId="346"/>
-    <cellStyle name="Normal 6 3 7 3" xfId="110"/>
-    <cellStyle name="Normal 6 3 7 4" xfId="109"/>
-    <cellStyle name="Normal 6 3 8" xfId="501"/>
-    <cellStyle name="Normal 6 3 8 2" xfId="305"/>
-    <cellStyle name="Normal 6 3 8 3" xfId="306"/>
-    <cellStyle name="Normal 6 3 9" xfId="502"/>
-    <cellStyle name="Normal 6 4" xfId="311"/>
-    <cellStyle name="Normal 6 4 10" xfId="100"/>
-    <cellStyle name="Normal 6 4 2" xfId="92"/>
-    <cellStyle name="Normal 6 4 2 2" xfId="140"/>
-    <cellStyle name="Normal 6 4 2 2 2" xfId="375"/>
-    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381"/>
-    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266"/>
-    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268"/>
-    <cellStyle name="Normal 6 4 2 2 3" xfId="395"/>
-    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188"/>
-    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481"/>
-    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484"/>
-    <cellStyle name="Normal 6 4 2 2 4" xfId="402"/>
-    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429"/>
-    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428"/>
-    <cellStyle name="Normal 6 4 2 2 5" xfId="401"/>
-    <cellStyle name="Normal 6 4 2 2 6" xfId="379"/>
-    <cellStyle name="Normal 6 4 2 3" xfId="139"/>
-    <cellStyle name="Normal 6 4 2 3 2" xfId="587"/>
-    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655"/>
-    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656"/>
-    <cellStyle name="Normal 6 4 2 3 3" xfId="588"/>
-    <cellStyle name="Normal 6 4 2 3 4" xfId="591"/>
-    <cellStyle name="Normal 6 4 2 4" xfId="138"/>
-    <cellStyle name="Normal 6 4 2 4 2" xfId="623"/>
-    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605"/>
-    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604"/>
-    <cellStyle name="Normal 6 4 2 4 3" xfId="622"/>
-    <cellStyle name="Normal 6 4 2 4 4" xfId="621"/>
-    <cellStyle name="Normal 6 4 2 5" xfId="137"/>
-    <cellStyle name="Normal 6 4 2 5 2" xfId="184"/>
-    <cellStyle name="Normal 6 4 2 5 3" xfId="185"/>
-    <cellStyle name="Normal 6 4 2 6" xfId="136"/>
-    <cellStyle name="Normal 6 4 2 7" xfId="135"/>
-    <cellStyle name="Normal 6 4 3" xfId="91"/>
-    <cellStyle name="Normal 6 4 3 2" xfId="342"/>
-    <cellStyle name="Normal 6 4 3 2 2" xfId="200"/>
-    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127"/>
-    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128"/>
-    <cellStyle name="Normal 6 4 3 2 3" xfId="201"/>
-    <cellStyle name="Normal 6 4 3 2 4" xfId="204"/>
-    <cellStyle name="Normal 6 4 3 3" xfId="343"/>
-    <cellStyle name="Normal 6 4 3 3 2" xfId="643"/>
-    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298"/>
-    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297"/>
-    <cellStyle name="Normal 6 4 3 3 3" xfId="642"/>
-    <cellStyle name="Normal 6 4 3 3 4" xfId="583"/>
-    <cellStyle name="Normal 6 4 3 4" xfId="340"/>
-    <cellStyle name="Normal 6 4 3 4 2" xfId="444"/>
-    <cellStyle name="Normal 6 4 3 4 3" xfId="445"/>
-    <cellStyle name="Normal 6 4 3 5" xfId="341"/>
-    <cellStyle name="Normal 6 4 3 6" xfId="339"/>
-    <cellStyle name="Normal 6 4 4" xfId="441"/>
-    <cellStyle name="Normal 6 4 4 2" xfId="292"/>
-    <cellStyle name="Normal 6 4 4 2 2" xfId="247"/>
-    <cellStyle name="Normal 6 4 4 2 3" xfId="246"/>
-    <cellStyle name="Normal 6 4 4 3" xfId="412"/>
-    <cellStyle name="Normal 6 4 4 4" xfId="293"/>
-    <cellStyle name="Normal 6 4 5" xfId="440"/>
-    <cellStyle name="Normal 6 4 5 2" xfId="460"/>
-    <cellStyle name="Normal 6 4 5 2 2" xfId="517"/>
-    <cellStyle name="Normal 6 4 5 2 3" xfId="520"/>
-    <cellStyle name="Normal 6 4 5 3" xfId="461"/>
-    <cellStyle name="Normal 6 4 5 4" xfId="462"/>
-    <cellStyle name="Normal 6 4 6" xfId="88"/>
-    <cellStyle name="Normal 6 4 6 2" xfId="5"/>
-    <cellStyle name="Normal 6 4 6 2 2" xfId="595"/>
-    <cellStyle name="Normal 6 4 6 2 3" xfId="594"/>
-    <cellStyle name="Normal 6 4 6 3" xfId="4"/>
-    <cellStyle name="Normal 6 4 6 4" xfId="10"/>
-    <cellStyle name="Normal 6 4 7" xfId="87"/>
-    <cellStyle name="Normal 6 4 7 2" xfId="221"/>
-    <cellStyle name="Normal 6 4 7 2 2" xfId="403"/>
-    <cellStyle name="Normal 6 4 7 2 3" xfId="404"/>
-    <cellStyle name="Normal 6 4 7 3" xfId="222"/>
-    <cellStyle name="Normal 6 4 7 4" xfId="224"/>
-    <cellStyle name="Normal 6 4 8" xfId="97"/>
-    <cellStyle name="Normal 6 4 8 2" xfId="95"/>
-    <cellStyle name="Normal 6 4 8 3" xfId="380"/>
-    <cellStyle name="Normal 6 4 9" xfId="96"/>
-    <cellStyle name="Normal 6 5" xfId="310"/>
-    <cellStyle name="Normal 6 5 2" xfId="285"/>
-    <cellStyle name="Normal 6 5 2 2" xfId="534"/>
-    <cellStyle name="Normal 6 5 2 2 2" xfId="182"/>
-    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547"/>
-    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259"/>
-    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261"/>
-    <cellStyle name="Normal 6 5 2 2 3" xfId="417"/>
-    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106"/>
-    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301"/>
-    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79"/>
-    <cellStyle name="Normal 6 5 2 2 4" xfId="253"/>
-    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419"/>
-    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420"/>
-    <cellStyle name="Normal 6 5 2 2 5" xfId="254"/>
-    <cellStyle name="Normal 6 5 2 2 6" xfId="192"/>
-    <cellStyle name="Normal 6 5 2 3" xfId="535"/>
-    <cellStyle name="Normal 6 5 2 3 2" xfId="649"/>
-    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370"/>
-    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369"/>
-    <cellStyle name="Normal 6 5 2 3 3" xfId="70"/>
-    <cellStyle name="Normal 6 5 2 3 4" xfId="276"/>
-    <cellStyle name="Normal 6 5 2 4" xfId="532"/>
-    <cellStyle name="Normal 6 5 2 4 2" xfId="518"/>
-    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633"/>
-    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634"/>
-    <cellStyle name="Normal 6 5 2 4 3" xfId="519"/>
-    <cellStyle name="Normal 6 5 2 4 4" xfId="514"/>
-    <cellStyle name="Normal 6 5 2 5" xfId="447"/>
-    <cellStyle name="Normal 6 5 2 5 2" xfId="304"/>
-    <cellStyle name="Normal 6 5 2 5 3" xfId="303"/>
-    <cellStyle name="Normal 6 5 2 6" xfId="530"/>
-    <cellStyle name="Normal 6 5 2 7" xfId="531"/>
-    <cellStyle name="Normal 6 5 3" xfId="286"/>
-    <cellStyle name="Normal 6 5 3 2" xfId="321"/>
-    <cellStyle name="Normal 6 5 3 2 2" xfId="134"/>
-    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600"/>
-    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599"/>
-    <cellStyle name="Normal 6 5 3 2 3" xfId="229"/>
-    <cellStyle name="Normal 6 5 3 2 4" xfId="472"/>
-    <cellStyle name="Normal 6 5 3 3" xfId="320"/>
-    <cellStyle name="Normal 6 5 3 3 2" xfId="32"/>
-    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423"/>
-    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424"/>
-    <cellStyle name="Normal 6 5 3 3 3" xfId="34"/>
-    <cellStyle name="Normal 6 5 3 3 4" xfId="9"/>
-    <cellStyle name="Normal 6 5 3 4" xfId="319"/>
-    <cellStyle name="Normal 6 5 3 4 2" xfId="94"/>
-    <cellStyle name="Normal 6 5 3 4 3" xfId="93"/>
-    <cellStyle name="Normal 6 5 3 5" xfId="318"/>
-    <cellStyle name="Normal 6 5 3 6" xfId="525"/>
-    <cellStyle name="Normal 6 5 4" xfId="283"/>
-    <cellStyle name="Normal 6 5 4 2" xfId="582"/>
-    <cellStyle name="Normal 6 5 4 2 2" xfId="478"/>
-    <cellStyle name="Normal 6 5 4 2 3" xfId="639"/>
-    <cellStyle name="Normal 6 5 4 3" xfId="197"/>
-    <cellStyle name="Normal 6 5 4 4" xfId="584"/>
-    <cellStyle name="Normal 6 5 5" xfId="284"/>
-    <cellStyle name="Normal 6 5 5 2" xfId="387"/>
-    <cellStyle name="Normal 6 5 5 2 2" xfId="119"/>
-    <cellStyle name="Normal 6 5 5 2 3" xfId="33"/>
-    <cellStyle name="Normal 6 5 5 3" xfId="386"/>
-    <cellStyle name="Normal 6 5 5 4" xfId="388"/>
-    <cellStyle name="Normal 6 5 6" xfId="281"/>
-    <cellStyle name="Normal 6 5 6 2" xfId="74"/>
-    <cellStyle name="Normal 6 5 6 3" xfId="356"/>
-    <cellStyle name="Normal 6 5 7" xfId="282"/>
-    <cellStyle name="Normal 6 5 8" xfId="280"/>
-    <cellStyle name="Normal 6 6" xfId="313"/>
-    <cellStyle name="Normal 6 6 2" xfId="326"/>
-    <cellStyle name="Normal 6 6 2 2" xfId="245"/>
-    <cellStyle name="Normal 6 6 2 2 2" xfId="64"/>
-    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515"/>
-    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617"/>
-    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619"/>
-    <cellStyle name="Normal 6 6 2 2 3" xfId="113"/>
-    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457"/>
-    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296"/>
-    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176"/>
-    <cellStyle name="Normal 6 6 2 2 4" xfId="80"/>
-    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199"/>
-    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198"/>
-    <cellStyle name="Normal 6 6 2 2 5" xfId="77"/>
-    <cellStyle name="Normal 6 6 2 2 6" xfId="129"/>
-    <cellStyle name="Normal 6 6 2 3" xfId="163"/>
-    <cellStyle name="Normal 6 6 2 3 2" xfId="662"/>
-    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278"/>
-    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279"/>
-    <cellStyle name="Normal 6 6 2 3 3" xfId="1"/>
-    <cellStyle name="Normal 6 6 2 3 4" xfId="2"/>
-    <cellStyle name="Normal 6 6 2 4" xfId="586"/>
-    <cellStyle name="Normal 6 6 2 4 2" xfId="581"/>
-    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383"/>
-    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516"/>
-    <cellStyle name="Normal 6 6 2 4 3" xfId="580"/>
-    <cellStyle name="Normal 6 6 2 4 4" xfId="579"/>
-    <cellStyle name="Normal 6 6 2 5" xfId="159"/>
-    <cellStyle name="Normal 6 6 2 5 2" xfId="141"/>
-    <cellStyle name="Normal 6 6 2 5 3" xfId="142"/>
-    <cellStyle name="Normal 6 6 2 6" xfId="162"/>
-    <cellStyle name="Normal 6 6 2 7" xfId="161"/>
-    <cellStyle name="Normal 6 6 3" xfId="325"/>
-    <cellStyle name="Normal 6 6 3 2" xfId="374"/>
-    <cellStyle name="Normal 6 6 3 2 2" xfId="275"/>
-    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410"/>
-    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411"/>
-    <cellStyle name="Normal 6 6 3 2 3" xfId="362"/>
-    <cellStyle name="Normal 6 6 3 2 4" xfId="277"/>
-    <cellStyle name="Normal 6 6 3 3" xfId="186"/>
-    <cellStyle name="Normal 6 6 3 3 2" xfId="105"/>
-    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300"/>
-    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299"/>
-    <cellStyle name="Normal 6 6 3 3 3" xfId="104"/>
-    <cellStyle name="Normal 6 6 3 3 4" xfId="574"/>
-    <cellStyle name="Normal 6 6 3 4" xfId="371"/>
-    <cellStyle name="Normal 6 6 3 4 2" xfId="391"/>
-    <cellStyle name="Normal 6 6 3 4 3" xfId="392"/>
-    <cellStyle name="Normal 6 6 3 5" xfId="372"/>
-    <cellStyle name="Normal 6 6 3 6" xfId="373"/>
-    <cellStyle name="Normal 6 6 4" xfId="108"/>
-    <cellStyle name="Normal 6 6 4 2" xfId="435"/>
-    <cellStyle name="Normal 6 6 4 2 2" xfId="433"/>
-    <cellStyle name="Normal 6 6 4 2 3" xfId="432"/>
-    <cellStyle name="Normal 6 6 4 3" xfId="434"/>
-    <cellStyle name="Normal 6 6 4 4" xfId="438"/>
-    <cellStyle name="Normal 6 6 5" xfId="585"/>
-    <cellStyle name="Normal 6 6 5 2" xfId="596"/>
-    <cellStyle name="Normal 6 6 5 2 2" xfId="554"/>
-    <cellStyle name="Normal 6 6 5 2 3" xfId="555"/>
-    <cellStyle name="Normal 6 6 5 3" xfId="597"/>
-    <cellStyle name="Normal 6 6 5 4" xfId="598"/>
-    <cellStyle name="Normal 6 6 6" xfId="616"/>
-    <cellStyle name="Normal 6 6 6 2" xfId="29"/>
-    <cellStyle name="Normal 6 6 6 3" xfId="28"/>
-    <cellStyle name="Normal 6 6 7" xfId="507"/>
-    <cellStyle name="Normal 6 6 8" xfId="513"/>
-    <cellStyle name="Normal 6 7" xfId="312"/>
-    <cellStyle name="Normal 6 7 2" xfId="65"/>
-    <cellStyle name="Normal 6 7 2 2" xfId="610"/>
-    <cellStyle name="Normal 6 7 2 2 2" xfId="122"/>
-    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244"/>
-    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120"/>
-    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562"/>
-    <cellStyle name="Normal 6 7 2 2 3" xfId="123"/>
-    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144"/>
-    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357"/>
-    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359"/>
-    <cellStyle name="Normal 6 7 2 2 4" xfId="124"/>
-    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170"/>
-    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171"/>
-    <cellStyle name="Normal 6 7 2 2 5" xfId="125"/>
-    <cellStyle name="Normal 6 7 2 2 6" xfId="126"/>
-    <cellStyle name="Normal 6 7 2 3" xfId="611"/>
-    <cellStyle name="Normal 6 7 2 3 2" xfId="572"/>
-    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49"/>
-    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327"/>
-    <cellStyle name="Normal 6 7 2 3 3" xfId="571"/>
-    <cellStyle name="Normal 6 7 2 3 4" xfId="573"/>
-    <cellStyle name="Normal 6 7 2 4" xfId="606"/>
-    <cellStyle name="Normal 6 7 2 4 2" xfId="272"/>
-    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179"/>
-    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536"/>
-    <cellStyle name="Normal 6 7 2 4 3" xfId="273"/>
-    <cellStyle name="Normal 6 7 2 4 4" xfId="271"/>
-    <cellStyle name="Normal 6 7 2 5" xfId="607"/>
-    <cellStyle name="Normal 6 7 2 5 2" xfId="86"/>
-    <cellStyle name="Normal 6 7 2 5 3" xfId="85"/>
-    <cellStyle name="Normal 6 7 2 6" xfId="608"/>
-    <cellStyle name="Normal 6 7 2 7" xfId="609"/>
-    <cellStyle name="Normal 6 7 3" xfId="66"/>
-    <cellStyle name="Normal 6 7 3 2" xfId="409"/>
-    <cellStyle name="Normal 6 7 3 2 2" xfId="476"/>
-    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353"/>
-    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352"/>
-    <cellStyle name="Normal 6 7 3 2 3" xfId="475"/>
-    <cellStyle name="Normal 6 7 3 2 4" xfId="477"/>
-    <cellStyle name="Normal 6 7 3 3" xfId="418"/>
-    <cellStyle name="Normal 6 7 3 3 2" xfId="650"/>
-    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19"/>
-    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23"/>
-    <cellStyle name="Normal 6 7 3 3 3" xfId="651"/>
-    <cellStyle name="Normal 6 7 3 3 4" xfId="652"/>
-    <cellStyle name="Normal 6 7 3 4" xfId="414"/>
-    <cellStyle name="Normal 6 7 3 4 2" xfId="563"/>
-    <cellStyle name="Normal 6 7 3 4 3" xfId="620"/>
-    <cellStyle name="Normal 6 7 3 5" xfId="413"/>
-    <cellStyle name="Normal 6 7 3 6" xfId="407"/>
-    <cellStyle name="Normal 6 7 4" xfId="60"/>
-    <cellStyle name="Normal 6 7 4 2" xfId="166"/>
-    <cellStyle name="Normal 6 7 4 2 2" xfId="509"/>
-    <cellStyle name="Normal 6 7 4 2 3" xfId="510"/>
-    <cellStyle name="Normal 6 7 4 3" xfId="490"/>
-    <cellStyle name="Normal 6 7 4 4" xfId="494"/>
-    <cellStyle name="Normal 6 7 5" xfId="61"/>
-    <cellStyle name="Normal 6 7 5 2" xfId="638"/>
-    <cellStyle name="Normal 6 7 5 2 2" xfId="152"/>
-    <cellStyle name="Normal 6 7 5 2 3" xfId="38"/>
-    <cellStyle name="Normal 6 7 5 3" xfId="637"/>
-    <cellStyle name="Normal 6 7 5 4" xfId="641"/>
-    <cellStyle name="Normal 6 7 6" xfId="62"/>
-    <cellStyle name="Normal 6 7 6 2" xfId="415"/>
-    <cellStyle name="Normal 6 7 6 3" xfId="416"/>
-    <cellStyle name="Normal 6 7 7" xfId="63"/>
-    <cellStyle name="Normal 6 7 8" xfId="59"/>
-    <cellStyle name="Normal 6 8" xfId="308"/>
-    <cellStyle name="Normal 6 8 2" xfId="364"/>
-    <cellStyle name="Normal 6 8 2 2" xfId="146"/>
-    <cellStyle name="Normal 6 8 2 2 2" xfId="3"/>
-    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345"/>
-    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344"/>
-    <cellStyle name="Normal 6 8 2 2 3" xfId="18"/>
-    <cellStyle name="Normal 6 8 2 2 4" xfId="575"/>
-    <cellStyle name="Normal 6 8 2 3" xfId="145"/>
-    <cellStyle name="Normal 6 8 2 3 2" xfId="240"/>
-    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202"/>
-    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203"/>
-    <cellStyle name="Normal 6 8 2 3 3" xfId="241"/>
-    <cellStyle name="Normal 6 8 2 3 4" xfId="239"/>
-    <cellStyle name="Normal 6 8 2 4" xfId="149"/>
-    <cellStyle name="Normal 6 8 2 4 2" xfId="625"/>
-    <cellStyle name="Normal 6 8 2 4 3" xfId="624"/>
-    <cellStyle name="Normal 6 8 2 5" xfId="148"/>
-    <cellStyle name="Normal 6 8 2 6" xfId="147"/>
-    <cellStyle name="Normal 6 8 3" xfId="363"/>
-    <cellStyle name="Normal 6 8 3 2" xfId="350"/>
-    <cellStyle name="Normal 6 8 3 2 2" xfId="488"/>
-    <cellStyle name="Normal 6 8 3 2 3" xfId="489"/>
-    <cellStyle name="Normal 6 8 3 3" xfId="351"/>
-    <cellStyle name="Normal 6 8 3 4" xfId="354"/>
-    <cellStyle name="Normal 6 8 4" xfId="368"/>
-    <cellStyle name="Normal 6 8 4 2" xfId="565"/>
-    <cellStyle name="Normal 6 8 4 2 2" xfId="165"/>
-    <cellStyle name="Normal 6 8 4 2 3" xfId="446"/>
-    <cellStyle name="Normal 6 8 4 3" xfId="564"/>
-    <cellStyle name="Normal 6 8 4 4" xfId="559"/>
-    <cellStyle name="Normal 6 8 5" xfId="367"/>
-    <cellStyle name="Normal 6 8 5 2" xfId="102"/>
-    <cellStyle name="Normal 6 8 5 3" xfId="103"/>
-    <cellStyle name="Normal 6 8 6" xfId="366"/>
-    <cellStyle name="Normal 6 8 7" xfId="365"/>
-    <cellStyle name="Normal 6 9" xfId="307"/>
-    <cellStyle name="Normal 6 9 2" xfId="537"/>
-    <cellStyle name="Normal 6 9 2 2" xfId="215"/>
-    <cellStyle name="Normal 6 9 2 2 2" xfId="264"/>
-    <cellStyle name="Normal 6 9 2 2 3" xfId="265"/>
-    <cellStyle name="Normal 6 9 2 3" xfId="566"/>
-    <cellStyle name="Normal 6 9 2 4" xfId="217"/>
-    <cellStyle name="Normal 6 9 3" xfId="538"/>
-    <cellStyle name="Normal 6 9 3 2" xfId="658"/>
-    <cellStyle name="Normal 6 9 3 2 2" xfId="426"/>
-    <cellStyle name="Normal 6 9 3 2 3" xfId="425"/>
-    <cellStyle name="Normal 6 9 3 3" xfId="657"/>
-    <cellStyle name="Normal 6 9 3 4" xfId="659"/>
-    <cellStyle name="Normal 6 9 4" xfId="540"/>
-    <cellStyle name="Normal 6 9 4 2" xfId="640"/>
-    <cellStyle name="Normal 6 9 4 3" xfId="567"/>
-    <cellStyle name="Normal 6 9 5" xfId="541"/>
-    <cellStyle name="Normal 6 9 6" xfId="539"/>
-    <cellStyle name="Normal 7" xfId="452"/>
-    <cellStyle name="Normal 7 2" xfId="529"/>
-    <cellStyle name="Normal 8" xfId="455"/>
-    <cellStyle name="Normal 8 2" xfId="576"/>
-    <cellStyle name="Normal 9" xfId="454"/>
-    <cellStyle name="Normal 9 2" xfId="58"/>
-    <cellStyle name="Percent 2" xfId="269"/>
-    <cellStyle name="Percent 2 2" xfId="78"/>
+    <cellStyle name="Normal 10" xfId="545" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="449" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2" xfId="439" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 3" xfId="448" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3 2" xfId="500" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 4" xfId="451" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 4 2" xfId="81" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 5" xfId="450" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 5 2" xfId="242" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 6" xfId="453" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 6 10" xfId="41" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 6 10 2" xfId="121" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 6 10 2 2" xfId="168" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 6 10 2 3" xfId="167" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 6 10 3" xfId="118" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 6 10 4" xfId="117" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 6 11" xfId="40" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 6 11 2" xfId="251" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 6 11 2 2" xfId="421" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 6 11 2 3" xfId="422" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 6 11 3" xfId="252" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 6 11 4" xfId="250" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 6 12" xfId="43" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 6 12 2" xfId="227" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 6 12 2 2" xfId="181" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 6 12 2 3" xfId="180" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Normal 6 12 3" xfId="226" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 6 12 4" xfId="225" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Normal 6 13" xfId="42" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 6 13 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normal 6 13 2 2" xfId="503" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normal 6 13 2 3" xfId="504" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normal 6 13 3" xfId="17" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normal 6 13 4" xfId="11" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 6 14" xfId="45" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 6 14 2" xfId="337" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 6 14 2 2" xfId="76" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 6 14 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 6 14 3" xfId="336" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 6 14 4" xfId="338" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 6 15" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Normal 6 15 2" xfId="130" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Normal 6 15 3" xfId="131" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Normal 6 16" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 6 17" xfId="46" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Normal 6 2" xfId="315" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 6 2 10" xfId="233" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 6 2 11" xfId="232" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Normal 6 2 2" xfId="578" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Normal 6 2 2 10" xfId="528" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 6 2 2 2" xfId="465" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2" xfId="485" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3" xfId="191" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4" xfId="178" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5" xfId="177" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 6 2 2 2 6" xfId="483" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 6 2 2 2 7" xfId="482" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 6 2 2 3" xfId="464" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3" xfId="25" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4" xfId="20" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 6 2 2 3 5" xfId="21" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal 6 2 2 3 6" xfId="22" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Normal 6 2 2 4" xfId="467" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2" xfId="206" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Normal 6 2 2 4 3" xfId="205" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Normal 6 2 2 4 4" xfId="533" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Normal 6 2 2 5" xfId="466" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2" xfId="405" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Normal 6 2 2 5 3" xfId="406" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Normal 6 2 2 5 4" xfId="408" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Normal 6 2 2 6" xfId="469" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2" xfId="602" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Normal 6 2 2 6 3" xfId="601" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Normal 6 2 2 6 4" xfId="603" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Normal 6 2 2 7" xfId="468" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2" xfId="156" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Normal 6 2 2 7 3" xfId="157" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Normal 6 2 2 7 4" xfId="158" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Normal 6 2 2 8" xfId="101" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Normal 6 2 2 8 2" xfId="349" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Normal 6 2 2 8 3" xfId="348" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Normal 6 2 2 9" xfId="99" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Normal 6 2 3" xfId="577" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Normal 6 2 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2" xfId="294" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3" xfId="295" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4" xfId="289" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Normal 6 2 3 2 5" xfId="290" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Normal 6 2 3 2 6" xfId="291" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Normal 6 2 3 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2" xfId="84" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Normal 6 2 3 3 3" xfId="83" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Normal 6 2 3 3 4" xfId="82" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Normal 6 2 3 4" xfId="14" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2" xfId="216" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="Normal 6 2 3 4 3" xfId="55" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Normal 6 2 3 4 4" xfId="223" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Normal 6 2 3 5" xfId="15" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="Normal 6 2 3 5 2" xfId="506" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="Normal 6 2 3 5 3" xfId="505" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Normal 6 2 3 6" xfId="69" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Normal 6 2 3 7" xfId="72" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="Normal 6 2 4" xfId="331" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="Normal 6 2 4 2" xfId="400" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2" xfId="256" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="Normal 6 2 4 2 3" xfId="255" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="Normal 6 2 4 2 4" xfId="257" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="Normal 6 2 4 3" xfId="399" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2" xfId="458" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="Normal 6 2 4 3 3" xfId="459" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="Normal 6 2 4 3 4" xfId="463" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
+    <cellStyle name="Normal 6 2 4 4" xfId="398" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
+    <cellStyle name="Normal 6 2 4 4 2" xfId="522" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
+    <cellStyle name="Normal 6 2 4 4 3" xfId="521" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
+    <cellStyle name="Normal 6 2 4 5" xfId="397" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
+    <cellStyle name="Normal 6 2 4 6" xfId="396" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
+    <cellStyle name="Normal 6 2 5" xfId="330" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
+    <cellStyle name="Normal 6 2 5 2" xfId="569" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
+    <cellStyle name="Normal 6 2 5 2 2" xfId="376" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="Normal 6 2 5 2 3" xfId="377" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="Normal 6 2 5 3" xfId="570" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="Normal 6 2 5 4" xfId="568" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="Normal 6 2 6" xfId="333" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="Normal 6 2 6 2" xfId="632" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="Normal 6 2 6 2 2" xfId="175" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="Normal 6 2 6 2 3" xfId="174" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="Normal 6 2 6 3" xfId="631" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="Normal 6 2 6 4" xfId="630" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="Normal 6 2 7" xfId="332" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="Normal 6 2 7 2" xfId="195" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="Normal 6 2 7 2 2" xfId="635" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="Normal 6 2 7 2 3" xfId="636" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="Normal 6 2 7 3" xfId="196" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="Normal 6 2 7 4" xfId="427" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="Normal 6 2 8" xfId="335" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="Normal 6 2 8 2" xfId="474" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="Normal 6 2 8 2 2" xfId="524" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="Normal 6 2 8 2 3" xfId="523" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="Normal 6 2 8 3" xfId="473" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="Normal 6 2 8 4" xfId="479" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="Normal 6 2 9" xfId="334" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="Normal 6 2 9 2" xfId="26" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="Normal 6 2 9 3" xfId="98" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="Normal 6 3" xfId="314" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="Normal 6 3 10" xfId="183" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="Normal 6 3 2" xfId="548" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="Normal 6 3 2 2" xfId="207" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2" xfId="237" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3" xfId="238" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4" xfId="234" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
+    <cellStyle name="Normal 6 3 2 2 5" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="Normal 6 3 2 2 6" xfId="236" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
+    <cellStyle name="Normal 6 3 2 3" xfId="208" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2" xfId="37" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
+    <cellStyle name="Normal 6 3 2 3 3" xfId="36" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
+    <cellStyle name="Normal 6 3 2 3 4" xfId="35" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
+    <cellStyle name="Normal 6 3 2 4" xfId="209" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2" xfId="627" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
+    <cellStyle name="Normal 6 3 2 4 3" xfId="628" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="Normal 6 3 2 4 4" xfId="629" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
+    <cellStyle name="Normal 6 3 2 5" xfId="210" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="Normal 6 3 2 5 2" xfId="431" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
+    <cellStyle name="Normal 6 3 2 5 3" xfId="430" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
+    <cellStyle name="Normal 6 3 2 6" xfId="211" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
+    <cellStyle name="Normal 6 3 2 7" xfId="212" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
+    <cellStyle name="Normal 6 3 3" xfId="549" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
+    <cellStyle name="Normal 6 3 3 2" xfId="645" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2" xfId="558" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
+    <cellStyle name="Normal 6 3 3 2 3" xfId="557" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
+    <cellStyle name="Normal 6 3 3 2 4" xfId="556" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
+    <cellStyle name="Normal 6 3 3 3" xfId="644" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
+    <cellStyle name="Normal 6 3 3 3 3" xfId="115" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="Normal 6 3 3 3 4" xfId="112" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
+    <cellStyle name="Normal 6 3 3 4" xfId="647" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
+    <cellStyle name="Normal 6 3 3 4 2" xfId="317" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
+    <cellStyle name="Normal 6 3 3 4 3" xfId="316" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
+    <cellStyle name="Normal 6 3 3 5" xfId="646" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
+    <cellStyle name="Normal 6 3 3 6" xfId="648" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
+    <cellStyle name="Normal 6 3 4" xfId="550" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
+    <cellStyle name="Normal 6 3 4 2" xfId="160" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
+    <cellStyle name="Normal 6 3 4 2 2" xfId="470" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
+    <cellStyle name="Normal 6 3 4 2 3" xfId="471" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
+    <cellStyle name="Normal 6 3 4 3" xfId="164" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
+    <cellStyle name="Normal 6 3 4 4" xfId="155" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
+    <cellStyle name="Normal 6 3 5" xfId="551" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
+    <cellStyle name="Normal 6 3 5 2" xfId="493" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
+    <cellStyle name="Normal 6 3 5 2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
+    <cellStyle name="Normal 6 3 5 2 3" xfId="52" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
+    <cellStyle name="Normal 6 3 5 3" xfId="492" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
+    <cellStyle name="Normal 6 3 5 4" xfId="491" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
+    <cellStyle name="Normal 6 3 6" xfId="552" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
+    <cellStyle name="Normal 6 3 6 2" xfId="323" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
+    <cellStyle name="Normal 6 3 6 2 2" xfId="153" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
+    <cellStyle name="Normal 6 3 6 2 3" xfId="154" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
+    <cellStyle name="Normal 6 3 6 3" xfId="324" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
+    <cellStyle name="Normal 6 3 6 4" xfId="322" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
+    <cellStyle name="Normal 6 3 7" xfId="553" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
+    <cellStyle name="Normal 6 3 7 2" xfId="111" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
+    <cellStyle name="Normal 6 3 7 2 2" xfId="347" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
+    <cellStyle name="Normal 6 3 7 2 3" xfId="346" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
+    <cellStyle name="Normal 6 3 7 3" xfId="110" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
+    <cellStyle name="Normal 6 3 7 4" xfId="109" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
+    <cellStyle name="Normal 6 3 8" xfId="501" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
+    <cellStyle name="Normal 6 3 8 2" xfId="305" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
+    <cellStyle name="Normal 6 3 8 3" xfId="306" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
+    <cellStyle name="Normal 6 3 9" xfId="502" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
+    <cellStyle name="Normal 6 4" xfId="311" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
+    <cellStyle name="Normal 6 4 10" xfId="100" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
+    <cellStyle name="Normal 6 4 2" xfId="92" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
+    <cellStyle name="Normal 6 4 2 2" xfId="140" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2" xfId="375" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3" xfId="395" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4" xfId="402" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
+    <cellStyle name="Normal 6 4 2 2 5" xfId="401" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
+    <cellStyle name="Normal 6 4 2 2 6" xfId="379" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="Normal 6 4 2 3" xfId="139" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2" xfId="587" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
+    <cellStyle name="Normal 6 4 2 3 3" xfId="588" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
+    <cellStyle name="Normal 6 4 2 3 4" xfId="591" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="Normal 6 4 2 4" xfId="138" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2" xfId="623" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
+    <cellStyle name="Normal 6 4 2 4 3" xfId="622" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
+    <cellStyle name="Normal 6 4 2 4 4" xfId="621" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
+    <cellStyle name="Normal 6 4 2 5" xfId="137" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
+    <cellStyle name="Normal 6 4 2 5 2" xfId="184" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
+    <cellStyle name="Normal 6 4 2 5 3" xfId="185" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
+    <cellStyle name="Normal 6 4 2 6" xfId="136" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
+    <cellStyle name="Normal 6 4 2 7" xfId="135" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="Normal 6 4 3" xfId="91" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
+    <cellStyle name="Normal 6 4 3 2" xfId="342" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2" xfId="200" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
+    <cellStyle name="Normal 6 4 3 2 3" xfId="201" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
+    <cellStyle name="Normal 6 4 3 2 4" xfId="204" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
+    <cellStyle name="Normal 6 4 3 3" xfId="343" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2" xfId="643" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="Normal 6 4 3 3 3" xfId="642" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
+    <cellStyle name="Normal 6 4 3 3 4" xfId="583" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
+    <cellStyle name="Normal 6 4 3 4" xfId="340" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="Normal 6 4 3 4 2" xfId="444" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
+    <cellStyle name="Normal 6 4 3 4 3" xfId="445" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
+    <cellStyle name="Normal 6 4 3 5" xfId="341" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
+    <cellStyle name="Normal 6 4 3 6" xfId="339" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
+    <cellStyle name="Normal 6 4 4" xfId="441" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
+    <cellStyle name="Normal 6 4 4 2" xfId="292" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
+    <cellStyle name="Normal 6 4 4 2 2" xfId="247" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
+    <cellStyle name="Normal 6 4 4 2 3" xfId="246" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
+    <cellStyle name="Normal 6 4 4 3" xfId="412" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
+    <cellStyle name="Normal 6 4 4 4" xfId="293" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
+    <cellStyle name="Normal 6 4 5" xfId="440" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
+    <cellStyle name="Normal 6 4 5 2" xfId="460" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
+    <cellStyle name="Normal 6 4 5 2 2" xfId="517" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
+    <cellStyle name="Normal 6 4 5 2 3" xfId="520" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
+    <cellStyle name="Normal 6 4 5 3" xfId="461" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
+    <cellStyle name="Normal 6 4 5 4" xfId="462" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
+    <cellStyle name="Normal 6 4 6" xfId="88" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
+    <cellStyle name="Normal 6 4 6 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
+    <cellStyle name="Normal 6 4 6 2 2" xfId="595" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
+    <cellStyle name="Normal 6 4 6 2 3" xfId="594" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
+    <cellStyle name="Normal 6 4 6 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
+    <cellStyle name="Normal 6 4 6 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
+    <cellStyle name="Normal 6 4 7" xfId="87" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
+    <cellStyle name="Normal 6 4 7 2" xfId="221" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
+    <cellStyle name="Normal 6 4 7 2 2" xfId="403" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
+    <cellStyle name="Normal 6 4 7 2 3" xfId="404" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
+    <cellStyle name="Normal 6 4 7 3" xfId="222" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
+    <cellStyle name="Normal 6 4 7 4" xfId="224" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
+    <cellStyle name="Normal 6 4 8" xfId="97" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
+    <cellStyle name="Normal 6 4 8 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
+    <cellStyle name="Normal 6 4 8 3" xfId="380" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
+    <cellStyle name="Normal 6 4 9" xfId="96" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
+    <cellStyle name="Normal 6 5" xfId="310" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
+    <cellStyle name="Normal 6 5 2" xfId="285" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
+    <cellStyle name="Normal 6 5 2 2" xfId="534" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2" xfId="182" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3" xfId="417" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4" xfId="253" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
+    <cellStyle name="Normal 6 5 2 2 5" xfId="254" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
+    <cellStyle name="Normal 6 5 2 2 6" xfId="192" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
+    <cellStyle name="Normal 6 5 2 3" xfId="535" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2" xfId="649" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
+    <cellStyle name="Normal 6 5 2 3 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
+    <cellStyle name="Normal 6 5 2 3 4" xfId="276" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
+    <cellStyle name="Normal 6 5 2 4" xfId="532" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2" xfId="518" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
+    <cellStyle name="Normal 6 5 2 4 3" xfId="519" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
+    <cellStyle name="Normal 6 5 2 4 4" xfId="514" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
+    <cellStyle name="Normal 6 5 2 5" xfId="447" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
+    <cellStyle name="Normal 6 5 2 5 2" xfId="304" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
+    <cellStyle name="Normal 6 5 2 5 3" xfId="303" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
+    <cellStyle name="Normal 6 5 2 6" xfId="530" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
+    <cellStyle name="Normal 6 5 2 7" xfId="531" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
+    <cellStyle name="Normal 6 5 3" xfId="286" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
+    <cellStyle name="Normal 6 5 3 2" xfId="321" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2" xfId="134" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
+    <cellStyle name="Normal 6 5 3 2 3" xfId="229" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
+    <cellStyle name="Normal 6 5 3 2 4" xfId="472" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
+    <cellStyle name="Normal 6 5 3 3" xfId="320" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
+    <cellStyle name="Normal 6 5 3 3 3" xfId="34" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
+    <cellStyle name="Normal 6 5 3 3 4" xfId="9" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
+    <cellStyle name="Normal 6 5 3 4" xfId="319" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
+    <cellStyle name="Normal 6 5 3 4 2" xfId="94" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
+    <cellStyle name="Normal 6 5 3 4 3" xfId="93" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
+    <cellStyle name="Normal 6 5 3 5" xfId="318" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
+    <cellStyle name="Normal 6 5 3 6" xfId="525" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
+    <cellStyle name="Normal 6 5 4" xfId="283" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
+    <cellStyle name="Normal 6 5 4 2" xfId="582" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
+    <cellStyle name="Normal 6 5 4 2 2" xfId="478" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
+    <cellStyle name="Normal 6 5 4 2 3" xfId="639" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
+    <cellStyle name="Normal 6 5 4 3" xfId="197" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
+    <cellStyle name="Normal 6 5 4 4" xfId="584" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
+    <cellStyle name="Normal 6 5 5" xfId="284" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
+    <cellStyle name="Normal 6 5 5 2" xfId="387" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
+    <cellStyle name="Normal 6 5 5 2 2" xfId="119" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
+    <cellStyle name="Normal 6 5 5 2 3" xfId="33" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
+    <cellStyle name="Normal 6 5 5 3" xfId="386" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
+    <cellStyle name="Normal 6 5 5 4" xfId="388" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
+    <cellStyle name="Normal 6 5 6" xfId="281" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
+    <cellStyle name="Normal 6 5 6 2" xfId="74" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
+    <cellStyle name="Normal 6 5 6 3" xfId="356" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
+    <cellStyle name="Normal 6 5 7" xfId="282" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
+    <cellStyle name="Normal 6 5 8" xfId="280" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
+    <cellStyle name="Normal 6 6" xfId="313" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
+    <cellStyle name="Normal 6 6 2" xfId="326" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
+    <cellStyle name="Normal 6 6 2 2" xfId="245" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2" xfId="64" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3" xfId="113" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4" xfId="80" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
+    <cellStyle name="Normal 6 6 2 2 5" xfId="77" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
+    <cellStyle name="Normal 6 6 2 2 6" xfId="129" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
+    <cellStyle name="Normal 6 6 2 3" xfId="163" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2" xfId="662" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
+    <cellStyle name="Normal 6 6 2 3 3" xfId="1" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
+    <cellStyle name="Normal 6 6 2 3 4" xfId="2" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
+    <cellStyle name="Normal 6 6 2 4" xfId="586" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2" xfId="581" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
+    <cellStyle name="Normal 6 6 2 4 3" xfId="580" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
+    <cellStyle name="Normal 6 6 2 4 4" xfId="579" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
+    <cellStyle name="Normal 6 6 2 5" xfId="159" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
+    <cellStyle name="Normal 6 6 2 5 2" xfId="141" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
+    <cellStyle name="Normal 6 6 2 5 3" xfId="142" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
+    <cellStyle name="Normal 6 6 2 6" xfId="162" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
+    <cellStyle name="Normal 6 6 2 7" xfId="161" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
+    <cellStyle name="Normal 6 6 3" xfId="325" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
+    <cellStyle name="Normal 6 6 3 2" xfId="374" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2" xfId="275" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
+    <cellStyle name="Normal 6 6 3 2 3" xfId="362" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
+    <cellStyle name="Normal 6 6 3 2 4" xfId="277" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
+    <cellStyle name="Normal 6 6 3 3" xfId="186" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2" xfId="105" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
+    <cellStyle name="Normal 6 6 3 3 3" xfId="104" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
+    <cellStyle name="Normal 6 6 3 3 4" xfId="574" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
+    <cellStyle name="Normal 6 6 3 4" xfId="371" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
+    <cellStyle name="Normal 6 6 3 4 2" xfId="391" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
+    <cellStyle name="Normal 6 6 3 4 3" xfId="392" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
+    <cellStyle name="Normal 6 6 3 5" xfId="372" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
+    <cellStyle name="Normal 6 6 3 6" xfId="373" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
+    <cellStyle name="Normal 6 6 4" xfId="108" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
+    <cellStyle name="Normal 6 6 4 2" xfId="435" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
+    <cellStyle name="Normal 6 6 4 2 2" xfId="433" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
+    <cellStyle name="Normal 6 6 4 2 3" xfId="432" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
+    <cellStyle name="Normal 6 6 4 3" xfId="434" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
+    <cellStyle name="Normal 6 6 4 4" xfId="438" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
+    <cellStyle name="Normal 6 6 5" xfId="585" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
+    <cellStyle name="Normal 6 6 5 2" xfId="596" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
+    <cellStyle name="Normal 6 6 5 2 2" xfId="554" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
+    <cellStyle name="Normal 6 6 5 2 3" xfId="555" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
+    <cellStyle name="Normal 6 6 5 3" xfId="597" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
+    <cellStyle name="Normal 6 6 5 4" xfId="598" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
+    <cellStyle name="Normal 6 6 6" xfId="616" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
+    <cellStyle name="Normal 6 6 6 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
+    <cellStyle name="Normal 6 6 6 3" xfId="28" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
+    <cellStyle name="Normal 6 6 7" xfId="507" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
+    <cellStyle name="Normal 6 6 8" xfId="513" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
+    <cellStyle name="Normal 6 7" xfId="312" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
+    <cellStyle name="Normal 6 7 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
+    <cellStyle name="Normal 6 7 2 2" xfId="610" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4" xfId="124" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
+    <cellStyle name="Normal 6 7 2 2 5" xfId="125" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
+    <cellStyle name="Normal 6 7 2 2 6" xfId="126" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
+    <cellStyle name="Normal 6 7 2 3" xfId="611" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2" xfId="572" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
+    <cellStyle name="Normal 6 7 2 3 3" xfId="571" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
+    <cellStyle name="Normal 6 7 2 3 4" xfId="573" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
+    <cellStyle name="Normal 6 7 2 4" xfId="606" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2" xfId="272" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
+    <cellStyle name="Normal 6 7 2 4 3" xfId="273" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
+    <cellStyle name="Normal 6 7 2 4 4" xfId="271" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
+    <cellStyle name="Normal 6 7 2 5" xfId="607" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
+    <cellStyle name="Normal 6 7 2 5 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
+    <cellStyle name="Normal 6 7 2 5 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
+    <cellStyle name="Normal 6 7 2 6" xfId="608" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
+    <cellStyle name="Normal 6 7 2 7" xfId="609" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
+    <cellStyle name="Normal 6 7 3" xfId="66" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
+    <cellStyle name="Normal 6 7 3 2" xfId="409" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2" xfId="476" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
+    <cellStyle name="Normal 6 7 3 2 3" xfId="475" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
+    <cellStyle name="Normal 6 7 3 2 4" xfId="477" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
+    <cellStyle name="Normal 6 7 3 3" xfId="418" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2" xfId="650" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
+    <cellStyle name="Normal 6 7 3 3 3" xfId="651" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
+    <cellStyle name="Normal 6 7 3 3 4" xfId="652" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
+    <cellStyle name="Normal 6 7 3 4" xfId="414" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
+    <cellStyle name="Normal 6 7 3 4 2" xfId="563" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
+    <cellStyle name="Normal 6 7 3 4 3" xfId="620" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
+    <cellStyle name="Normal 6 7 3 5" xfId="413" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
+    <cellStyle name="Normal 6 7 3 6" xfId="407" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
+    <cellStyle name="Normal 6 7 4" xfId="60" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
+    <cellStyle name="Normal 6 7 4 2" xfId="166" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
+    <cellStyle name="Normal 6 7 4 2 2" xfId="509" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
+    <cellStyle name="Normal 6 7 4 2 3" xfId="510" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
+    <cellStyle name="Normal 6 7 4 3" xfId="490" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
+    <cellStyle name="Normal 6 7 4 4" xfId="494" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
+    <cellStyle name="Normal 6 7 5" xfId="61" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
+    <cellStyle name="Normal 6 7 5 2" xfId="638" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
+    <cellStyle name="Normal 6 7 5 2 2" xfId="152" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
+    <cellStyle name="Normal 6 7 5 2 3" xfId="38" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
+    <cellStyle name="Normal 6 7 5 3" xfId="637" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
+    <cellStyle name="Normal 6 7 5 4" xfId="641" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
+    <cellStyle name="Normal 6 7 6" xfId="62" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
+    <cellStyle name="Normal 6 7 6 2" xfId="415" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
+    <cellStyle name="Normal 6 7 6 3" xfId="416" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
+    <cellStyle name="Normal 6 7 7" xfId="63" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
+    <cellStyle name="Normal 6 7 8" xfId="59" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
+    <cellStyle name="Normal 6 8" xfId="308" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
+    <cellStyle name="Normal 6 8 2" xfId="364" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
+    <cellStyle name="Normal 6 8 2 2" xfId="146" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
+    <cellStyle name="Normal 6 8 2 2 3" xfId="18" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
+    <cellStyle name="Normal 6 8 2 2 4" xfId="575" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
+    <cellStyle name="Normal 6 8 2 3" xfId="145" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2" xfId="240" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
+    <cellStyle name="Normal 6 8 2 3 3" xfId="241" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
+    <cellStyle name="Normal 6 8 2 3 4" xfId="239" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
+    <cellStyle name="Normal 6 8 2 4" xfId="149" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
+    <cellStyle name="Normal 6 8 2 4 2" xfId="625" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
+    <cellStyle name="Normal 6 8 2 4 3" xfId="624" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
+    <cellStyle name="Normal 6 8 2 5" xfId="148" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
+    <cellStyle name="Normal 6 8 2 6" xfId="147" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
+    <cellStyle name="Normal 6 8 3" xfId="363" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
+    <cellStyle name="Normal 6 8 3 2" xfId="350" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
+    <cellStyle name="Normal 6 8 3 2 2" xfId="488" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
+    <cellStyle name="Normal 6 8 3 2 3" xfId="489" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
+    <cellStyle name="Normal 6 8 3 3" xfId="351" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
+    <cellStyle name="Normal 6 8 3 4" xfId="354" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
+    <cellStyle name="Normal 6 8 4" xfId="368" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
+    <cellStyle name="Normal 6 8 4 2" xfId="565" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
+    <cellStyle name="Normal 6 8 4 2 2" xfId="165" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
+    <cellStyle name="Normal 6 8 4 2 3" xfId="446" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
+    <cellStyle name="Normal 6 8 4 3" xfId="564" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
+    <cellStyle name="Normal 6 8 4 4" xfId="559" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
+    <cellStyle name="Normal 6 8 5" xfId="367" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
+    <cellStyle name="Normal 6 8 5 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
+    <cellStyle name="Normal 6 8 5 3" xfId="103" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
+    <cellStyle name="Normal 6 8 6" xfId="366" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
+    <cellStyle name="Normal 6 8 7" xfId="365" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
+    <cellStyle name="Normal 6 9" xfId="307" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
+    <cellStyle name="Normal 6 9 2" xfId="537" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
+    <cellStyle name="Normal 6 9 2 2" xfId="215" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
+    <cellStyle name="Normal 6 9 2 2 2" xfId="264" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
+    <cellStyle name="Normal 6 9 2 2 3" xfId="265" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
+    <cellStyle name="Normal 6 9 2 3" xfId="566" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
+    <cellStyle name="Normal 6 9 2 4" xfId="217" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
+    <cellStyle name="Normal 6 9 3" xfId="538" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
+    <cellStyle name="Normal 6 9 3 2" xfId="658" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
+    <cellStyle name="Normal 6 9 3 2 2" xfId="426" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
+    <cellStyle name="Normal 6 9 3 2 3" xfId="425" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
+    <cellStyle name="Normal 6 9 3 3" xfId="657" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
+    <cellStyle name="Normal 6 9 3 4" xfId="659" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
+    <cellStyle name="Normal 6 9 4" xfId="540" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
+    <cellStyle name="Normal 6 9 4 2" xfId="640" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
+    <cellStyle name="Normal 6 9 4 3" xfId="567" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
+    <cellStyle name="Normal 6 9 5" xfId="541" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
+    <cellStyle name="Normal 6 9 6" xfId="539" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
+    <cellStyle name="Normal 7" xfId="452" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
+    <cellStyle name="Normal 7 2" xfId="529" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
+    <cellStyle name="Normal 8" xfId="455" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
+    <cellStyle name="Normal 8 2" xfId="576" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
+    <cellStyle name="Normal 9" xfId="454" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
+    <cellStyle name="Normal 9 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
+    <cellStyle name="Percent 2" xfId="269" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
+    <cellStyle name="Percent 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1745,6 +1814,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1780,6 +1866,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1955,14 +2058,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,7 +2097,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="10">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2010,7 +2113,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="13">
-        <v>220000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2043,21 +2146,45 @@
         <v>2000</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="6">
+        <v>2022</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B5:B6">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B5:B6" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
@@ -2068,17 +2195,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,17 +2215,20 @@
     <col min="3" max="3" width="11" style="23" customWidth="1"/>
     <col min="4" max="4" width="11" style="24" customWidth="1"/>
     <col min="5" max="7" width="7.42578125" style="24" customWidth="1"/>
-    <col min="8" max="11" width="7" style="24" customWidth="1"/>
-    <col min="12" max="13" width="7.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7" style="24" customWidth="1"/>
+    <col min="10" max="10" width="13" style="24" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="24" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="24" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="24" customWidth="1"/>
     <col min="14" max="15" width="7.85546875" style="24" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" style="24" customWidth="1"/>
-    <col min="17" max="18" width="10" style="24" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" style="24" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="24" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="24"/>
+    <col min="21" max="21" width="9.140625" style="24"/>
+    <col min="22" max="22" width="10.85546875" style="24" customWidth="1"/>
+    <col min="23" max="24" width="10" style="24" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" style="24" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
@@ -2121,43 +2251,25 @@
         <v>2000</v>
       </c>
       <c r="H1" s="17">
-        <v>2002</v>
+        <v>2010</v>
       </c>
       <c r="I1" s="17">
-        <v>2004</v>
-      </c>
-      <c r="J1" s="17">
-        <v>2009</v>
-      </c>
-      <c r="K1" s="17">
-        <v>2011</v>
-      </c>
-      <c r="L1" s="17">
-        <v>2012</v>
-      </c>
-      <c r="M1" s="17">
-        <v>2013</v>
-      </c>
-      <c r="N1" s="17">
-        <v>2014</v>
-      </c>
-      <c r="O1" s="17">
-        <v>2015</v>
-      </c>
-      <c r="P1" s="1" t="s">
+        <v>2017</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="M1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="17" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="2" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
@@ -2165,110 +2277,107 @@
         <v>5</v>
       </c>
       <c r="C2" s="19"/>
-      <c r="J2" s="20">
+      <c r="I2" s="20">
         <v>0</v>
       </c>
-      <c r="O2" s="20">
-        <v>1</v>
-      </c>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
       <c r="U2" s="21"/>
       <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
     </row>
-    <row r="3" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="19"/>
-      <c r="P3" s="20">
-        <v>75</v>
-      </c>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
+      <c r="I3" s="20">
+        <v>0</v>
+      </c>
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
     </row>
-    <row r="4" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="26" t="s">
+    <row r="4" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="26">
-        <v>5</v>
+      <c r="C5" s="25">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-    </row>
-    <row r="6" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="F6" s="20">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
+      <c r="C6" s="19">
+        <v>1</v>
+      </c>
       <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
     </row>
-    <row r="7" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
+      <c r="U7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E2:O2 Q2:Q3 Q5:Q6">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="W6:W7 W2:W4 E2:O3" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E3:Q3 E5:Q6">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C9:C1048576 C2:C7" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E6:O7 V6:W7" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>

</xml_diff>

<commit_message>
changing cdr from uniform distribution to beta distribution
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -1925,7 +1925,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>16.38367506937023</v>
+        <v>16.48368279065028</v>
       </c>
     </row>
     <row r="3">
@@ -1935,7 +1935,7 @@
         </is>
       </c>
       <c r="B3" s="26" t="n">
-        <v>0.6664125115791701</v>
+        <v>0.6596736217947906</v>
       </c>
       <c r="C3" s="26" t="n">
         <v>0.0001</v>
@@ -1966,7 +1966,7 @@
         </is>
       </c>
       <c r="B5" s="12" t="n">
-        <v>1901.062578098745</v>
+        <v>1899.68673035834</v>
       </c>
     </row>
     <row r="6">
@@ -1976,7 +1976,7 @@
         </is>
       </c>
       <c r="B6" s="13" t="n">
-        <v>116133.8956668223</v>
+        <v>113795.6479117848</v>
       </c>
     </row>
     <row r="7">
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.741458080701942</v>
+        <v>0.7335900370457137</v>
       </c>
     </row>
     <row r="15">
@@ -2072,7 +2072,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.06904533961598</v>
+        <v>1.102460887445562</v>
       </c>
     </row>
     <row r="16">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3.378492928678497</v>
+        <v>3.357761185341813</v>
       </c>
     </row>
     <row r="17">
@@ -2092,7 +2092,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.8710042175011699</v>
+        <v>0.8534673593383884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-enter increased TB risk param for dorms in spreadsheets (had disapeared)
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3C9B84-919B-4EE6-8F89-18DC7CCD0D48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AEDEEA-C67D-4F49-8053-4AC53B93E4CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>parameter</t>
   </si>
@@ -167,13 +167,16 @@
   </si>
   <si>
     <t>tb_perc_mdr_prevalence</t>
+  </si>
+  <si>
+    <t>riskgroup_multiplier_force_infection_dorm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,13 +212,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="6" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -226,20 +222,6 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="3" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,15 +247,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,18 +259,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB9DAED"/>
         <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1043,46 +1006,44 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="661" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="661" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="661" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="661" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="661" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="662" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="662" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="662" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="661" applyFont="1"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="661" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="661" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="662" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="662" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="662" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="58" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="58" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="662" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="662" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
@@ -2052,21 +2013,21 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="51.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="5" customWidth="1"/>
     <col min="3" max="11" width="9.140625" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2074,164 +2035,262 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="18">
         <v>25.839399894259731</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="21">
         <v>0.73688549512196821</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="21">
         <v>1E-3</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="21">
         <v>1</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="24">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="16"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="25">
         <v>1896.862755319999</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="25">
         <v>140625.15351351909</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="25">
         <v>807610</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="26">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="22">
         <v>15</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="22">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="26">
         <v>2000</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="26">
         <v>2017</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="26">
         <v>2019</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="26">
         <v>2022</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="22">
         <v>0.71838866714733918</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="22">
         <v>0.90944542195189282</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="22">
         <v>3.0469597687615231</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="22">
         <v>1.054688651351396</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="6">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="B17" s="26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="26">
         <v>1930</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="26">
         <v>6</v>
       </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="30">
+        <v>10</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2273,51 +2332,51 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="19" customWidth="1"/>
-    <col min="4" max="4" width="11" style="20" customWidth="1"/>
-    <col min="5" max="7" width="7.42578125" style="20" customWidth="1"/>
-    <col min="8" max="9" width="7" style="20" customWidth="1"/>
-    <col min="10" max="10" width="13" style="20" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="20" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="20" customWidth="1"/>
-    <col min="14" max="15" width="7.85546875" style="20" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="20" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" style="20" customWidth="1"/>
-    <col min="23" max="24" width="10" style="20" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" style="20" customWidth="1"/>
-    <col min="26" max="28" width="9.140625" style="20" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="56" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="11" customWidth="1"/>
+    <col min="4" max="4" width="11" style="12" customWidth="1"/>
+    <col min="5" max="7" width="7.42578125" style="12" customWidth="1"/>
+    <col min="8" max="9" width="7" style="12" customWidth="1"/>
+    <col min="10" max="10" width="13" style="12" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="12" customWidth="1"/>
+    <col min="14" max="15" width="7.85546875" style="12" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="12" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" style="12" customWidth="1"/>
+    <col min="23" max="24" width="10" style="12" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" style="12" customWidth="1"/>
+    <col min="26" max="28" width="9.140625" style="12" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="16">
+      <c r="D1" s="8">
         <v>1920</v>
       </c>
-      <c r="E1" s="16">
+      <c r="E1" s="8">
         <v>1980</v>
       </c>
-      <c r="F1" s="16">
+      <c r="F1" s="8">
         <v>1990</v>
       </c>
-      <c r="G1" s="16">
+      <c r="G1" s="8">
         <v>2000</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="8">
         <v>2010</v>
       </c>
-      <c r="I1" s="16">
+      <c r="I1" s="8">
         <v>2017</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -2329,113 +2388,113 @@
       <c r="L1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="12">
         <v>0</v>
       </c>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="12">
         <v>0</v>
       </c>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="12">
         <v>10</v>
       </c>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-    </row>
-    <row r="5" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+    </row>
+    <row r="5" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="11">
         <v>1</v>
       </c>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="17"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="4">

</xml_diff>

<commit_message>
Decent manual calibration for Bhutan
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AEDEEA-C67D-4F49-8053-4AC53B93E4CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A69FC-77E6-46A1-9BF2-7D49A4FD45A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>parameter</t>
   </si>
@@ -103,6 +103,21 @@
     <t>active</t>
   </si>
   <si>
+    <t>tb_prop_amplification</t>
+  </si>
+  <si>
+    <t>mdr_introduce_time</t>
+  </si>
+  <si>
+    <t>tb_perc_mdr_prevalence</t>
+  </si>
+  <si>
+    <t>riskgroup_multiplier_force_infection_dorm</t>
+  </si>
+  <si>
+    <t>program_prop_clinical_assign_strain</t>
+  </si>
+  <si>
     <t>program</t>
   </si>
   <si>
@@ -145,6 +160,12 @@
     <t>program_perc_nonsuccess_new_death</t>
   </si>
   <si>
+    <t>program_perc_treatment_inappropriate_new_success</t>
+  </si>
+  <si>
+    <t>program_perc_treatment_inappropriate_treated_success</t>
+  </si>
+  <si>
     <t>scipy</t>
   </si>
   <si>
@@ -158,25 +179,13 @@
   </si>
   <si>
     <t>runge_kutta</t>
-  </si>
-  <si>
-    <t>tb_prop_amplification</t>
-  </si>
-  <si>
-    <t>mdr_introduce_time</t>
-  </si>
-  <si>
-    <t>tb_perc_mdr_prevalence</t>
-  </si>
-  <si>
-    <t>riskgroup_multiplier_force_infection_dorm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,8 +256,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +297,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB9DAED"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1004,11 +1048,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="661" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="661" applyFont="1" applyBorder="1"/>
@@ -1019,31 +1062,34 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="662" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="662" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="662" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="661" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="58" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="58" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="662" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="662" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="58" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="10" fillId="3" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
@@ -2013,21 +2059,21 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="5" customWidth="1"/>
-    <col min="3" max="11" width="9.140625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="51.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
+    <col min="3" max="13" width="9.140625" style="13" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2035,262 +2081,250 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18">
-        <v>25.839399894259731</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="B2" s="15">
+        <v>25</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16">
+        <v>17.79</v>
+      </c>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21">
-        <v>0.73688549512196821</v>
-      </c>
-      <c r="C3" s="21">
+      <c r="B3" s="18">
+        <v>0.68515275107201679</v>
+      </c>
+      <c r="C3" s="18">
         <v>1E-3</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="18">
         <v>1</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="20">
         <v>1</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="25">
-        <v>1896.862755319999</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="B5" s="21">
+        <v>1917.2549645099309</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="25">
-        <v>140625.15351351909</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="B6" s="21">
+        <v>190014.66637936319</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="21">
         <v>807610</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="22">
         <v>5</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="25">
         <v>15</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="25">
         <v>25</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="26">
-        <v>2000</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="B9" s="22">
+        <v>1990</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="22">
         <v>2017</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="22">
         <v>2019</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="22">
         <v>2022</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="22">
-        <v>0.71838866714733918</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="B13" s="25">
+        <v>0.73310088078129476</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="22">
-        <v>0.90944542195189282</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="B14" s="25">
+        <v>0.78231454698772207</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="22">
-        <v>3.0469597687615231</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="B15" s="25">
+        <v>2.685754571491803</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="22">
-        <v>1.054688651351396</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="26">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="26">
-        <v>1930</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="26">
+      <c r="B16" s="25">
+        <v>1.4251099978452271</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="22">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="22">
+        <v>1948</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="22">
         <v>6</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="30">
-        <v>10</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="26">
+        <v>5</v>
+      </c>
+      <c r="C20" s="16"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="28">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2321,193 +2355,219 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="11" customWidth="1"/>
-    <col min="4" max="4" width="11" style="12" customWidth="1"/>
-    <col min="5" max="7" width="7.42578125" style="12" customWidth="1"/>
-    <col min="8" max="9" width="7" style="12" customWidth="1"/>
-    <col min="10" max="10" width="13" style="12" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="12" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="12" customWidth="1"/>
-    <col min="14" max="15" width="7.85546875" style="12" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="12" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" style="12" customWidth="1"/>
-    <col min="23" max="24" width="10" style="12" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" style="12" customWidth="1"/>
-    <col min="26" max="28" width="9.140625" style="12" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="56" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11" style="16" customWidth="1"/>
+    <col min="5" max="7" width="7.42578125" style="16" customWidth="1"/>
+    <col min="8" max="9" width="7" style="16" customWidth="1"/>
+    <col min="10" max="10" width="13" style="16" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="16" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="16" customWidth="1"/>
+    <col min="14" max="15" width="7.85546875" style="16" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="16" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" style="16" customWidth="1"/>
+    <col min="23" max="24" width="10" style="16" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" style="16" customWidth="1"/>
+    <col min="26" max="30" width="9.140625" style="16" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="8">
+    <row r="1" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="7">
         <v>1920</v>
       </c>
-      <c r="E1" s="8">
+      <c r="E1" s="7">
         <v>1980</v>
       </c>
-      <c r="F1" s="8">
+      <c r="F1" s="7">
         <v>1990</v>
       </c>
-      <c r="G1" s="8">
+      <c r="G1" s="7">
         <v>2000</v>
       </c>
-      <c r="H1" s="8">
+      <c r="H1" s="7">
         <v>2010</v>
       </c>
-      <c r="I1" s="8">
+      <c r="I1" s="7">
         <v>2017</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="12">
+      <c r="A2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="16">
         <v>0</v>
       </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="12">
+      <c r="A3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="16">
         <v>0</v>
       </c>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="12">
+      <c r="A4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="16">
         <v>10</v>
       </c>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-    </row>
-    <row r="5" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="13">
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+    </row>
+    <row r="5" spans="1:26" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="11">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>1</v>
       </c>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+    </row>
+    <row r="7" spans="1:26" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31">
+        <v>10</v>
+      </c>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31">
+        <v>10</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="W6:W7 W2:W4 E2:O3" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="W6 W2:W4 E2:O3" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C9:C1048576 C2:C7" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E6:O6 V6:W6 D8:J8 D7:L7" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E6:O7 V6:W7" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C10:C1048576 C2:C8" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2533,35 +2593,35 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add scenarios for IPT 0-5, IPT5-15 and Xpert to Bhutan spreadsheet
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016C4DBB-D18C-4102-BD16-16AEC527F85C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D18ED43-5356-433D-A1A3-59A8B3CF7BEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>parameter</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>int_perc_firstline_dst</t>
+  </si>
+  <si>
+    <t>int_perc_xpert</t>
   </si>
 </sst>
 </file>
@@ -2365,13 +2368,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AB9"/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2452,6 +2455,12 @@
       <c r="K2" s="16">
         <v>0</v>
       </c>
+      <c r="L2" s="16">
+        <v>100</v>
+      </c>
+      <c r="M2" s="16">
+        <v>100</v>
+      </c>
       <c r="R2" s="16"/>
       <c r="S2" s="16"/>
       <c r="T2" s="16"/>
@@ -2474,6 +2483,9 @@
       <c r="K3" s="16">
         <v>0</v>
       </c>
+      <c r="M3" s="16">
+        <v>100</v>
+      </c>
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
       <c r="T3" s="16"/>
@@ -2600,6 +2612,17 @@
       </c>
       <c r="K9" s="16">
         <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" s="16">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Treatment support intervention for Bhutan
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D18ED43-5356-433D-A1A3-59A8B3CF7BEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D5A316-F03B-472C-9724-21624B3DBD32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <author>Romain Ragonnet</author>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>parameter</t>
   </si>
@@ -185,13 +185,25 @@
   </si>
   <si>
     <t>int_perc_xpert</t>
+  </si>
+  <si>
+    <t>int_perc_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>int_perc_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>scenario_5</t>
+  </si>
+  <si>
+    <t>scenario_6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,14 +267,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1" tint="0.249977111117893"/>
       <name val="Calibri"/>
@@ -272,27 +276,43 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="5" tint="-0.499984740745262"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="6" tint="-0.499984740745262"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="4" tint="-0.499984740745262"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,12 +328,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,7 +1074,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="661" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1069,13 +1083,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="662" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="662" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="661" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1096,13 +1105,29 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="662" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="58" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="10" fillId="3" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="58" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="661" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="662" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="662" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="662" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="661" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="661" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="661" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="661" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
@@ -2074,7 +2099,7 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2082,8 +2107,8 @@
   <cols>
     <col min="1" max="1" width="51.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
-    <col min="3" max="13" width="9.140625" style="13" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="13"/>
+    <col min="3" max="13" width="9.140625" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2095,247 +2120,247 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="12">
         <v>26</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13">
         <v>17.79</v>
       </c>
-      <c r="F2" s="16"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="15">
         <v>0.6</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="15">
         <v>1E-3</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="15">
         <v>1</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="17">
         <v>1</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="18">
         <v>1910</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="18">
         <v>190014.66637936319</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="18">
         <v>807610</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="19">
         <v>5</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="22">
         <v>15</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="22">
         <v>25</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="19">
         <v>1990</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="19">
         <v>2017</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="19">
         <v>2019</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="19">
         <v>2022</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="22">
         <v>0.73310088078129476</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="22">
         <v>0.78231454698772207</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="22">
         <v>2.685754571491803</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="22">
         <v>1.4251099978452271</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="19">
         <v>0.1</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="19">
         <v>1950</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="19">
         <v>6</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="23">
         <v>3</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="25">
         <v>0.04</v>
       </c>
     </row>
@@ -2368,34 +2393,35 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AB18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="10" customWidth="1"/>
-    <col min="4" max="4" width="11" style="16" customWidth="1"/>
-    <col min="5" max="7" width="7.42578125" style="16" customWidth="1"/>
-    <col min="8" max="11" width="7" style="16" customWidth="1"/>
-    <col min="12" max="12" width="13" style="16" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" style="16" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" style="16" customWidth="1"/>
-    <col min="16" max="17" width="7.85546875" style="16" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" style="16" customWidth="1"/>
-    <col min="24" max="24" width="10.85546875" style="16" customWidth="1"/>
-    <col min="25" max="26" width="10" style="16" customWidth="1"/>
-    <col min="27" max="27" width="10.140625" style="16" customWidth="1"/>
-    <col min="28" max="32" width="9.140625" style="16" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="56" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11" style="13" customWidth="1"/>
+    <col min="5" max="7" width="7.42578125" style="13" customWidth="1"/>
+    <col min="8" max="11" width="7" style="13" customWidth="1"/>
+    <col min="12" max="12" width="13" style="13" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="13" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="13" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="13" style="13" customWidth="1"/>
+    <col min="17" max="17" width="7.85546875" style="13" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" style="13" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" style="13" customWidth="1"/>
+    <col min="25" max="26" width="10" style="13" customWidth="1"/>
+    <col min="27" max="27" width="10.140625" style="13" customWidth="1"/>
+    <col min="28" max="32" width="9.140625" style="13" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2444,199 +2470,289 @@
       <c r="O1" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="P1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="27">
+        <v>1</v>
+      </c>
+      <c r="W4" s="32"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="32"/>
+      <c r="AB4" s="32"/>
+    </row>
+    <row r="5" spans="1:28" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="E5" s="35">
         <v>30</v>
       </c>
-      <c r="B2" s="10" t="s">
+    </row>
+    <row r="6" spans="1:28" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35">
+        <v>30</v>
+      </c>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35"/>
+      <c r="V6" s="35"/>
+    </row>
+    <row r="7" spans="1:28" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="E7" s="36">
+        <v>0</v>
+      </c>
+      <c r="G7" s="36">
+        <v>0</v>
+      </c>
+      <c r="H7" s="36">
+        <v>0</v>
+      </c>
+      <c r="I7" s="36">
+        <v>15</v>
+      </c>
+      <c r="J7" s="36">
+        <v>30</v>
+      </c>
+      <c r="K7" s="36">
+        <v>55</v>
+      </c>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="35"/>
+    </row>
+    <row r="8" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="16">
+      <c r="C8" s="39"/>
+      <c r="K8" s="40">
         <v>0</v>
       </c>
-      <c r="L2" s="16">
+      <c r="L8" s="40">
         <v>100</v>
       </c>
-      <c r="M2" s="16">
+      <c r="M8" s="40">
         <v>100</v>
       </c>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="W8" s="41"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41"/>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="41"/>
+      <c r="AB8" s="41"/>
+    </row>
+    <row r="9" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B9" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="16">
+      <c r="C9" s="39"/>
+      <c r="K9" s="40">
         <v>0</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M9" s="40">
         <v>100</v>
       </c>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="16">
-        <v>10</v>
-      </c>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-    </row>
-    <row r="5" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="41"/>
+      <c r="AB9" s="41"/>
+    </row>
+    <row r="10" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="10" t="s">
+      <c r="C10" s="39"/>
+      <c r="N10" s="40">
+        <v>100</v>
+      </c>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="42"/>
+      <c r="U10" s="42"/>
+      <c r="V10" s="42"/>
+    </row>
+    <row r="11" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="10">
-        <v>1</v>
-      </c>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="8"/>
-    </row>
-    <row r="7" spans="1:28" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31">
-        <v>30</v>
-      </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31">
-        <v>30</v>
-      </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="16">
-        <v>0</v>
-      </c>
-      <c r="G9" s="16">
-        <v>0</v>
-      </c>
-      <c r="H9" s="16">
-        <v>0</v>
-      </c>
-      <c r="I9" s="16">
-        <v>15</v>
-      </c>
-      <c r="J9" s="16">
-        <v>30</v>
-      </c>
-      <c r="K9" s="16">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10" s="16">
+      <c r="C11" s="39"/>
+      <c r="O11" s="40">
         <v>100</v>
       </c>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="42"/>
+      <c r="V11" s="42"/>
+    </row>
+    <row r="12" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="O12" s="40">
+        <v>100</v>
+      </c>
+      <c r="R12" s="42"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="42"/>
+      <c r="V12" s="42"/>
+    </row>
+    <row r="13" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="42"/>
+      <c r="V13" s="42"/>
+    </row>
+    <row r="14" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="42"/>
+      <c r="V14" s="42"/>
+    </row>
+    <row r="15" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="42"/>
+      <c r="V15" s="42"/>
+    </row>
+    <row r="16" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="42"/>
+      <c r="V16" s="42"/>
+    </row>
+    <row r="17" spans="1:22" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="R17" s="42"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="42"/>
+      <c r="V17" s="42"/>
+    </row>
+    <row r="18" spans="1:22" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="R18" s="42"/>
+      <c r="S18" s="42"/>
+      <c r="T18" s="42"/>
+      <c r="U18" s="42"/>
+      <c r="V18" s="42"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="Y6 Y2:Y4 E2:Q3" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="Y4 E8:Q9 Y8:Y9 Y2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E6:Q6 X6:Y6 D8:L8 D7:N7" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E4:Q4 X4:Y4 D6:L6 D5:N5" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C10:C1048576 C2:C8" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C6 C15:C1048576 C8:C12" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Manual calibration for Bhutan
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D5A316-F03B-472C-9724-21624B3DBD32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67348BE4-93EB-4191-B004-8F31CE4DF6A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>parameter</t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>scenario_6</t>
+  </si>
+  <si>
+    <t>int_perc_xpertacf_dorm</t>
+  </si>
+  <si>
+    <t>int_prop_acf_detections_per_round_dorm</t>
+  </si>
+  <si>
+    <t>int_timeperiod_acf_rounds</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1083,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="661" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1128,6 +1137,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="58" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
@@ -2097,10 +2108,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,7 +2135,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -2138,7 +2149,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="15">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="C3" s="15">
         <v>1E-3</v>
@@ -2180,7 +2191,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="18">
-        <v>190014.66637936319</v>
+        <v>192000</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -2316,7 +2327,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="19">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -2352,7 +2363,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C20" s="13"/>
     </row>
@@ -2361,7 +2372,23 @@
         <v>22</v>
       </c>
       <c r="B21" s="25">
-        <v>0.04</v>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="44">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="44">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2393,13 +2420,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AB18"/>
+  <dimension ref="A1:AC18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2408,23 +2435,23 @@
     <col min="2" max="2" width="11" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="9" customWidth="1"/>
     <col min="4" max="4" width="11" style="13" customWidth="1"/>
-    <col min="5" max="7" width="7.42578125" style="13" customWidth="1"/>
-    <col min="8" max="11" width="7" style="13" customWidth="1"/>
-    <col min="12" max="12" width="13" style="13" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" style="13" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="13" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="13" style="13" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" style="13" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" style="13" customWidth="1"/>
-    <col min="24" max="24" width="10.85546875" style="13" customWidth="1"/>
-    <col min="25" max="26" width="10" style="13" customWidth="1"/>
-    <col min="27" max="27" width="10.140625" style="13" customWidth="1"/>
-    <col min="28" max="32" width="9.140625" style="13" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="13"/>
+    <col min="5" max="8" width="7.42578125" style="13" customWidth="1"/>
+    <col min="9" max="12" width="7" style="13" customWidth="1"/>
+    <col min="13" max="13" width="13" style="13" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="13" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="13" customWidth="1"/>
+    <col min="17" max="17" width="13" style="13" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" style="13" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="13" customWidth="1"/>
+    <col min="25" max="25" width="10.85546875" style="13" customWidth="1"/>
+    <col min="26" max="27" width="10" style="13" customWidth="1"/>
+    <col min="28" max="28" width="10.140625" style="13" customWidth="1"/>
+    <col min="29" max="33" width="9.140625" style="13" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
@@ -2447,37 +2474,40 @@
         <v>2000</v>
       </c>
       <c r="H1" s="7">
+        <v>2009</v>
+      </c>
+      <c r="I1" s="7">
         <v>2010</v>
       </c>
-      <c r="I1" s="7">
+      <c r="J1" s="7">
         <v>2012</v>
       </c>
-      <c r="J1" s="7">
+      <c r="K1" s="7">
         <v>2014</v>
       </c>
-      <c r="K1" s="7">
+      <c r="L1" s="7">
         <v>2017</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>33</v>
       </c>
@@ -2486,10 +2516,10 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>35</v>
       </c>
@@ -2499,8 +2529,11 @@
       <c r="C3" s="30">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>36</v>
       </c>
@@ -2510,13 +2543,13 @@
       <c r="C4" s="27">
         <v>1</v>
       </c>
-      <c r="W4" s="32"/>
-      <c r="Y4" s="32"/>
+      <c r="X4" s="32"/>
       <c r="Z4" s="32"/>
       <c r="AA4" s="32"/>
       <c r="AB4" s="32"/>
-    </row>
-    <row r="5" spans="1:28" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC4" s="32"/>
+    </row>
+    <row r="5" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>37</v>
       </c>
@@ -2528,7 +2561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>38</v>
       </c>
@@ -2547,13 +2580,14 @@
       <c r="J6" s="35"/>
       <c r="K6" s="35"/>
       <c r="L6" s="35"/>
-      <c r="R6" s="35"/>
+      <c r="M6" s="35"/>
       <c r="S6" s="35"/>
       <c r="T6" s="35"/>
       <c r="U6" s="35"/>
       <c r="V6" s="35"/>
-    </row>
-    <row r="7" spans="1:28" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W6" s="35"/>
+    </row>
+    <row r="7" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>44</v>
       </c>
@@ -2567,25 +2601,25 @@
       <c r="G7" s="36">
         <v>0</v>
       </c>
-      <c r="H7" s="36">
+      <c r="I7" s="36">
         <v>0</v>
-      </c>
-      <c r="I7" s="36">
-        <v>15</v>
       </c>
       <c r="J7" s="36">
         <v>30</v>
       </c>
       <c r="K7" s="36">
+        <v>45</v>
+      </c>
+      <c r="L7" s="36">
         <v>55</v>
       </c>
-      <c r="R7" s="35"/>
       <c r="S7" s="35"/>
       <c r="T7" s="35"/>
       <c r="U7" s="35"/>
       <c r="V7" s="35"/>
-    </row>
-    <row r="8" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W7" s="35"/>
+    </row>
+    <row r="8" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>30</v>
       </c>
@@ -2593,23 +2627,32 @@
         <v>31</v>
       </c>
       <c r="C8" s="39"/>
-      <c r="K8" s="40">
+      <c r="H8" s="40">
         <v>0</v>
       </c>
+      <c r="I8" s="40">
+        <v>5</v>
+      </c>
       <c r="L8" s="40">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="M8" s="40">
         <v>100</v>
       </c>
-      <c r="W8" s="41"/>
+      <c r="N8" s="40">
+        <v>100</v>
+      </c>
+      <c r="R8" s="40">
+        <v>100</v>
+      </c>
       <c r="X8" s="41"/>
       <c r="Y8" s="41"/>
       <c r="Z8" s="41"/>
       <c r="AA8" s="41"/>
       <c r="AB8" s="41"/>
-    </row>
-    <row r="9" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC8" s="41"/>
+    </row>
+    <row r="9" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>32</v>
       </c>
@@ -2617,20 +2660,23 @@
         <v>31</v>
       </c>
       <c r="C9" s="39"/>
-      <c r="K9" s="40">
+      <c r="L9" s="40">
         <v>0</v>
       </c>
-      <c r="M9" s="40">
+      <c r="N9" s="40">
         <v>100</v>
       </c>
-      <c r="W9" s="41"/>
+      <c r="R9" s="40">
+        <v>100</v>
+      </c>
       <c r="X9" s="41"/>
       <c r="Y9" s="41"/>
       <c r="Z9" s="41"/>
       <c r="AA9" s="41"/>
       <c r="AB9" s="41"/>
-    </row>
-    <row r="10" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC9" s="41"/>
+    </row>
+    <row r="10" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>45</v>
       </c>
@@ -2638,16 +2684,22 @@
         <v>31</v>
       </c>
       <c r="C10" s="39"/>
-      <c r="N10" s="40">
+      <c r="L10" s="40">
+        <v>0</v>
+      </c>
+      <c r="O10" s="40">
         <v>100</v>
       </c>
-      <c r="R10" s="42"/>
+      <c r="R10" s="40">
+        <v>100</v>
+      </c>
       <c r="S10" s="42"/>
       <c r="T10" s="42"/>
       <c r="U10" s="42"/>
       <c r="V10" s="42"/>
-    </row>
-    <row r="11" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W10" s="42"/>
+    </row>
+    <row r="11" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>46</v>
       </c>
@@ -2655,16 +2707,22 @@
         <v>31</v>
       </c>
       <c r="C11" s="39"/>
-      <c r="O11" s="40">
+      <c r="L11" s="40">
+        <v>0</v>
+      </c>
+      <c r="P11" s="40">
         <v>100</v>
       </c>
-      <c r="R11" s="42"/>
+      <c r="R11" s="40">
+        <v>100</v>
+      </c>
       <c r="S11" s="42"/>
       <c r="T11" s="42"/>
       <c r="U11" s="42"/>
       <c r="V11" s="42"/>
-    </row>
-    <row r="12" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W11" s="42"/>
+    </row>
+    <row r="12" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
         <v>47</v>
       </c>
@@ -2672,83 +2730,102 @@
         <v>31</v>
       </c>
       <c r="C12" s="39"/>
-      <c r="O12" s="40">
+      <c r="L12" s="40">
+        <v>0</v>
+      </c>
+      <c r="P12" s="40">
         <v>100</v>
       </c>
-      <c r="R12" s="42"/>
+      <c r="R12" s="40">
+        <v>100</v>
+      </c>
       <c r="S12" s="42"/>
       <c r="T12" s="42"/>
       <c r="U12" s="42"/>
       <c r="V12" s="42"/>
-    </row>
-    <row r="13" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="39"/>
+      <c r="W12" s="42"/>
+    </row>
+    <row r="13" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>34</v>
+      </c>
       <c r="C13" s="39"/>
-      <c r="R13" s="42"/>
+      <c r="L13" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="40">
+        <v>20</v>
+      </c>
+      <c r="R13" s="40">
+        <v>20</v>
+      </c>
       <c r="S13" s="42"/>
       <c r="T13" s="42"/>
       <c r="U13" s="42"/>
       <c r="V13" s="42"/>
-    </row>
-    <row r="14" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W13" s="42"/>
+    </row>
+    <row r="14" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
-      <c r="R14" s="42"/>
       <c r="S14" s="42"/>
       <c r="T14" s="42"/>
       <c r="U14" s="42"/>
       <c r="V14" s="42"/>
-    </row>
-    <row r="15" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W14" s="42"/>
+    </row>
+    <row r="15" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
-      <c r="R15" s="42"/>
       <c r="S15" s="42"/>
       <c r="T15" s="42"/>
       <c r="U15" s="42"/>
       <c r="V15" s="42"/>
-    </row>
-    <row r="16" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W15" s="42"/>
+    </row>
+    <row r="16" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
-      <c r="R16" s="42"/>
       <c r="S16" s="42"/>
       <c r="T16" s="42"/>
       <c r="U16" s="42"/>
       <c r="V16" s="42"/>
-    </row>
-    <row r="17" spans="1:22" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W16" s="42"/>
+    </row>
+    <row r="17" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
-      <c r="R17" s="42"/>
       <c r="S17" s="42"/>
       <c r="T17" s="42"/>
       <c r="U17" s="42"/>
       <c r="V17" s="42"/>
-    </row>
-    <row r="18" spans="1:22" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W17" s="42"/>
+    </row>
+    <row r="18" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
-      <c r="R18" s="42"/>
       <c r="S18" s="42"/>
       <c r="T18" s="42"/>
       <c r="U18" s="42"/>
       <c r="V18" s="42"/>
+      <c r="W18" s="42"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="Y4 E8:Q9 Y8:Y9 Y2" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="Z4 Z8:Z9 Z2 R8:R9 E8:P9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E4:Q4 X4:Y4 D6:L6 D5:N5" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E4:R4 Y4:Z4 D6:M6 D5:O5" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
loading the latest pickle file from saved_uncertainty_analyses directory
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -1956,7 +1956,7 @@
         </is>
       </c>
       <c r="B2" s="12" t="n">
-        <v>27.29802261071613</v>
+        <v>23.70558129644467</v>
       </c>
       <c r="C2" s="13" t="n"/>
       <c r="D2" s="13" t="n"/>
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="B3" s="15" t="n">
-        <v>0.7554573204062807</v>
+        <v>0.7293812134916696</v>
       </c>
       <c r="C3" s="15" t="n">
         <v>0.001</v>
@@ -2008,7 +2008,7 @@
         </is>
       </c>
       <c r="B5" s="18" t="n">
-        <v>1916.020112335067</v>
+        <v>1900.817683522394</v>
       </c>
       <c r="C5" s="13" t="n"/>
       <c r="D5" s="13" t="n"/>
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="B6" s="18" t="n">
-        <v>168138.8982421885</v>
+        <v>177447.9812439665</v>
       </c>
       <c r="C6" s="13" t="n"/>
       <c r="D6" s="13" t="n"/>
@@ -2124,7 +2124,7 @@
         </is>
       </c>
       <c r="B13" s="22" t="n">
-        <v>0.7286191478564942</v>
+        <v>0.7278559562870588</v>
       </c>
       <c r="C13" s="13" t="n"/>
       <c r="D13" s="13" t="n"/>
@@ -2138,7 +2138,7 @@
         </is>
       </c>
       <c r="B14" s="22" t="n">
-        <v>0.6290953052768301</v>
+        <v>0.6015346188309691</v>
       </c>
       <c r="C14" s="13" t="n"/>
       <c r="D14" s="13" t="n"/>
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="B15" s="22" t="n">
-        <v>2.892536556327145</v>
+        <v>2.747031447972637</v>
       </c>
       <c r="C15" s="13" t="n"/>
       <c r="D15" s="13" t="n"/>
@@ -2166,7 +2166,7 @@
         </is>
       </c>
       <c r="B16" s="22" t="n">
-        <v>1.248002213081375</v>
+        <v>1.317098396709526</v>
       </c>
       <c r="C16" s="13" t="n"/>
       <c r="D16" s="13" t="n"/>
@@ -2194,7 +2194,7 @@
         </is>
       </c>
       <c r="B18" s="19" t="n">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="C18" s="13" t="n"/>
       <c r="D18" s="13" t="n"/>

</xml_diff>

<commit_message>
BHU: Connect input costs to model properly
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06CF45A-32D3-4F27-B03D-4BA6AF88A8B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC62328C-E6F3-450A-AA39-E6AEA1E6CCAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="92">
   <si>
     <t>parameter</t>
   </si>
@@ -184,12 +184,6 @@
     <t>int_perc_xpert</t>
   </si>
   <si>
-    <t>int_perc_treatment_support_relative_ds</t>
-  </si>
-  <si>
-    <t>int_perc_treatment_support_relative_mdr</t>
-  </si>
-  <si>
     <t>int_perc_xpertacf_dorm</t>
   </si>
   <si>
@@ -236,6 +230,99 @@
   </si>
   <si>
     <t>econ_saturation_sputum_transport</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ipt_age0to5</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_ipt_age0to5</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ipt_age0to5</t>
+  </si>
+  <si>
+    <t>econ_startupduration_ipt_age0to5</t>
+  </si>
+  <si>
+    <t>econ_saturation_ipt_age0to5</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_startupduration_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_saturation_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ipt</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_ipt</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ipt</t>
+  </si>
+  <si>
+    <t>econ_startupduration_ipt</t>
+  </si>
+  <si>
+    <t>econ_saturation_ipt</t>
+  </si>
+  <si>
+    <t>econ_unitcost_xpert</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_xpert</t>
+  </si>
+  <si>
+    <t>econ_startupcost_xpert</t>
+  </si>
+  <si>
+    <t>econ_startupduration_xpert</t>
+  </si>
+  <si>
+    <t>econ_saturation_xpert</t>
+  </si>
+  <si>
+    <t>econ_unitcost_treatment_support_relative</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_treatment_support_relative</t>
+  </si>
+  <si>
+    <t>econ_startupcost_treatment_support_relative</t>
+  </si>
+  <si>
+    <t>econ_startupduration_treatment_support_relative</t>
+  </si>
+  <si>
+    <t>econ_saturation_treatment_support_relative</t>
+  </si>
+  <si>
+    <t>econ_unitcost_xpertacf_dorm</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_xpertacf_dorm</t>
+  </si>
+  <si>
+    <t>econ_startupcost_xpertacf_dorm</t>
+  </si>
+  <si>
+    <t>econ_startupduration_xpertacf_dorm</t>
+  </si>
+  <si>
+    <t>econ_saturation_xpertacf_dorm</t>
+  </si>
+  <si>
+    <t>int_perc_treatment_support_relative</t>
   </si>
 </sst>
 </file>
@@ -358,7 +445,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +467,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1126,7 +1225,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="661" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1183,7 +1282,12 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="662" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="662" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="662" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
@@ -2153,10 +2257,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2436,81 +2540,285 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+    <row r="24" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
+      <c r="B56" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
+      <c r="B57" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
-      <c r="B29" s="44"/>
-    </row>
-    <row r="30" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
-      <c r="B30" s="44"/>
-    </row>
-    <row r="31" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
-      <c r="B31" s="44"/>
-    </row>
-    <row r="32" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="46"/>
-      <c r="B32" s="44"/>
-    </row>
-    <row r="33" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="46"/>
-      <c r="B33" s="44"/>
-    </row>
-    <row r="34" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
-      <c r="B34" s="44"/>
-    </row>
-    <row r="35" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
-      <c r="B35" s="44"/>
-    </row>
-    <row r="36" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
-      <c r="B36" s="44"/>
-    </row>
-    <row r="37" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
-      <c r="B37" s="44"/>
+      <c r="B58" s="47">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2532,7 +2840,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2541,13 +2849,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AC17"/>
+  <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2630,13 +2938,13 @@
         <v>33</v>
       </c>
       <c r="S1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -2804,7 +3112,7 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>37</v>
@@ -2846,7 +3154,7 @@
     </row>
     <row r="12" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="B12" s="37" t="s">
         <v>37</v>
@@ -2868,29 +3176,28 @@
     </row>
     <row r="13" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="37"/>
       <c r="L13" s="38">
         <v>0</v>
       </c>
-      <c r="R13" s="38">
-        <v>100</v>
-      </c>
-      <c r="S13" s="40"/>
+      <c r="S13" s="40">
+        <v>20</v>
+      </c>
       <c r="T13" s="40"/>
       <c r="U13" s="40">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="V13" s="40"/>
       <c r="W13" s="40"/>
     </row>
     <row r="14" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B14" s="37" t="s">
         <v>35</v>
@@ -2899,34 +3206,23 @@
       <c r="L14" s="38">
         <v>0</v>
       </c>
-      <c r="S14" s="40">
-        <v>20</v>
-      </c>
-      <c r="T14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40">
+        <v>100</v>
+      </c>
       <c r="U14" s="40">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="V14" s="40"/>
       <c r="W14" s="40"/>
     </row>
     <row r="15" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>35</v>
-      </c>
+      <c r="A15" s="36"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="37"/>
-      <c r="L15" s="38">
-        <v>0</v>
-      </c>
       <c r="S15" s="40"/>
-      <c r="T15" s="40">
-        <v>100</v>
-      </c>
-      <c r="U15" s="40">
-        <v>100</v>
-      </c>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
       <c r="V15" s="40"/>
       <c r="W15" s="40"/>
     </row>
@@ -2939,16 +3235,6 @@
       <c r="U16" s="40"/>
       <c r="V16" s="40"/>
       <c r="W16" s="40"/>
-    </row>
-    <row r="17" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="S17" s="40"/>
-      <c r="T17" s="40"/>
-      <c r="U17" s="40"/>
-      <c r="V17" s="40"/>
-      <c r="W17" s="40"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2961,7 +3247,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C6 C15:C1048576 C11:C13 C8:C9" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C6 C14:C1048576 C11:C12 C8:C9" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2993,10 +3279,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3007,15 +3293,15 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BHU: make treatment support strain-specific
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC62328C-E6F3-450A-AA39-E6AEA1E6CCAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6D12D7-68AC-4E75-B2E7-DB7566D3DDD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
   <si>
     <t>parameter</t>
   </si>
@@ -292,21 +292,6 @@
     <t>econ_saturation_xpert</t>
   </si>
   <si>
-    <t>econ_unitcost_treatment_support_relative</t>
-  </si>
-  <si>
-    <t>econ_inflectioncost_treatment_support_relative</t>
-  </si>
-  <si>
-    <t>econ_startupcost_treatment_support_relative</t>
-  </si>
-  <si>
-    <t>econ_startupduration_treatment_support_relative</t>
-  </si>
-  <si>
-    <t>econ_saturation_treatment_support_relative</t>
-  </si>
-  <si>
     <t>econ_unitcost_xpertacf_dorm</t>
   </si>
   <si>
@@ -322,7 +307,40 @@
     <t>econ_saturation_xpertacf_dorm</t>
   </si>
   <si>
-    <t>int_perc_treatment_support_relative</t>
+    <t>int_perc_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>int_perc_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>econ_unitcost_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>econ_startupcost_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>econ_startupduration_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>econ_saturation_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>econ_unitcost_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>econ_startupcost_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>econ_startupduration_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>econ_saturation_treatment_support_relative_mdr</t>
   </si>
 </sst>
 </file>
@@ -445,7 +463,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,6 +497,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1225,7 +1249,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="661" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1288,6 +1312,9 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="662" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="662" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
@@ -2257,10 +2284,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2392,7 +2419,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="19">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -2404,7 +2431,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="19">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -2416,7 +2443,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="19">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -2702,7 +2729,7 @@
     </row>
     <row r="44" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B44" s="47">
         <v>6</v>
@@ -2710,7 +2737,7 @@
     </row>
     <row r="45" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B45" s="47">
         <v>6</v>
@@ -2718,7 +2745,7 @@
     </row>
     <row r="46" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B46" s="47">
         <v>6</v>
@@ -2726,7 +2753,7 @@
     </row>
     <row r="47" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="46" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B47" s="47">
         <v>6</v>
@@ -2734,89 +2761,129 @@
     </row>
     <row r="48" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="46" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B48" s="47">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="B49" s="44">
+    <row r="49" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="53">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="53">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="53">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="53">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="53">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="44">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" s="44">
+    <row r="55" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" s="44">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="44">
+    <row r="56" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" s="44">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="B52" s="44">
+    <row r="57" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="44">
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" s="44">
+    <row r="58" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="44">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="46" t="s">
+    <row r="59" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="47">
+      <c r="B59" s="47">
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="46" t="s">
+    <row r="60" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="47">
+      <c r="B60" s="47">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="46" t="s">
+    <row r="61" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="47">
+      <c r="B61" s="47">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="46" t="s">
+    <row r="62" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="47">
+      <c r="B62" s="47">
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="46" t="s">
+    <row r="63" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="47">
+      <c r="B63" s="47">
         <v>8</v>
       </c>
     </row>
@@ -2849,13 +2916,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3154,7 +3221,7 @@
     </row>
     <row r="12" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B12" s="37" t="s">
         <v>37</v>
@@ -3176,28 +3243,29 @@
     </row>
     <row r="13" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C13" s="37"/>
       <c r="L13" s="38">
         <v>0</v>
       </c>
-      <c r="S13" s="40">
-        <v>20</v>
-      </c>
+      <c r="R13" s="38">
+        <v>100</v>
+      </c>
+      <c r="S13" s="40"/>
       <c r="T13" s="40"/>
       <c r="U13" s="40">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="V13" s="40"/>
       <c r="W13" s="40"/>
     </row>
     <row r="14" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B14" s="37" t="s">
         <v>35</v>
@@ -3206,23 +3274,34 @@
       <c r="L14" s="38">
         <v>0</v>
       </c>
-      <c r="S14" s="40"/>
-      <c r="T14" s="40">
-        <v>100</v>
-      </c>
+      <c r="S14" s="40">
+        <v>20</v>
+      </c>
+      <c r="T14" s="40"/>
       <c r="U14" s="40">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="V14" s="40"/>
       <c r="W14" s="40"/>
     </row>
     <row r="15" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="37"/>
+      <c r="A15" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>35</v>
+      </c>
       <c r="C15" s="37"/>
+      <c r="L15" s="38">
+        <v>0</v>
+      </c>
       <c r="S15" s="40"/>
-      <c r="T15" s="40"/>
-      <c r="U15" s="40"/>
+      <c r="T15" s="40">
+        <v>100</v>
+      </c>
+      <c r="U15" s="40">
+        <v>100</v>
+      </c>
       <c r="V15" s="40"/>
       <c r="W15" s="40"/>
     </row>
@@ -3235,6 +3314,16 @@
       <c r="U16" s="40"/>
       <c r="V16" s="40"/>
       <c r="W16" s="40"/>
+    </row>
+    <row r="17" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="40"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -3247,7 +3336,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C6 C14:C1048576 C11:C12 C8:C9" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C6 C15:C1048576 C8:C9 C11:C13" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
BHU: Age-specific popsizes for IPT
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1163F31F-A4CB-4C4E-9AD9-94E2E6C7C0AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4807F4C-20D8-4385-8EE7-CE261227D95C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="102">
   <si>
     <t>parameter</t>
   </si>
@@ -344,6 +344,15 @@
   </si>
   <si>
     <t>report_start_time</t>
+  </si>
+  <si>
+    <t>nb_screened_per_detected_tb_age0to5</t>
+  </si>
+  <si>
+    <t>nb_screened_per_detected_tb_age5to15</t>
+  </si>
+  <si>
+    <t>nb_screened_per_detected_tb_allages</t>
   </si>
 </sst>
 </file>
@@ -2296,10 +2305,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:XFD64"/>
+  <dimension ref="A1:XFD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18969,153 +18978,156 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="47">
-        <v>1</v>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.45</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="47">
-        <v>1</v>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="47">
-        <v>1</v>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="4">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B28" s="47">
-        <v>1</v>
+        <f>24.03+0.5*4.5</f>
+        <v>26.28</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="47">
+        <v>429544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="47">
+      <c r="B32" s="47">
         <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="50">
-        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="49" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B33" s="50">
-        <v>2</v>
+        <f>24.03+0.5*5</f>
+        <v>26.53</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="47">
-        <v>3</v>
+      <c r="B37" s="50">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="46" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B38" s="47">
-        <v>3</v>
+        <f>24.03+0.5*5.5</f>
+        <v>26.78</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="47">
+        <v>429544</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="50">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" s="50">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="50">
-        <v>5</v>
+      <c r="B42" s="47">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="49" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B43" s="50">
         <v>5</v>
@@ -19123,39 +19135,39 @@
     </row>
     <row r="44" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="49" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B44" s="50">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="47">
-        <v>6</v>
+    <row r="45" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="50">
+        <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" s="47">
-        <v>6</v>
+    <row r="46" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="50">
+        <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B47" s="47">
-        <v>6</v>
+    <row r="47" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="50">
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="46" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B48" s="47">
         <v>6</v>
@@ -19163,39 +19175,39 @@
     </row>
     <row r="49" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="46" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B49" s="47">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="52" t="s">
-        <v>93</v>
-      </c>
-      <c r="B50" s="53">
-        <v>6.5</v>
+    <row r="50" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="47">
+        <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="52" t="s">
-        <v>94</v>
-      </c>
-      <c r="B51" s="53">
-        <v>6.5</v>
+    <row r="51" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="47">
+        <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="B52" s="53">
-        <v>6.5</v>
+    <row r="52" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="47">
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B53" s="53">
         <v>6.5</v>
@@ -19203,39 +19215,39 @@
     </row>
     <row r="54" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="52" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B54" s="53">
         <v>6.5</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="B55" s="44">
-        <v>7</v>
+    <row r="55" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="53">
+        <v>6.5</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="44">
-        <v>7</v>
+    <row r="56" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="53">
+        <v>6.5</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="B57" s="44">
-        <v>7</v>
+    <row r="57" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="53">
+        <v>6.5</v>
       </c>
     </row>
     <row r="58" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B58" s="44">
         <v>7</v>
@@ -19243,39 +19255,39 @@
     </row>
     <row r="59" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="43" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B59" s="44">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" s="47">
-        <v>8</v>
+    <row r="60" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" s="44">
+        <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="B61" s="47">
-        <v>8</v>
+    <row r="61" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" s="44">
+        <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B62" s="47">
-        <v>8</v>
+    <row r="62" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="44">
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="46" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B63" s="47">
         <v>8</v>
@@ -19283,9 +19295,33 @@
     </row>
     <row r="64" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="47">
+      <c r="B67" s="47">
         <v>8</v>
       </c>
     </row>
@@ -19540,10 +19576,10 @@
         <v>0</v>
       </c>
       <c r="I8" s="38">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L8" s="38">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M8" s="38">
         <v>100</v>

</xml_diff>

<commit_message>
BHU: Add fixed yearly costs
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BE3A4B-5B2B-4D1F-9684-95352F452B63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CA32F8-5B84-4F0E-83FF-4A4C6ADCFFEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="107">
   <si>
     <t>parameter</t>
   </si>
@@ -357,6 +357,18 @@
   <si>
     <t>int_prop_infections_in_household</t>
   </si>
+  <si>
+    <t>int_number_tests_per_tb_presentation</t>
+  </si>
+  <si>
+    <t>econ_yearlycost_ipt</t>
+  </si>
+  <si>
+    <t>econ_yearlycost_xpert</t>
+  </si>
+  <si>
+    <t>econ_yearlycost_xpertacf_dorm</t>
+  </si>
 </sst>
 </file>
 
@@ -485,7 +497,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,6 +537,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1271,7 +1289,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="661" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1342,6 +1360,10 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="58" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="662" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="8" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
@@ -2311,10 +2333,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:XFD68"/>
+  <dimension ref="A1:XFD72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35398,196 +35420,196 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="46" t="s">
+    <row r="29" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A29" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="47">
+      <c r="B30" s="47">
         <f>24.03+0.5*4.5</f>
         <v>26.28</v>
       </c>
     </row>
-    <row r="30" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+    <row r="31" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="48">
+      <c r="B31" s="48">
         <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="47">
-        <v>429544</v>
       </c>
     </row>
     <row r="32" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="47">
-        <v>10</v>
+        <v>429544</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="47">
-        <v>1</v>
+      <c r="B34" s="47">
+        <v>1.2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="49" t="s">
+    <row r="35" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="50">
+      <c r="B35" s="50">
         <f>24.03+0.5*5</f>
         <v>26.53</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="s">
+    <row r="36" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="50">
+      <c r="B36" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" s="50">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="50">
-        <v>1</v>
+      <c r="B39" s="50">
+        <v>1.2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="46" t="s">
+    <row r="40" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="47">
+      <c r="B40" s="47">
         <f>24.03+0.5*5.5</f>
         <v>26.78</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="46" t="s">
+    <row r="41" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="48">
+      <c r="B41" s="48">
         <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="B41" s="47">
-        <v>429544</v>
       </c>
     </row>
     <row r="42" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B42" s="47">
-        <v>10</v>
+        <v>429544</v>
       </c>
     </row>
     <row r="43" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="47">
-        <v>1</v>
+      <c r="B44" s="47">
+        <v>1.2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="49" t="s">
-        <v>76</v>
+    <row r="45" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="46" t="s">
+        <v>104</v>
       </c>
-      <c r="B44" s="50">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" s="50">
-        <v>5</v>
+      <c r="B45" s="47">
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="49" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B46" s="50">
-        <v>5</v>
+        <v>21.67</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="49" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B47" s="50">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="50">
+        <v>20480</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="B48" s="50">
-        <v>5</v>
+      <c r="B50" s="50">
+        <v>1.2</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="46" t="s">
-        <v>88</v>
+    <row r="51" spans="1:2" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="59" t="s">
+        <v>105</v>
       </c>
-      <c r="B49" s="47">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="47">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51" s="47">
-        <v>6</v>
+      <c r="B51" s="60">
+        <v>8060</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="46" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B52" s="47">
         <v>6</v>
@@ -35595,39 +35617,39 @@
     </row>
     <row r="53" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="46" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B53" s="47">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="52" t="s">
-        <v>93</v>
+    <row r="54" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="46" t="s">
+        <v>90</v>
       </c>
-      <c r="B54" s="53">
-        <v>6.5</v>
+      <c r="B54" s="47">
+        <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="52" t="s">
-        <v>94</v>
+    <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="46" t="s">
+        <v>91</v>
       </c>
-      <c r="B55" s="53">
-        <v>6.5</v>
+      <c r="B55" s="47">
+        <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="52" t="s">
-        <v>95</v>
+    <row r="56" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="46" t="s">
+        <v>92</v>
       </c>
-      <c r="B56" s="53">
-        <v>6.5</v>
+      <c r="B56" s="47">
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B57" s="53">
         <v>6.5</v>
@@ -35635,39 +35657,39 @@
     </row>
     <row r="58" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="52" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B58" s="53">
         <v>6.5</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="43" t="s">
-        <v>81</v>
+    <row r="59" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="52" t="s">
+        <v>95</v>
       </c>
-      <c r="B59" s="44">
-        <v>7</v>
+      <c r="B59" s="53">
+        <v>6.5</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="43" t="s">
-        <v>82</v>
+    <row r="60" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="52" t="s">
+        <v>96</v>
       </c>
-      <c r="B60" s="44">
-        <v>7</v>
+      <c r="B60" s="53">
+        <v>6.5</v>
       </c>
     </row>
-    <row r="61" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="43" t="s">
-        <v>83</v>
+    <row r="61" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="52" t="s">
+        <v>97</v>
       </c>
-      <c r="B61" s="44">
-        <v>7</v>
+      <c r="B61" s="53">
+        <v>6.5</v>
       </c>
     </row>
     <row r="62" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B62" s="44">
         <v>7</v>
@@ -35675,49 +35697,81 @@
     </row>
     <row r="63" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="43" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B63" s="44">
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="46" t="s">
-        <v>56</v>
+    <row r="64" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="43" t="s">
+        <v>83</v>
       </c>
-      <c r="B64" s="47">
-        <v>8</v>
+      <c r="B64" s="44">
+        <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="46" t="s">
-        <v>57</v>
+    <row r="65" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="43" t="s">
+        <v>84</v>
       </c>
-      <c r="B65" s="47">
-        <v>8</v>
+      <c r="B65" s="44">
+        <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="46" t="s">
-        <v>58</v>
+    <row r="66" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="43" t="s">
+        <v>85</v>
       </c>
-      <c r="B66" s="47">
-        <v>8</v>
+      <c r="B66" s="44">
+        <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="46" t="s">
-        <v>59</v>
+    <row r="67" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="43" t="s">
+        <v>106</v>
       </c>
-      <c r="B67" s="47">
-        <v>8</v>
+      <c r="B67" s="44">
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B69" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B68" s="47">
+      <c r="B72" s="47">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BHU: populate costing data for Treatment support
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CA32F8-5B84-4F0E-83FF-4A4C6ADCFFEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A302822B-0148-421A-9FDB-E9D6426E5DFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2335,8 +2335,8 @@
   </sheetPr>
   <dimension ref="A1:XFD72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView topLeftCell="A39" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35612,7 +35612,7 @@
         <v>88</v>
       </c>
       <c r="B52" s="47">
-        <v>6</v>
+        <v>170.89</v>
       </c>
     </row>
     <row r="53" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -35620,7 +35620,7 @@
         <v>89</v>
       </c>
       <c r="B53" s="47">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -35628,7 +35628,7 @@
         <v>90</v>
       </c>
       <c r="B54" s="47">
-        <v>6</v>
+        <v>16095</v>
       </c>
     </row>
     <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -35636,7 +35636,7 @@
         <v>91</v>
       </c>
       <c r="B55" s="47">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -35644,7 +35644,7 @@
         <v>92</v>
       </c>
       <c r="B56" s="47">
-        <v>6</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="57" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
@@ -35652,7 +35652,7 @@
         <v>93</v>
       </c>
       <c r="B57" s="53">
-        <v>6.5</v>
+        <v>170.89</v>
       </c>
     </row>
     <row r="58" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
@@ -35660,7 +35660,7 @@
         <v>94</v>
       </c>
       <c r="B58" s="53">
-        <v>6.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
@@ -35668,7 +35668,7 @@
         <v>95</v>
       </c>
       <c r="B59" s="53">
-        <v>6.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
@@ -35676,7 +35676,7 @@
         <v>96</v>
       </c>
       <c r="B60" s="53">
-        <v>6.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
@@ -35684,7 +35684,7 @@
         <v>97</v>
       </c>
       <c r="B61" s="53">
-        <v>6.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="62" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -35806,11 +35806,11 @@
   </sheetPr>
   <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
BHU: Populate costing data for Dorm ACF
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A302822B-0148-421A-9FDB-E9D6426E5DFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9270567-9F02-44E5-95A6-64E1DEFC6819}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2335,8 +2335,8 @@
   </sheetPr>
   <dimension ref="A1:XFD72"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35692,7 +35692,7 @@
         <v>81</v>
       </c>
       <c r="B62" s="44">
-        <v>7</v>
+        <v>22.36</v>
       </c>
     </row>
     <row r="63" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -35700,7 +35700,7 @@
         <v>82</v>
       </c>
       <c r="B63" s="44">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -35708,7 +35708,7 @@
         <v>83</v>
       </c>
       <c r="B64" s="44">
-        <v>7</v>
+        <v>44500</v>
       </c>
     </row>
     <row r="65" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -35716,7 +35716,7 @@
         <v>84</v>
       </c>
       <c r="B65" s="44">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -35724,7 +35724,7 @@
         <v>85</v>
       </c>
       <c r="B66" s="44">
-        <v>7</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="67" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -35732,7 +35732,7 @@
         <v>106</v>
       </c>
       <c r="B67" s="44">
-        <v>7</v>
+        <v>24493</v>
       </c>
     </row>
     <row r="68" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -35806,7 +35806,7 @@
   </sheetPr>
   <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
BHU: Popsize calculation and costing inputs for improved sputum transportation
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9270567-9F02-44E5-95A6-64E1DEFC6819}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9B9686-3D68-457A-8290-B1FF1B858317}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2335,8 +2335,8 @@
   </sheetPr>
   <dimension ref="A1:XFD72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35740,7 +35740,7 @@
         <v>56</v>
       </c>
       <c r="B68" s="47">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -35748,7 +35748,7 @@
         <v>57</v>
       </c>
       <c r="B69" s="47">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -35756,7 +35756,7 @@
         <v>58</v>
       </c>
       <c r="B70" s="47">
-        <v>8</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="71" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -35764,7 +35764,7 @@
         <v>59</v>
       </c>
       <c r="B71" s="47">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -35772,7 +35772,7 @@
         <v>60</v>
       </c>
       <c r="B72" s="47">
-        <v>8</v>
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BHU: clean data spreadsheet
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA835AB7-C8B7-4ED2-AC34-461A8CB2B07B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC5B81E-1C58-40BD-B2C5-28A58419C6C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="5510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2338,8 +2338,8 @@
   </sheetPr>
   <dimension ref="A1:XFD73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19010,7 +19010,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="42">
-        <v>0.23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:16384" x14ac:dyDescent="0.35">
@@ -35822,10 +35822,10 @@
   <dimension ref="A1:AC17"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36178,7 +36178,7 @@
         <v>0</v>
       </c>
       <c r="S14" s="40">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="T14" s="40"/>
       <c r="U14" s="40">

</xml_diff>

<commit_message>
BHU: scenario plots produced for each scenario separately in addition to combined plot
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC5B81E-1C58-40BD-B2C5-28A58419C6C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E9577C-FB68-4D4D-AE7C-C2BB59685469}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="5510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="5510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2338,7 +2338,7 @@
   </sheetPr>
   <dimension ref="A1:XFD73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -35821,11 +35821,11 @@
   </sheetPr>
   <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36178,7 +36178,7 @@
         <v>0</v>
       </c>
       <c r="S14" s="40">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="T14" s="40"/>
       <c r="U14" s="40">

</xml_diff>

<commit_message>
BHU: Comit to mark the version used for analysis run (6/12/2019)
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E9577C-FB68-4D4D-AE7C-C2BB59685469}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB67F00-6D41-4722-9BBD-0F819DE96F72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="5510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2342,15 +2342,15 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="4" customWidth="1"/>
-    <col min="3" max="14" width="9.1796875" style="10" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="10"/>
+    <col min="1" max="1" width="51.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
+    <col min="3" max="14" width="9.140625" style="10" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
@@ -2426,7 +2426,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>8</v>
       </c>
@@ -2438,7 +2438,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
@@ -2454,7 +2454,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
@@ -2466,7 +2466,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:16384" s="56" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16384" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
         <v>98</v>
       </c>
@@ -18856,7 +18856,7 @@
       <c r="XFC10" s="55"/>
       <c r="XFD10" s="55"/>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>11</v>
       </c>
@@ -18868,7 +18868,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>12</v>
       </c>
@@ -18880,7 +18880,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>107</v>
       </c>
@@ -18892,7 +18892,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>13</v>
       </c>
@@ -18904,7 +18904,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>14</v>
       </c>
@@ -18916,7 +18916,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>15</v>
       </c>
@@ -18928,7 +18928,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>16</v>
       </c>
@@ -18940,7 +18940,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>17</v>
       </c>
@@ -18952,7 +18952,7 @@
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>18</v>
       </c>
@@ -18964,7 +18964,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>19</v>
       </c>
@@ -18976,7 +18976,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>20</v>
       </c>
@@ -18988,7 +18988,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>21</v>
       </c>
@@ -18997,7 +18997,7 @@
       </c>
       <c r="C22" s="13"/>
     </row>
-    <row r="23" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
         <v>22</v>
       </c>
@@ -19005,7 +19005,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
         <v>23</v>
       </c>
@@ -19013,7 +19013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
         <v>24</v>
       </c>
@@ -19021,7 +19021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>99</v>
       </c>
@@ -19029,7 +19029,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="27" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>100</v>
       </c>
@@ -19037,7 +19037,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
         <v>102</v>
       </c>
@@ -35427,7 +35427,7 @@
       <c r="XFC28" s="57"/>
       <c r="XFD28" s="57"/>
     </row>
-    <row r="29" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>101</v>
       </c>
@@ -35435,7 +35435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A30" s="58" t="s">
         <v>103</v>
       </c>
@@ -35443,7 +35443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
         <v>61</v>
       </c>
@@ -35452,7 +35452,7 @@
         <v>26.28</v>
       </c>
     </row>
-    <row r="32" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="46" t="s">
         <v>62</v>
       </c>
@@ -35460,7 +35460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="46" t="s">
         <v>63</v>
       </c>
@@ -35468,7 +35468,7 @@
         <v>429544</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="46" t="s">
         <v>64</v>
       </c>
@@ -35476,7 +35476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
         <v>65</v>
       </c>
@@ -35484,7 +35484,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="49" t="s">
         <v>66</v>
       </c>
@@ -35493,7 +35493,7 @@
         <v>26.53</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="49" t="s">
         <v>67</v>
       </c>
@@ -35501,7 +35501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="49" t="s">
         <v>68</v>
       </c>
@@ -35509,7 +35509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49" t="s">
         <v>69</v>
       </c>
@@ -35517,7 +35517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="49" t="s">
         <v>70</v>
       </c>
@@ -35525,7 +35525,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
         <v>71</v>
       </c>
@@ -35534,7 +35534,7 @@
         <v>26.78</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
         <v>72</v>
       </c>
@@ -35542,7 +35542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
         <v>73</v>
       </c>
@@ -35550,7 +35550,7 @@
         <v>429544</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
         <v>74</v>
       </c>
@@ -35558,7 +35558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
         <v>75</v>
       </c>
@@ -35566,7 +35566,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
         <v>104</v>
       </c>
@@ -35574,7 +35574,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="49" t="s">
         <v>76</v>
       </c>
@@ -35582,7 +35582,7 @@
         <v>21.67</v>
       </c>
     </row>
-    <row r="48" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="49" t="s">
         <v>77</v>
       </c>
@@ -35590,7 +35590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="49" t="s">
         <v>78</v>
       </c>
@@ -35598,7 +35598,7 @@
         <v>20480</v>
       </c>
     </row>
-    <row r="50" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="49" t="s">
         <v>79</v>
       </c>
@@ -35606,7 +35606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="49" t="s">
         <v>80</v>
       </c>
@@ -35614,7 +35614,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="52" spans="1:2" s="61" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="59" t="s">
         <v>105</v>
       </c>
@@ -35622,7 +35622,7 @@
         <v>8060</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="46" t="s">
         <v>88</v>
       </c>
@@ -35630,7 +35630,7 @@
         <v>170.89</v>
       </c>
     </row>
-    <row r="54" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="46" t="s">
         <v>89</v>
       </c>
@@ -35638,7 +35638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="46" t="s">
         <v>90</v>
       </c>
@@ -35646,7 +35646,7 @@
         <v>16095</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="46" t="s">
         <v>91</v>
       </c>
@@ -35654,7 +35654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="46" t="s">
         <v>92</v>
       </c>
@@ -35662,7 +35662,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="52" t="s">
         <v>93</v>
       </c>
@@ -35670,7 +35670,7 @@
         <v>170.89</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="52" t="s">
         <v>94</v>
       </c>
@@ -35678,7 +35678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="52" t="s">
         <v>95</v>
       </c>
@@ -35686,7 +35686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="52" t="s">
         <v>96</v>
       </c>
@@ -35694,7 +35694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="52" t="s">
         <v>97</v>
       </c>
@@ -35702,7 +35702,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="43" t="s">
         <v>81</v>
       </c>
@@ -35710,7 +35710,7 @@
         <v>22.36</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="43" t="s">
         <v>82</v>
       </c>
@@ -35718,7 +35718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="43" t="s">
         <v>83</v>
       </c>
@@ -35726,7 +35726,7 @@
         <v>44500</v>
       </c>
     </row>
-    <row r="66" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="43" t="s">
         <v>84</v>
       </c>
@@ -35734,7 +35734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="43" t="s">
         <v>85</v>
       </c>
@@ -35742,7 +35742,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="43" t="s">
         <v>106</v>
       </c>
@@ -35750,7 +35750,7 @@
         <v>24493</v>
       </c>
     </row>
-    <row r="69" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="46" t="s">
         <v>56</v>
       </c>
@@ -35758,7 +35758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="46" t="s">
         <v>57</v>
       </c>
@@ -35766,7 +35766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="46" t="s">
         <v>58</v>
       </c>
@@ -35774,7 +35774,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="72" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="46" t="s">
         <v>59</v>
       </c>
@@ -35782,7 +35782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="46" t="s">
         <v>60</v>
       </c>
@@ -35822,37 +35822,37 @@
   <dimension ref="A1:AC17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
+      <selection pane="bottomRight" activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="9" customWidth="1"/>
     <col min="4" max="4" width="11" style="13" customWidth="1"/>
-    <col min="5" max="8" width="7.453125" style="13" customWidth="1"/>
+    <col min="5" max="8" width="7.42578125" style="13" customWidth="1"/>
     <col min="9" max="12" width="7" style="13" customWidth="1"/>
     <col min="13" max="13" width="13" style="13" customWidth="1"/>
-    <col min="14" max="14" width="12.1796875" style="13" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" style="13" customWidth="1"/>
-    <col min="16" max="16" width="11.1796875" style="13" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="13" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="13" customWidth="1"/>
     <col min="17" max="17" width="13" style="13" customWidth="1"/>
-    <col min="18" max="18" width="11.26953125" style="13" customWidth="1"/>
-    <col min="19" max="19" width="11.1796875" customWidth="1"/>
-    <col min="20" max="20" width="10.453125" customWidth="1"/>
-    <col min="24" max="24" width="9.1796875" style="13" customWidth="1"/>
-    <col min="25" max="25" width="10.81640625" style="13" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="13" customWidth="1"/>
+    <col min="25" max="25" width="10.85546875" style="13" customWidth="1"/>
     <col min="26" max="27" width="10" style="13" customWidth="1"/>
-    <col min="28" max="28" width="10.1796875" style="13" customWidth="1"/>
-    <col min="29" max="34" width="9.1796875" style="13" customWidth="1"/>
-    <col min="35" max="16384" width="9.1796875" style="13"/>
+    <col min="28" max="28" width="10.140625" style="13" customWidth="1"/>
+    <col min="29" max="34" width="9.140625" style="13" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
@@ -35917,7 +35917,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>34</v>
       </c>
@@ -35929,7 +35929,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>36</v>
       </c>
@@ -35943,7 +35943,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>38</v>
       </c>
@@ -35959,7 +35959,7 @@
       <c r="AB4" s="30"/>
       <c r="AC4" s="30"/>
     </row>
-    <row r="5" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>39</v>
       </c>
@@ -35971,7 +35971,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="34" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>40</v>
       </c>
@@ -35997,7 +35997,7 @@
       <c r="V6" s="33"/>
       <c r="W6" s="33"/>
     </row>
-    <row r="7" spans="1:29" s="34" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>41</v>
       </c>
@@ -36029,7 +36029,7 @@
       <c r="V7" s="33"/>
       <c r="W7" s="33"/>
     </row>
-    <row r="8" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>42</v>
       </c>
@@ -36059,7 +36059,7 @@
       <c r="AB8" s="39"/>
       <c r="AC8" s="39"/>
     </row>
-    <row r="9" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>43</v>
       </c>
@@ -36080,7 +36080,7 @@
       <c r="AB9" s="39"/>
       <c r="AC9" s="39"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>51</v>
       </c>
@@ -36100,7 +36100,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>44</v>
       </c>
@@ -36122,7 +36122,7 @@
       <c r="V11" s="40"/>
       <c r="W11" s="40"/>
     </row>
-    <row r="12" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>86</v>
       </c>
@@ -36144,7 +36144,7 @@
       <c r="V12" s="40"/>
       <c r="W12" s="40"/>
     </row>
-    <row r="13" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>87</v>
       </c>
@@ -36166,7 +36166,7 @@
       <c r="V13" s="40"/>
       <c r="W13" s="40"/>
     </row>
-    <row r="14" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
         <v>45</v>
       </c>
@@ -36187,7 +36187,7 @@
       <c r="V14" s="40"/>
       <c r="W14" s="40"/>
     </row>
-    <row r="15" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
         <v>55</v>
       </c>
@@ -36208,7 +36208,7 @@
       <c r="V15" s="40"/>
       <c r="W15" s="40"/>
     </row>
-    <row r="16" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="37"/>
       <c r="C16" s="37"/>
@@ -36218,7 +36218,7 @@
       <c r="V16" s="40"/>
       <c r="W16" s="40"/>
     </row>
-    <row r="17" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -36261,9 +36261,9 @@
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -36277,7 +36277,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -36288,7 +36288,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
BHU: Cosmetic changes to plots
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB67F00-6D41-4722-9BBD-0F819DE96F72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF89641-2586-4A18-8B67-167550E7A6CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2338,8 +2338,8 @@
   </sheetPr>
   <dimension ref="A1:XFD73"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2407,7 +2407,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="18">
-        <v>1900.817683522394</v>
+        <v>1901</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -35819,13 +35819,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AC17"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X12" sqref="X12"/>
+      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35835,24 +35835,24 @@
     <col min="3" max="3" width="11" style="9" customWidth="1"/>
     <col min="4" max="4" width="11" style="13" customWidth="1"/>
     <col min="5" max="8" width="7.42578125" style="13" customWidth="1"/>
-    <col min="9" max="12" width="7" style="13" customWidth="1"/>
-    <col min="13" max="13" width="13" style="13" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="13" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="13" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" style="13" customWidth="1"/>
-    <col min="17" max="17" width="13" style="13" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="11.140625" customWidth="1"/>
-    <col min="20" max="20" width="10.42578125" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="13" customWidth="1"/>
-    <col min="25" max="25" width="10.85546875" style="13" customWidth="1"/>
-    <col min="26" max="27" width="10" style="13" customWidth="1"/>
-    <col min="28" max="28" width="10.140625" style="13" customWidth="1"/>
-    <col min="29" max="34" width="9.140625" style="13" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="13"/>
+    <col min="9" max="13" width="7" style="13" customWidth="1"/>
+    <col min="14" max="14" width="13" style="13" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="13" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" style="13" customWidth="1"/>
+    <col min="18" max="18" width="13" style="13" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" style="13" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="13" customWidth="1"/>
+    <col min="26" max="26" width="10.85546875" style="13" customWidth="1"/>
+    <col min="27" max="28" width="10" style="13" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" style="13" customWidth="1"/>
+    <col min="30" max="35" width="9.140625" style="13" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
@@ -35889,35 +35889,38 @@
       <c r="L1" s="7">
         <v>2019</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="7">
+        <v>2020</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>34</v>
       </c>
@@ -35929,7 +35932,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>36</v>
       </c>
@@ -35943,7 +35946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>38</v>
       </c>
@@ -35953,13 +35956,13 @@
       <c r="C4" s="25">
         <v>1</v>
       </c>
-      <c r="X4" s="30"/>
-      <c r="Z4" s="30"/>
+      <c r="Y4" s="30"/>
       <c r="AA4" s="30"/>
       <c r="AB4" s="30"/>
       <c r="AC4" s="30"/>
+      <c r="AD4" s="30"/>
     </row>
-    <row r="5" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>39</v>
       </c>
@@ -35971,7 +35974,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>40</v>
       </c>
@@ -35991,13 +35994,14 @@
       <c r="K6" s="33"/>
       <c r="L6" s="33"/>
       <c r="M6" s="33"/>
-      <c r="S6" s="33"/>
+      <c r="N6" s="33"/>
       <c r="T6" s="33"/>
       <c r="U6" s="33"/>
       <c r="V6" s="33"/>
       <c r="W6" s="33"/>
+      <c r="X6" s="33"/>
     </row>
-    <row r="7" spans="1:29" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>41</v>
       </c>
@@ -36023,13 +36027,13 @@
       <c r="L7" s="34">
         <v>55</v>
       </c>
-      <c r="S7" s="33"/>
       <c r="T7" s="33"/>
       <c r="U7" s="33"/>
       <c r="V7" s="33"/>
       <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
     </row>
-    <row r="8" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>42</v>
       </c>
@@ -36046,20 +36050,20 @@
       <c r="L8" s="38">
         <v>0</v>
       </c>
-      <c r="M8" s="38">
-        <v>100</v>
-      </c>
       <c r="N8" s="38">
         <v>100</v>
       </c>
-      <c r="X8" s="39"/>
+      <c r="O8" s="38">
+        <v>100</v>
+      </c>
       <c r="Y8" s="39"/>
       <c r="Z8" s="39"/>
       <c r="AA8" s="39"/>
       <c r="AB8" s="39"/>
       <c r="AC8" s="39"/>
+      <c r="AD8" s="39"/>
     </row>
-    <row r="9" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>43</v>
       </c>
@@ -36070,17 +36074,17 @@
       <c r="L9" s="38">
         <v>0</v>
       </c>
-      <c r="N9" s="38">
+      <c r="O9" s="38">
         <v>100</v>
       </c>
-      <c r="X9" s="39"/>
       <c r="Y9" s="39"/>
       <c r="Z9" s="39"/>
       <c r="AA9" s="39"/>
       <c r="AB9" s="39"/>
       <c r="AC9" s="39"/>
+      <c r="AD9" s="39"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>51</v>
       </c>
@@ -36090,17 +36094,17 @@
       <c r="L10" s="13">
         <v>0</v>
       </c>
-      <c r="O10" s="13">
-        <v>100</v>
-      </c>
       <c r="P10" s="13">
         <v>100</v>
       </c>
-      <c r="U10">
+      <c r="Q10" s="13">
+        <v>100</v>
+      </c>
+      <c r="V10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>44</v>
       </c>
@@ -36111,18 +36115,18 @@
       <c r="L11" s="38">
         <v>0</v>
       </c>
-      <c r="Q11" s="38">
+      <c r="R11" s="38">
         <v>100</v>
       </c>
-      <c r="S11" s="40"/>
       <c r="T11" s="40"/>
-      <c r="U11" s="40">
+      <c r="U11" s="40"/>
+      <c r="V11" s="40">
         <v>100</v>
       </c>
-      <c r="V11" s="40"/>
       <c r="W11" s="40"/>
+      <c r="X11" s="40"/>
     </row>
-    <row r="12" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>86</v>
       </c>
@@ -36133,18 +36137,18 @@
       <c r="L12" s="38">
         <v>0</v>
       </c>
-      <c r="R12" s="38">
+      <c r="S12" s="38">
         <v>100</v>
       </c>
-      <c r="S12" s="40"/>
       <c r="T12" s="40"/>
-      <c r="U12" s="40">
+      <c r="U12" s="40"/>
+      <c r="V12" s="40">
         <v>100</v>
       </c>
-      <c r="V12" s="40"/>
       <c r="W12" s="40"/>
+      <c r="X12" s="40"/>
     </row>
-    <row r="13" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>87</v>
       </c>
@@ -36155,18 +36159,18 @@
       <c r="L13" s="38">
         <v>0</v>
       </c>
-      <c r="R13" s="38">
+      <c r="S13" s="38">
         <v>100</v>
       </c>
-      <c r="S13" s="40"/>
       <c r="T13" s="40"/>
-      <c r="U13" s="40">
+      <c r="U13" s="40"/>
+      <c r="V13" s="40">
         <v>100</v>
       </c>
-      <c r="V13" s="40"/>
       <c r="W13" s="40"/>
+      <c r="X13" s="40"/>
     </row>
-    <row r="14" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
         <v>45</v>
       </c>
@@ -36177,17 +36181,20 @@
       <c r="L14" s="38">
         <v>0</v>
       </c>
-      <c r="S14" s="40">
+      <c r="M14" s="38">
+        <v>0</v>
+      </c>
+      <c r="T14" s="40">
         <v>20</v>
       </c>
-      <c r="T14" s="40"/>
-      <c r="U14" s="40">
+      <c r="U14" s="40"/>
+      <c r="V14" s="40">
         <v>20</v>
       </c>
-      <c r="V14" s="40"/>
       <c r="W14" s="40"/>
+      <c r="X14" s="40"/>
     </row>
-    <row r="15" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
         <v>55</v>
       </c>
@@ -36198,44 +36205,44 @@
       <c r="L15" s="38">
         <v>0</v>
       </c>
-      <c r="S15" s="40"/>
-      <c r="T15" s="40">
-        <v>100</v>
-      </c>
+      <c r="T15" s="40"/>
       <c r="U15" s="40">
         <v>100</v>
       </c>
-      <c r="V15" s="40"/>
+      <c r="V15" s="40">
+        <v>100</v>
+      </c>
       <c r="W15" s="40"/>
+      <c r="X15" s="40"/>
     </row>
-    <row r="16" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="37"/>
       <c r="C16" s="37"/>
-      <c r="S16" s="40"/>
       <c r="T16" s="40"/>
       <c r="U16" s="40"/>
       <c r="V16" s="40"/>
       <c r="W16" s="40"/>
+      <c r="X16" s="40"/>
     </row>
-    <row r="17" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
-      <c r="S17" s="40"/>
       <c r="T17" s="40"/>
       <c r="U17" s="40"/>
       <c r="V17" s="40"/>
       <c r="W17" s="40"/>
+      <c r="X17" s="40"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="Z4 Z8:Z9 Z2 R8:R9 E8:P9" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="AA4 AA8:AA9 AA2 S8:S9 E8:Q9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E4:R4 Y4:Z4 D6:M6 D5:O5" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="L6:N6 Z4:AA4 L5:P5 D5:K6 E4:S4" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
BHU: Add baseline treatment intervention to account for cost-savings through interventions
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF89641-2586-4A18-8B67-167550E7A6CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3CCFBA-A2FF-4354-8090-1A698E33C8BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="5510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="120">
   <si>
     <t>parameter</t>
   </si>
@@ -371,6 +371,42 @@
   </si>
   <si>
     <t>before_intervention_time</t>
+  </si>
+  <si>
+    <t>int_perc_baseline_treatment_ds</t>
+  </si>
+  <si>
+    <t>int_perc_baseline_treatment_mdr</t>
+  </si>
+  <si>
+    <t>econ_unitcost_baseline_treatment_ds</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_baseline_treatment_ds</t>
+  </si>
+  <si>
+    <t>econ_startupcost_baseline_treatment_ds</t>
+  </si>
+  <si>
+    <t>econ_startupduration_baseline_treatment_ds</t>
+  </si>
+  <si>
+    <t>econ_saturation_baseline_treatment_ds</t>
+  </si>
+  <si>
+    <t>econ_unitcost_baseline_treatment_mdr</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_baseline_treatment_mdr</t>
+  </si>
+  <si>
+    <t>econ_startupcost_baseline_treatment_mdr</t>
+  </si>
+  <si>
+    <t>econ_startupduration_baseline_treatment_mdr</t>
+  </si>
+  <si>
+    <t>econ_saturation_baseline_treatment_mdr</t>
   </si>
 </sst>
 </file>
@@ -2336,21 +2372,21 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:XFD73"/>
+  <dimension ref="A1:XFD83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
-    <col min="3" max="14" width="9.140625" style="10" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="51.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="4" customWidth="1"/>
+    <col min="3" max="14" width="9.1796875" style="10" customWidth="1"/>
+    <col min="15" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2358,7 +2394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
@@ -2372,7 +2408,7 @@
       </c>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
@@ -2390,7 +2426,7 @@
       </c>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
@@ -2402,7 +2438,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
@@ -2414,7 +2450,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
@@ -2426,7 +2462,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>8</v>
       </c>
@@ -2438,7 +2474,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
@@ -2454,7 +2490,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
@@ -2466,7 +2502,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:16384" s="56" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16384" s="56" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="55" t="s">
         <v>98</v>
       </c>
@@ -18856,7 +18892,7 @@
       <c r="XFC10" s="55"/>
       <c r="XFD10" s="55"/>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>11</v>
       </c>
@@ -18868,7 +18904,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
         <v>12</v>
       </c>
@@ -18880,7 +18916,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>107</v>
       </c>
@@ -18892,7 +18928,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>13</v>
       </c>
@@ -18904,7 +18940,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
         <v>14</v>
       </c>
@@ -18916,7 +18952,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
         <v>15</v>
       </c>
@@ -18928,7 +18964,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
         <v>16</v>
       </c>
@@ -18940,7 +18976,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
         <v>17</v>
       </c>
@@ -18952,7 +18988,7 @@
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
         <v>18</v>
       </c>
@@ -18964,7 +19000,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>19</v>
       </c>
@@ -18976,7 +19012,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
         <v>20</v>
       </c>
@@ -18988,7 +19024,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
         <v>21</v>
       </c>
@@ -18997,7 +19033,7 @@
       </c>
       <c r="C22" s="13"/>
     </row>
-    <row r="23" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A23" s="41" t="s">
         <v>22</v>
       </c>
@@ -19005,7 +19041,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A24" s="41" t="s">
         <v>23</v>
       </c>
@@ -19013,7 +19049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A25" s="41" t="s">
         <v>24</v>
       </c>
@@ -19021,7 +19057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>99</v>
       </c>
@@ -19029,7 +19065,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="27" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>100</v>
       </c>
@@ -19037,7 +19073,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A28" s="57" t="s">
         <v>102</v>
       </c>
@@ -35427,7 +35463,7 @@
       <c r="XFC28" s="57"/>
       <c r="XFD28" s="57"/>
     </row>
-    <row r="29" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>101</v>
       </c>
@@ -35435,7 +35471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A30" s="58" t="s">
         <v>103</v>
       </c>
@@ -35443,7 +35479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="46" t="s">
         <v>61</v>
       </c>
@@ -35452,7 +35488,7 @@
         <v>26.28</v>
       </c>
     </row>
-    <row r="32" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="46" t="s">
         <v>62</v>
       </c>
@@ -35460,7 +35496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="46" t="s">
         <v>63</v>
       </c>
@@ -35468,7 +35504,7 @@
         <v>429544</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="46" t="s">
         <v>64</v>
       </c>
@@ -35476,7 +35512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="46" t="s">
         <v>65</v>
       </c>
@@ -35484,7 +35520,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="49" t="s">
         <v>66</v>
       </c>
@@ -35493,7 +35529,7 @@
         <v>26.53</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="49" t="s">
         <v>67</v>
       </c>
@@ -35501,7 +35537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="49" t="s">
         <v>68</v>
       </c>
@@ -35509,7 +35545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="49" t="s">
         <v>69</v>
       </c>
@@ -35517,7 +35553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="49" t="s">
         <v>70</v>
       </c>
@@ -35525,7 +35561,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="46" t="s">
         <v>71</v>
       </c>
@@ -35534,7 +35570,7 @@
         <v>26.78</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="46" t="s">
         <v>72</v>
       </c>
@@ -35542,7 +35578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="46" t="s">
         <v>73</v>
       </c>
@@ -35550,7 +35586,7 @@
         <v>429544</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="46" t="s">
         <v>74</v>
       </c>
@@ -35558,7 +35594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="46" t="s">
         <v>75</v>
       </c>
@@ -35566,7 +35602,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="46" t="s">
         <v>104</v>
       </c>
@@ -35574,7 +35610,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="49" t="s">
         <v>76</v>
       </c>
@@ -35582,7 +35618,7 @@
         <v>21.67</v>
       </c>
     </row>
-    <row r="48" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="49" t="s">
         <v>77</v>
       </c>
@@ -35590,7 +35626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="49" t="s">
         <v>78</v>
       </c>
@@ -35598,7 +35634,7 @@
         <v>20480</v>
       </c>
     </row>
-    <row r="50" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="49" t="s">
         <v>79</v>
       </c>
@@ -35606,7 +35642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="49" t="s">
         <v>80</v>
       </c>
@@ -35614,7 +35650,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="52" spans="1:2" s="61" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" s="61" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="59" t="s">
         <v>105</v>
       </c>
@@ -35622,7 +35658,7 @@
         <v>8060</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="46" t="s">
         <v>88</v>
       </c>
@@ -35630,7 +35666,7 @@
         <v>170.89</v>
       </c>
     </row>
-    <row r="54" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="46" t="s">
         <v>89</v>
       </c>
@@ -35638,7 +35674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="46" t="s">
         <v>90</v>
       </c>
@@ -35646,7 +35682,7 @@
         <v>16095</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="46" t="s">
         <v>91</v>
       </c>
@@ -35654,7 +35690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="46" t="s">
         <v>92</v>
       </c>
@@ -35662,7 +35698,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="52" t="s">
         <v>93</v>
       </c>
@@ -35670,7 +35706,7 @@
         <v>170.89</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="52" t="s">
         <v>94</v>
       </c>
@@ -35678,7 +35714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="52" t="s">
         <v>95</v>
       </c>
@@ -35686,7 +35722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="52" t="s">
         <v>96</v>
       </c>
@@ -35694,7 +35730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="52" t="s">
         <v>97</v>
       </c>
@@ -35702,7 +35738,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="43" t="s">
         <v>81</v>
       </c>
@@ -35710,7 +35746,7 @@
         <v>22.36</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="43" t="s">
         <v>82</v>
       </c>
@@ -35718,7 +35754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="43" t="s">
         <v>83</v>
       </c>
@@ -35726,7 +35762,7 @@
         <v>44500</v>
       </c>
     </row>
-    <row r="66" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="43" t="s">
         <v>84</v>
       </c>
@@ -35734,7 +35770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="43" t="s">
         <v>85</v>
       </c>
@@ -35742,7 +35778,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="43" t="s">
         <v>106</v>
       </c>
@@ -35750,7 +35786,7 @@
         <v>24493</v>
       </c>
     </row>
-    <row r="69" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="46" t="s">
         <v>56</v>
       </c>
@@ -35758,7 +35794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="46" t="s">
         <v>57</v>
       </c>
@@ -35766,7 +35802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="46" t="s">
         <v>58</v>
       </c>
@@ -35774,7 +35810,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="72" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="46" t="s">
         <v>59</v>
       </c>
@@ -35782,11 +35818,91 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="46" t="s">
         <v>60</v>
       </c>
       <c r="B73" s="47">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="B74" s="50">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="B75" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B76" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="B77" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B78" s="50">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="B79" s="50">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B80" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B81" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="B82" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="B83" s="50">
         <v>1.2</v>
       </c>
     </row>
@@ -35819,40 +35935,40 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AD17"/>
+  <dimension ref="A1:AD18"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="56" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="9" customWidth="1"/>
     <col min="4" max="4" width="11" style="13" customWidth="1"/>
-    <col min="5" max="8" width="7.42578125" style="13" customWidth="1"/>
+    <col min="5" max="8" width="7.453125" style="13" customWidth="1"/>
     <col min="9" max="13" width="7" style="13" customWidth="1"/>
     <col min="14" max="14" width="13" style="13" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" style="13" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="12.1796875" style="13" customWidth="1"/>
+    <col min="16" max="16" width="11.453125" style="13" customWidth="1"/>
+    <col min="17" max="17" width="11.1796875" style="13" customWidth="1"/>
     <col min="18" max="18" width="13" style="13" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" style="13" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" style="13" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" style="13" customWidth="1"/>
+    <col min="19" max="19" width="11.26953125" style="13" customWidth="1"/>
+    <col min="20" max="20" width="11.1796875" customWidth="1"/>
+    <col min="21" max="21" width="10.453125" customWidth="1"/>
+    <col min="25" max="25" width="9.1796875" style="13" customWidth="1"/>
+    <col min="26" max="26" width="10.81640625" style="13" customWidth="1"/>
     <col min="27" max="28" width="10" style="13" customWidth="1"/>
-    <col min="29" max="29" width="10.140625" style="13" customWidth="1"/>
-    <col min="30" max="35" width="9.140625" style="13" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="13"/>
+    <col min="29" max="29" width="10.1796875" style="13" customWidth="1"/>
+    <col min="30" max="35" width="9.1796875" style="13" customWidth="1"/>
+    <col min="36" max="16384" width="9.1796875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
@@ -35920,7 +36036,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>34</v>
       </c>
@@ -35932,7 +36048,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>36</v>
       </c>
@@ -35946,7 +36062,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
         <v>38</v>
       </c>
@@ -35962,7 +36078,7 @@
       <c r="AC4" s="30"/>
       <c r="AD4" s="30"/>
     </row>
-    <row r="5" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
         <v>39</v>
       </c>
@@ -35974,7 +36090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="31" t="s">
         <v>40</v>
       </c>
@@ -36001,7 +36117,7 @@
       <c r="W6" s="33"/>
       <c r="X6" s="33"/>
     </row>
-    <row r="7" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
         <v>41</v>
       </c>
@@ -36033,7 +36149,7 @@
       <c r="W7" s="33"/>
       <c r="X7" s="33"/>
     </row>
-    <row r="8" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
         <v>42</v>
       </c>
@@ -36063,7 +36179,7 @@
       <c r="AC8" s="39"/>
       <c r="AD8" s="39"/>
     </row>
-    <row r="9" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="36" t="s">
         <v>43</v>
       </c>
@@ -36084,7 +36200,7 @@
       <c r="AC9" s="39"/>
       <c r="AD9" s="39"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>51</v>
       </c>
@@ -36104,7 +36220,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
         <v>44</v>
       </c>
@@ -36126,7 +36242,7 @@
       <c r="W11" s="40"/>
       <c r="X11" s="40"/>
     </row>
-    <row r="12" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="36" t="s">
         <v>86</v>
       </c>
@@ -36148,7 +36264,7 @@
       <c r="W12" s="40"/>
       <c r="X12" s="40"/>
     </row>
-    <row r="13" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
         <v>87</v>
       </c>
@@ -36170,7 +36286,7 @@
       <c r="W13" s="40"/>
       <c r="X13" s="40"/>
     </row>
-    <row r="14" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
         <v>45</v>
       </c>
@@ -36194,7 +36310,7 @@
       <c r="W14" s="40"/>
       <c r="X14" s="40"/>
     </row>
-    <row r="15" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
         <v>55</v>
       </c>
@@ -36215,25 +36331,55 @@
       <c r="W15" s="40"/>
       <c r="X15" s="40"/>
     </row>
-    <row r="16" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="37"/>
+    <row r="16" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>37</v>
+      </c>
       <c r="C16" s="37"/>
+      <c r="D16" s="38">
+        <v>1</v>
+      </c>
+      <c r="M16" s="38">
+        <v>1</v>
+      </c>
       <c r="T16" s="40"/>
       <c r="U16" s="40"/>
       <c r="V16" s="40"/>
       <c r="W16" s="40"/>
       <c r="X16" s="40"/>
     </row>
-    <row r="17" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
+    <row r="17" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>37</v>
+      </c>
       <c r="C17" s="37"/>
+      <c r="D17" s="38">
+        <v>1</v>
+      </c>
+      <c r="M17" s="38">
+        <v>1</v>
+      </c>
       <c r="T17" s="40"/>
       <c r="U17" s="40"/>
       <c r="V17" s="40"/>
       <c r="W17" s="40"/>
       <c r="X17" s="40"/>
+    </row>
+    <row r="18" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="40"/>
+      <c r="X18" s="40"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -36246,7 +36392,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C6 C15:C1048576 C8:C9 C11:C13" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C6 C11:C13 C8:C9 C15:C1048576" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -36268,9 +36414,9 @@
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -36284,7 +36430,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -36295,7 +36441,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
BHU: new costing data for basleine treatment
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3CCFBA-A2FF-4354-8090-1A698E33C8BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92A7F56-FE5F-4A48-B7A4-717BA9303076}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="5510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="5510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2374,8 +2374,8 @@
   </sheetPr>
   <dimension ref="A1:XFD83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView topLeftCell="A71" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35831,7 +35831,7 @@
         <v>110</v>
       </c>
       <c r="B74" s="50">
-        <v>1000</v>
+        <v>123.93</v>
       </c>
     </row>
     <row r="75" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
@@ -35863,7 +35863,7 @@
         <v>114</v>
       </c>
       <c r="B78" s="50">
-        <v>1.2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
@@ -35871,7 +35871,7 @@
         <v>115</v>
       </c>
       <c r="B79" s="50">
-        <v>1000</v>
+        <v>2591.36</v>
       </c>
     </row>
     <row r="80" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
@@ -35903,7 +35903,7 @@
         <v>119</v>
       </c>
       <c r="B83" s="50">
-        <v>1.2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -35937,11 +35937,11 @@
   </sheetPr>
   <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36340,10 +36340,10 @@
       </c>
       <c r="C16" s="37"/>
       <c r="D16" s="38">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="M16" s="38">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="T16" s="40"/>
       <c r="U16" s="40"/>
@@ -36360,10 +36360,10 @@
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="38">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="M17" s="38">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="T17" s="40"/>
       <c r="U17" s="40"/>

</xml_diff>

<commit_message>
BHU: Change Dorm ACF coverage from 20 to 80%. Full analysis run again
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92A7F56-FE5F-4A48-B7A4-717BA9303076}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AF73D6-DD2E-4BB4-AF37-CCFC1138B60E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="5510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2378,15 +2378,15 @@
       <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="4" customWidth="1"/>
-    <col min="3" max="14" width="9.1796875" style="10" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="10"/>
+    <col min="1" max="1" width="51.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
+    <col min="3" max="14" width="9.140625" style="10" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
@@ -2438,7 +2438,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
@@ -2450,7 +2450,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
@@ -2462,7 +2462,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>8</v>
       </c>
@@ -2474,7 +2474,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
@@ -2490,7 +2490,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
@@ -2502,7 +2502,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:16384" s="56" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16384" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
         <v>98</v>
       </c>
@@ -18892,7 +18892,7 @@
       <c r="XFC10" s="55"/>
       <c r="XFD10" s="55"/>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>11</v>
       </c>
@@ -18904,7 +18904,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>12</v>
       </c>
@@ -18916,7 +18916,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>107</v>
       </c>
@@ -18928,7 +18928,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>13</v>
       </c>
@@ -18940,7 +18940,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>14</v>
       </c>
@@ -18952,7 +18952,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>15</v>
       </c>
@@ -18964,7 +18964,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>16</v>
       </c>
@@ -18976,7 +18976,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>17</v>
       </c>
@@ -18988,7 +18988,7 @@
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>18</v>
       </c>
@@ -19000,7 +19000,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>19</v>
       </c>
@@ -19012,7 +19012,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>20</v>
       </c>
@@ -19024,7 +19024,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>21</v>
       </c>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="C22" s="13"/>
     </row>
-    <row r="23" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
         <v>22</v>
       </c>
@@ -19041,7 +19041,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
         <v>23</v>
       </c>
@@ -19049,7 +19049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
         <v>24</v>
       </c>
@@ -19057,7 +19057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>99</v>
       </c>
@@ -19065,7 +19065,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="27" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>100</v>
       </c>
@@ -19073,7 +19073,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
         <v>102</v>
       </c>
@@ -35463,7 +35463,7 @@
       <c r="XFC28" s="57"/>
       <c r="XFD28" s="57"/>
     </row>
-    <row r="29" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>101</v>
       </c>
@@ -35471,7 +35471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A30" s="58" t="s">
         <v>103</v>
       </c>
@@ -35479,7 +35479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
         <v>61</v>
       </c>
@@ -35488,7 +35488,7 @@
         <v>26.28</v>
       </c>
     </row>
-    <row r="32" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16384" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="46" t="s">
         <v>62</v>
       </c>
@@ -35496,7 +35496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="46" t="s">
         <v>63</v>
       </c>
@@ -35504,7 +35504,7 @@
         <v>429544</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="46" t="s">
         <v>64</v>
       </c>
@@ -35512,7 +35512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
         <v>65</v>
       </c>
@@ -35520,7 +35520,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="49" t="s">
         <v>66</v>
       </c>
@@ -35529,7 +35529,7 @@
         <v>26.53</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="49" t="s">
         <v>67</v>
       </c>
@@ -35537,7 +35537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="49" t="s">
         <v>68</v>
       </c>
@@ -35545,7 +35545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49" t="s">
         <v>69</v>
       </c>
@@ -35553,7 +35553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="49" t="s">
         <v>70</v>
       </c>
@@ -35561,7 +35561,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
         <v>71</v>
       </c>
@@ -35570,7 +35570,7 @@
         <v>26.78</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
         <v>72</v>
       </c>
@@ -35578,7 +35578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
         <v>73</v>
       </c>
@@ -35586,7 +35586,7 @@
         <v>429544</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
         <v>74</v>
       </c>
@@ -35594,7 +35594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
         <v>75</v>
       </c>
@@ -35602,7 +35602,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
         <v>104</v>
       </c>
@@ -35610,7 +35610,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="49" t="s">
         <v>76</v>
       </c>
@@ -35618,7 +35618,7 @@
         <v>21.67</v>
       </c>
     </row>
-    <row r="48" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="49" t="s">
         <v>77</v>
       </c>
@@ -35626,7 +35626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="49" t="s">
         <v>78</v>
       </c>
@@ -35634,7 +35634,7 @@
         <v>20480</v>
       </c>
     </row>
-    <row r="50" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="49" t="s">
         <v>79</v>
       </c>
@@ -35642,7 +35642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="49" t="s">
         <v>80</v>
       </c>
@@ -35650,7 +35650,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="52" spans="1:2" s="61" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="59" t="s">
         <v>105</v>
       </c>
@@ -35658,7 +35658,7 @@
         <v>8060</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="46" t="s">
         <v>88</v>
       </c>
@@ -35666,7 +35666,7 @@
         <v>170.89</v>
       </c>
     </row>
-    <row r="54" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="46" t="s">
         <v>89</v>
       </c>
@@ -35674,7 +35674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="46" t="s">
         <v>90</v>
       </c>
@@ -35682,7 +35682,7 @@
         <v>16095</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="46" t="s">
         <v>91</v>
       </c>
@@ -35690,7 +35690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="46" t="s">
         <v>92</v>
       </c>
@@ -35698,7 +35698,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="52" t="s">
         <v>93</v>
       </c>
@@ -35706,7 +35706,7 @@
         <v>170.89</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="52" t="s">
         <v>94</v>
       </c>
@@ -35714,7 +35714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="52" t="s">
         <v>95</v>
       </c>
@@ -35722,7 +35722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="52" t="s">
         <v>96</v>
       </c>
@@ -35730,7 +35730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="52" t="s">
         <v>97</v>
       </c>
@@ -35738,7 +35738,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="43" t="s">
         <v>81</v>
       </c>
@@ -35746,7 +35746,7 @@
         <v>22.36</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="43" t="s">
         <v>82</v>
       </c>
@@ -35754,7 +35754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="43" t="s">
         <v>83</v>
       </c>
@@ -35762,7 +35762,7 @@
         <v>44500</v>
       </c>
     </row>
-    <row r="66" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="43" t="s">
         <v>84</v>
       </c>
@@ -35770,7 +35770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="43" t="s">
         <v>85</v>
       </c>
@@ -35778,7 +35778,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="43" t="s">
         <v>106</v>
       </c>
@@ -35786,7 +35786,7 @@
         <v>24493</v>
       </c>
     </row>
-    <row r="69" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="46" t="s">
         <v>56</v>
       </c>
@@ -35794,7 +35794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="46" t="s">
         <v>57</v>
       </c>
@@ -35802,7 +35802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="46" t="s">
         <v>58</v>
       </c>
@@ -35810,7 +35810,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="72" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="46" t="s">
         <v>59</v>
       </c>
@@ -35818,7 +35818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="46" t="s">
         <v>60</v>
       </c>
@@ -35826,7 +35826,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="74" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="49" t="s">
         <v>110</v>
       </c>
@@ -35834,7 +35834,7 @@
         <v>123.93</v>
       </c>
     </row>
-    <row r="75" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="49" t="s">
         <v>111</v>
       </c>
@@ -35842,7 +35842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="49" t="s">
         <v>112</v>
       </c>
@@ -35850,7 +35850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="49" t="s">
         <v>113</v>
       </c>
@@ -35858,7 +35858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
         <v>114</v>
       </c>
@@ -35866,7 +35866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
         <v>115</v>
       </c>
@@ -35874,7 +35874,7 @@
         <v>2591.36</v>
       </c>
     </row>
-    <row r="80" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="49" t="s">
         <v>116</v>
       </c>
@@ -35882,7 +35882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="49" t="s">
         <v>117</v>
       </c>
@@ -35890,7 +35890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="49" t="s">
         <v>118</v>
       </c>
@@ -35898,7 +35898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="49" t="s">
         <v>119</v>
       </c>
@@ -35938,37 +35938,37 @@
   <dimension ref="A1:AD18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="9" customWidth="1"/>
     <col min="4" max="4" width="11" style="13" customWidth="1"/>
-    <col min="5" max="8" width="7.453125" style="13" customWidth="1"/>
+    <col min="5" max="8" width="7.42578125" style="13" customWidth="1"/>
     <col min="9" max="13" width="7" style="13" customWidth="1"/>
     <col min="14" max="14" width="13" style="13" customWidth="1"/>
-    <col min="15" max="15" width="12.1796875" style="13" customWidth="1"/>
-    <col min="16" max="16" width="11.453125" style="13" customWidth="1"/>
-    <col min="17" max="17" width="11.1796875" style="13" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="13" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" style="13" customWidth="1"/>
     <col min="18" max="18" width="13" style="13" customWidth="1"/>
-    <col min="19" max="19" width="11.26953125" style="13" customWidth="1"/>
-    <col min="20" max="20" width="11.1796875" customWidth="1"/>
-    <col min="21" max="21" width="10.453125" customWidth="1"/>
-    <col min="25" max="25" width="9.1796875" style="13" customWidth="1"/>
-    <col min="26" max="26" width="10.81640625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" style="13" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="13" customWidth="1"/>
+    <col min="26" max="26" width="10.85546875" style="13" customWidth="1"/>
     <col min="27" max="28" width="10" style="13" customWidth="1"/>
-    <col min="29" max="29" width="10.1796875" style="13" customWidth="1"/>
-    <col min="30" max="35" width="9.1796875" style="13" customWidth="1"/>
-    <col min="36" max="16384" width="9.1796875" style="13"/>
+    <col min="29" max="29" width="10.140625" style="13" customWidth="1"/>
+    <col min="30" max="35" width="9.140625" style="13" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
@@ -36036,7 +36036,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>34</v>
       </c>
@@ -36048,7 +36048,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>36</v>
       </c>
@@ -36062,7 +36062,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>38</v>
       </c>
@@ -36078,7 +36078,7 @@
       <c r="AC4" s="30"/>
       <c r="AD4" s="30"/>
     </row>
-    <row r="5" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>39</v>
       </c>
@@ -36090,7 +36090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>40</v>
       </c>
@@ -36117,7 +36117,7 @@
       <c r="W6" s="33"/>
       <c r="X6" s="33"/>
     </row>
-    <row r="7" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>41</v>
       </c>
@@ -36149,7 +36149,7 @@
       <c r="W7" s="33"/>
       <c r="X7" s="33"/>
     </row>
-    <row r="8" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>42</v>
       </c>
@@ -36179,7 +36179,7 @@
       <c r="AC8" s="39"/>
       <c r="AD8" s="39"/>
     </row>
-    <row r="9" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>43</v>
       </c>
@@ -36200,7 +36200,7 @@
       <c r="AC9" s="39"/>
       <c r="AD9" s="39"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>51</v>
       </c>
@@ -36220,7 +36220,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>44</v>
       </c>
@@ -36242,7 +36242,7 @@
       <c r="W11" s="40"/>
       <c r="X11" s="40"/>
     </row>
-    <row r="12" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>86</v>
       </c>
@@ -36264,7 +36264,7 @@
       <c r="W12" s="40"/>
       <c r="X12" s="40"/>
     </row>
-    <row r="13" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>87</v>
       </c>
@@ -36286,7 +36286,7 @@
       <c r="W13" s="40"/>
       <c r="X13" s="40"/>
     </row>
-    <row r="14" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
         <v>45</v>
       </c>
@@ -36301,7 +36301,7 @@
         <v>0</v>
       </c>
       <c r="T14" s="40">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U14" s="40"/>
       <c r="V14" s="40">
@@ -36310,7 +36310,7 @@
       <c r="W14" s="40"/>
       <c r="X14" s="40"/>
     </row>
-    <row r="15" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
         <v>55</v>
       </c>
@@ -36331,7 +36331,7 @@
       <c r="W15" s="40"/>
       <c r="X15" s="40"/>
     </row>
-    <row r="16" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>108</v>
       </c>
@@ -36351,7 +36351,7 @@
       <c r="W16" s="40"/>
       <c r="X16" s="40"/>
     </row>
-    <row r="17" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
         <v>109</v>
       </c>
@@ -36371,7 +36371,7 @@
       <c r="W17" s="40"/>
       <c r="X17" s="40"/>
     </row>
-    <row r="18" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -36414,9 +36414,9 @@
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -36430,7 +36430,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -36441,7 +36441,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
BHU: cosmetic change to fig title and fix wrong coverage in SC_9
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bhutan.xlsx
+++ b/autumn/xls/data_bhutan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AF73D6-DD2E-4BB4-AF37-CCFC1138B60E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9036944B-CB71-40AC-8DEF-4F13C685E3EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2374,8 +2374,8 @@
   </sheetPr>
   <dimension ref="A1:XFD83"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35937,11 +35937,11 @@
   </sheetPr>
   <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T14" sqref="T14"/>
+      <selection pane="bottomRight" activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36305,7 +36305,7 @@
       </c>
       <c r="U14" s="40"/>
       <c r="V14" s="40">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W14" s="40"/>
       <c r="X14" s="40"/>

</xml_diff>